<commit_message>
Salli muita oikeustyyppejä kuin :luku/:kirjoitus
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="1020" windowWidth="51200" windowHeight="28260" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="0" windowWidth="40820" windowHeight="23380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="126">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
   <si>
-    <t>R = lukuoikeus, RW = luku- ja kirjoitusoikeus, R* = rajoitettu lukuoikeus ilman taloustietoja, tyhjä = ei näe osiota</t>
-  </si>
-  <si>
     <t>Kirjoitusoikeus ei tarkoita "täyttä" kaiken muokkausmahdollisuutta, tilaaja/urakoitsija ero vaikuttaa mitä asioita näkymässä voi kirjoittaa.</t>
   </si>
   <si>
@@ -82,9 +79,6 @@
     <t>Yleiset</t>
   </si>
   <si>
-    <t>RW</t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
@@ -100,9 +94,6 @@
     <t>Suunnittelu / Yksikköhintaiset työt</t>
   </si>
   <si>
-    <t>Suunnittelu / Muutos- ja lisätyöt</t>
-  </si>
-  <si>
     <t>Suunnittelu / Suola</t>
   </si>
   <si>
@@ -115,9 +106,6 @@
     <t>Toteumat / Yksikköhintaiset työt</t>
   </si>
   <si>
-    <t>Toteumat / Muutos- ja lisätyöt</t>
-  </si>
-  <si>
     <t>Toteumat / Suola</t>
   </si>
   <si>
@@ -383,6 +371,33 @@
   </si>
   <si>
     <t>testikäyttö</t>
+  </si>
+  <si>
+    <t>Suunnittelu / Muutos- ja-lisätyöt</t>
+  </si>
+  <si>
+    <t>Toteumat / Muutos- ja-lisätyöt</t>
+  </si>
+  <si>
+    <t>R,W</t>
+  </si>
+  <si>
+    <t>Huomiot</t>
+  </si>
+  <si>
+    <t>synteettinen rooli</t>
+  </si>
+  <si>
+    <t>Tiemerkitsija</t>
+  </si>
+  <si>
+    <t>Tiemerkitsijä</t>
+  </si>
+  <si>
+    <t>R = lukuoikeus, R,W = luku- ja kirjoitusoikeus, tyhjä = ei näe osiota, muut erikoisoikeuksia</t>
+  </si>
+  <si>
+    <t>R,TM-valmis</t>
   </si>
 </sst>
 </file>
@@ -495,7 +510,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -631,6 +646,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -641,7 +676,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -701,12 +736,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -739,6 +769,24 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1078,11 +1126,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T55"/>
+  <dimension ref="A1:U55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T28" sqref="T28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1105,1256 +1153,1280 @@
     <col min="17" max="17" width="11.5" customWidth="1"/>
     <col min="18" max="18" width="10.6640625" customWidth="1"/>
     <col min="19" max="19" width="11.1640625" customWidth="1"/>
-    <col min="20" max="20" width="39" customWidth="1"/>
+    <col min="20" max="20" width="11.1640625" style="27" customWidth="1"/>
+    <col min="21" max="21" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15.75" customHeight="1">
+    <row r="1" spans="1:21" ht="15.75" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-    </row>
-    <row r="2" spans="1:20" ht="15.75" customHeight="1">
+      <c r="C1" s="43" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+    </row>
+    <row r="2" spans="1:21" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-    </row>
-    <row r="3" spans="1:20" ht="15.75" customHeight="1">
+      <c r="C2" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+    </row>
+    <row r="3" spans="1:21" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="4" t="s">
+    </row>
+    <row r="4" spans="1:21" ht="15.75" customHeight="1">
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="1:21" ht="15.75" customHeight="1">
+      <c r="C5" s="42" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" ht="15.75" customHeight="1">
-      <c r="C4" s="5"/>
-    </row>
-    <row r="5" spans="1:20" ht="15.75" customHeight="1">
-      <c r="C5" s="29" t="s">
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="29" t="s">
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
+      <c r="N5" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="29" t="s">
+      <c r="O5" s="41"/>
+      <c r="P5" s="41"/>
+      <c r="Q5" s="41"/>
+      <c r="R5" s="41"/>
+      <c r="S5" s="41"/>
+      <c r="U5" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="15.75" customHeight="1">
+      <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="O5" s="28"/>
-      <c r="P5" s="28"/>
-      <c r="Q5" s="28"/>
-      <c r="R5" s="28"/>
-      <c r="S5" s="28"/>
-      <c r="T5" s="5" t="s">
+      <c r="B6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="N6" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="O6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="P6" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q6" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="R6" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="S6" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="T6" s="9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="15.75" customHeight="1">
+      <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" ht="15.75" customHeight="1">
-      <c r="A6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="K6" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="L6" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="M6" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="N6" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="O6" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="P6" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q6" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="R6" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="S6" s="9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" ht="15.75" customHeight="1">
-      <c r="A7" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="N7" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="O7" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="P7" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q7" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="R7" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="S7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="T7" s="47"/>
+      <c r="U7" s="13"/>
+    </row>
+    <row r="8" spans="1:21" ht="15.75" customHeight="1">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="L7" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="M7" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="N7" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="O7" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="P7" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q7" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="R7" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="S7" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="T7" s="13"/>
-    </row>
-    <row r="8" spans="1:20" ht="15.75" customHeight="1">
-      <c r="A8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H8" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="N8" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="O8" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="P8" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q8" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="R8" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="S8" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="T8" s="47"/>
+      <c r="U8" s="13"/>
+    </row>
+    <row r="9" spans="1:21" ht="15.75" customHeight="1">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="I8" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="J8" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K8" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="L8" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="M8" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="N8" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="O8" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="P8" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q8" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="R8" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="S8" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="T8" s="13"/>
-    </row>
-    <row r="9" spans="1:20" ht="15.75" customHeight="1">
-      <c r="A9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="K9" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L9" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="M9" s="16" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="M9" s="12" t="s">
+        <v>19</v>
       </c>
       <c r="N9" s="14" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="O9" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="P9" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q9" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="R9" s="17"/>
       <c r="S9" s="18"/>
-      <c r="T9" s="13"/>
-    </row>
-    <row r="10" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T9" s="47"/>
+      <c r="U9" s="13"/>
+    </row>
+    <row r="10" spans="1:21" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>117</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="K10" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L10" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="M10" s="16" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="M10" s="12" t="s">
+        <v>19</v>
       </c>
       <c r="N10" s="14" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="O10" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="P10" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q10" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="R10" s="17"/>
       <c r="S10" s="18"/>
-      <c r="T10" s="13"/>
-    </row>
-    <row r="11" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T10" s="47"/>
+      <c r="U10" s="13"/>
+    </row>
+    <row r="11" spans="1:21" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="F11" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" s="16" t="s">
-        <v>23</v>
-      </c>
       <c r="I11" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J11" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="K11" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L11" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="M11" s="16" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="M11" s="12" t="s">
+        <v>19</v>
       </c>
       <c r="N11" s="14" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="O11" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="P11" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q11" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="R11" s="17"/>
       <c r="S11" s="18"/>
-      <c r="T11" s="13"/>
-    </row>
-    <row r="12" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T11" s="47"/>
+      <c r="U11" s="13"/>
+    </row>
+    <row r="12" spans="1:21" ht="15.75" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="F12" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12" s="16" t="s">
-        <v>23</v>
-      </c>
       <c r="I12" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="K12" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L12" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="M12" s="16" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="M12" s="12" t="s">
+        <v>19</v>
       </c>
       <c r="N12" s="14" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="O12" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="P12" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q12" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="R12" s="17"/>
       <c r="S12" s="18"/>
-      <c r="T12" s="13"/>
-    </row>
-    <row r="13" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T12" s="47"/>
+      <c r="U12" s="13"/>
+    </row>
+    <row r="13" spans="1:21" ht="15.75" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="F13" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" s="16" t="s">
-        <v>23</v>
-      </c>
       <c r="I13" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J13" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="K13" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L13" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="M13" s="16" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="M13" s="12" t="s">
+        <v>19</v>
       </c>
       <c r="N13" s="14" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="O13" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="P13" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q13" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="R13" s="17"/>
       <c r="S13" s="18"/>
-      <c r="T13" s="13"/>
-    </row>
-    <row r="14" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T13" s="47"/>
+      <c r="U13" s="13"/>
+    </row>
+    <row r="14" spans="1:21" ht="15.75" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="F14" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="H14" s="16" t="s">
-        <v>23</v>
-      </c>
       <c r="I14" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J14" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="K14" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L14" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="M14" s="16" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>19</v>
       </c>
       <c r="N14" s="14" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="O14" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="P14" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q14" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="R14" s="17"/>
       <c r="S14" s="18"/>
-      <c r="T14" s="13"/>
-    </row>
-    <row r="15" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T14" s="47"/>
+      <c r="U14" s="13"/>
+    </row>
+    <row r="15" spans="1:21" ht="15.75" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>31</v>
+        <v>118</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="F15" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="H15" s="16" t="s">
-        <v>23</v>
-      </c>
       <c r="I15" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J15" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="K15" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L15" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="M15" s="16" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="M15" s="12" t="s">
+        <v>19</v>
       </c>
       <c r="N15" s="14" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="O15" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="P15" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q15" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="R15" s="17"/>
       <c r="S15" s="18"/>
-      <c r="T15" s="13"/>
-    </row>
-    <row r="16" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T15" s="47"/>
+      <c r="U15" s="13"/>
+    </row>
+    <row r="16" spans="1:21" ht="15.75" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="F16" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="H16" s="16" t="s">
-        <v>23</v>
-      </c>
       <c r="I16" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J16" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="K16" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L16" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="M16" s="16" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="M16" s="12" t="s">
+        <v>19</v>
       </c>
       <c r="N16" s="14" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="O16" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="P16" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q16" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="R16" s="17"/>
       <c r="S16" s="18"/>
-      <c r="T16" s="13"/>
-    </row>
-    <row r="17" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T16" s="47"/>
+      <c r="U16" s="13"/>
+    </row>
+    <row r="17" spans="1:21" ht="15.75" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C17" s="14"/>
       <c r="D17" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="F17" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="G17" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="H17" s="16" t="s">
-        <v>23</v>
-      </c>
       <c r="I17" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J17" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="K17" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L17" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="M17" s="16" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="M17" s="12" t="s">
+        <v>19</v>
       </c>
       <c r="N17" s="14" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="O17" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="P17" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q17" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="R17" s="17"/>
       <c r="S17" s="18"/>
-      <c r="T17" s="13"/>
-    </row>
-    <row r="18" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T17" s="47"/>
+      <c r="U17" s="13"/>
+    </row>
+    <row r="18" spans="1:21" ht="15.75" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C18" s="14"/>
       <c r="D18" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="F18" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="H18" s="16" t="s">
-        <v>23</v>
-      </c>
       <c r="I18" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J18" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="K18" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L18" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="M18" s="16" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="M18" s="12" t="s">
+        <v>19</v>
       </c>
       <c r="N18" s="14" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="O18" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="P18" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q18" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="R18" s="17"/>
       <c r="S18" s="18"/>
-      <c r="T18" s="13"/>
-    </row>
-    <row r="19" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T18" s="47"/>
+      <c r="U18" s="13"/>
+    </row>
+    <row r="19" spans="1:21" ht="15.75" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C19" s="14"/>
       <c r="D19" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H19" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I19" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J19" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="K19" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L19" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M19" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N19" s="14" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="O19" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="P19" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q19" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="R19" s="17"/>
       <c r="S19" s="18"/>
-      <c r="T19" s="13"/>
-    </row>
-    <row r="20" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T19" s="47"/>
+      <c r="U19" s="13"/>
+    </row>
+    <row r="20" spans="1:21" ht="15.75" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C20" s="14"/>
       <c r="D20" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H20" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I20" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J20" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="K20" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L20" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M20" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N20" s="14" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="O20" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="P20" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q20" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="R20" s="17"/>
       <c r="S20" s="18"/>
-      <c r="T20" s="13"/>
-    </row>
-    <row r="21" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T20" s="47"/>
+      <c r="U20" s="13"/>
+    </row>
+    <row r="21" spans="1:21" ht="15.75" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C21" s="14"/>
       <c r="D21" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I21" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J21" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="K21" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L21" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M21" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N21" s="14" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="O21" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="P21" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q21" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="R21" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="S21" s="18"/>
-      <c r="T21" s="13"/>
-    </row>
-    <row r="22" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T21" s="47"/>
+      <c r="U21" s="13"/>
+    </row>
+    <row r="22" spans="1:21" ht="15.75" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C22" s="14"/>
       <c r="D22" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I22" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J22" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="K22" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L22" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M22" s="16" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="N22" s="14" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="O22" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="P22" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q22" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="R22" s="17"/>
       <c r="S22" s="18"/>
-      <c r="T22" s="13"/>
-    </row>
-    <row r="23" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T22" s="47"/>
+      <c r="U22" s="13"/>
+    </row>
+    <row r="23" spans="1:21" ht="15.75" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C23" s="14"/>
       <c r="D23" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H23" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J23" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="K23" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L23" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M23" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N23" s="14" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="O23" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="P23" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q23" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="R23" s="17"/>
       <c r="S23" s="18"/>
-      <c r="T23" s="13"/>
-    </row>
-    <row r="24" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T23" s="47"/>
+      <c r="U23" s="13"/>
+    </row>
+    <row r="24" spans="1:21" ht="15.75" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C24" s="14"/>
       <c r="D24" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H24" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J24" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="K24" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L24" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M24" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N24" s="14" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="O24" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="P24" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q24" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="R24" s="17"/>
       <c r="S24" s="18"/>
-      <c r="T24" s="13"/>
-    </row>
-    <row r="25" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T24" s="47"/>
+      <c r="U24" s="13"/>
+    </row>
+    <row r="25" spans="1:21" ht="15.75" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C25" s="14"/>
       <c r="D25" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G25" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H25" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="J25" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="K25" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L25" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M25" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N25" s="14" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="O25" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="P25" s="17"/>
       <c r="Q25" s="17"/>
       <c r="R25" s="17"/>
       <c r="S25" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="T25" s="13"/>
-    </row>
-    <row r="26" spans="1:20" ht="15.75" customHeight="1">
+        <v>19</v>
+      </c>
+      <c r="T25" s="47"/>
+      <c r="U25" s="13"/>
+    </row>
+    <row r="26" spans="1:21" ht="15.75" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C26" s="14"/>
       <c r="D26" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G26" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H26" s="18"/>
       <c r="I26" s="14" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="J26" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="K26" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L26" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M26" s="18"/>
       <c r="N26" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="O26" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="P26" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q26" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="R26" s="17"/>
       <c r="S26" s="18"/>
-      <c r="T26" s="13"/>
-    </row>
-    <row r="27" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T26" s="47"/>
+      <c r="U26" s="13"/>
+    </row>
+    <row r="27" spans="1:21" ht="15.75" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C27" s="14"/>
       <c r="D27" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="F27" s="17"/>
       <c r="G27" s="17"/>
       <c r="H27" s="18"/>
       <c r="I27" s="14" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="J27" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="K27" s="17"/>
       <c r="L27" s="17"/>
@@ -2365,315 +2437,323 @@
       <c r="Q27" s="17"/>
       <c r="R27" s="17"/>
       <c r="S27" s="18"/>
-      <c r="T27" s="20" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T27" s="47"/>
+      <c r="U27" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" ht="15.75" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C28" s="14"/>
       <c r="D28" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G28" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H28" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I28" s="14" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="J28" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="K28" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L28" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M28" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N28" s="14" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="O28" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="P28" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q28" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="R28" s="17"/>
       <c r="S28" s="18"/>
-      <c r="T28" s="13"/>
-    </row>
-    <row r="29" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T28" s="47" t="s">
+        <v>125</v>
+      </c>
+      <c r="U28" s="13"/>
+    </row>
+    <row r="29" spans="1:21" ht="15.75" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C29" s="14"/>
       <c r="D29" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G29" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H29" s="16" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I29" s="14" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="J29" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="K29" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L29" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M29" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N29" s="14" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="O29" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="P29" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q29" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="R29" s="17"/>
       <c r="S29" s="18"/>
-      <c r="T29" s="13"/>
-    </row>
-    <row r="30" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T29" s="47"/>
+      <c r="U29" s="13"/>
+    </row>
+    <row r="30" spans="1:21" ht="15.75" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C30" s="14"/>
       <c r="D30" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G30" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H30" s="16" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I30" s="14" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="J30" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="K30" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L30" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M30" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N30" s="14" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="O30" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="P30" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q30" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="R30" s="17"/>
       <c r="S30" s="18"/>
-      <c r="T30" s="13"/>
-    </row>
-    <row r="31" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T30" s="47"/>
+      <c r="U30" s="13"/>
+    </row>
+    <row r="31" spans="1:21" ht="15.75" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C31" s="14"/>
       <c r="D31" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G31" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H31" s="16" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I31" s="14" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="J31" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="K31" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L31" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M31" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N31" s="14" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="O31" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="P31" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q31" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="R31" s="17"/>
       <c r="S31" s="18"/>
-      <c r="T31" s="13"/>
-    </row>
-    <row r="32" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T31" s="47"/>
+      <c r="U31" s="13"/>
+    </row>
+    <row r="32" spans="1:21" ht="15.75" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C32" s="14"/>
       <c r="D32" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G32" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H32" s="16" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I32" s="14" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="J32" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="K32" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L32" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M32" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N32" s="14" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="O32" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="P32" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q32" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="R32" s="17"/>
       <c r="S32" s="18"/>
-      <c r="T32" s="13"/>
-    </row>
-    <row r="33" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T32" s="47"/>
+      <c r="U32" s="13"/>
+    </row>
+    <row r="33" spans="1:21" ht="15.75" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C33" s="14"/>
       <c r="D33" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H33" s="16" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I33" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J33" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K33" s="17"/>
       <c r="L33" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M33" s="16" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="N33" s="19"/>
       <c r="O33" s="17"/>
@@ -2681,45 +2761,46 @@
       <c r="Q33" s="17"/>
       <c r="R33" s="17"/>
       <c r="S33" s="18"/>
-      <c r="T33" s="13"/>
-    </row>
-    <row r="34" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T33" s="47"/>
+      <c r="U33" s="13"/>
+    </row>
+    <row r="34" spans="1:21" ht="15.75" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C34" s="14"/>
       <c r="D34" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G34" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H34" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I34" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J34" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K34" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L34" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M34" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N34" s="19"/>
       <c r="O34" s="17"/>
@@ -2727,45 +2808,46 @@
       <c r="Q34" s="17"/>
       <c r="R34" s="17"/>
       <c r="S34" s="18"/>
-      <c r="T34" s="13"/>
-    </row>
-    <row r="35" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T34" s="47"/>
+      <c r="U34" s="13"/>
+    </row>
+    <row r="35" spans="1:21" ht="15.75" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C35" s="14"/>
       <c r="D35" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G35" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H35" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I35" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J35" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K35" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L35" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M35" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N35" s="19"/>
       <c r="O35" s="17"/>
@@ -2773,45 +2855,46 @@
       <c r="Q35" s="17"/>
       <c r="R35" s="17"/>
       <c r="S35" s="18"/>
-      <c r="T35" s="13"/>
-    </row>
-    <row r="36" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T35" s="47"/>
+      <c r="U35" s="13"/>
+    </row>
+    <row r="36" spans="1:21" ht="15.75" customHeight="1">
       <c r="A36" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="C36" s="14"/>
       <c r="D36" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G36" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H36" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I36" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J36" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K36" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L36" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M36" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N36" s="19"/>
       <c r="O36" s="17"/>
@@ -2819,45 +2902,46 @@
       <c r="Q36" s="17"/>
       <c r="R36" s="17"/>
       <c r="S36" s="18"/>
-      <c r="T36" s="13"/>
-    </row>
-    <row r="37" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T36" s="47"/>
+      <c r="U36" s="13"/>
+    </row>
+    <row r="37" spans="1:21" ht="15.75" customHeight="1">
       <c r="A37" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C37" s="14"/>
       <c r="D37" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G37" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H37" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I37" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J37" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K37" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L37" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M37" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N37" s="19"/>
       <c r="O37" s="17"/>
@@ -2865,43 +2949,44 @@
       <c r="Q37" s="17"/>
       <c r="R37" s="17"/>
       <c r="S37" s="18"/>
-      <c r="T37" s="13"/>
-    </row>
-    <row r="38" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T37" s="47"/>
+      <c r="U37" s="13"/>
+    </row>
+    <row r="38" spans="1:21" ht="15.75" customHeight="1">
       <c r="A38" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C38" s="14"/>
       <c r="D38" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F38" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G38" s="17"/>
       <c r="H38" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I38" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J38" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K38" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L38" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M38" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N38" s="19"/>
       <c r="O38" s="17"/>
@@ -2909,38 +2994,39 @@
       <c r="Q38" s="17"/>
       <c r="R38" s="17"/>
       <c r="S38" s="18"/>
-      <c r="T38" s="13"/>
-    </row>
-    <row r="39" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T38" s="47"/>
+      <c r="U38" s="13"/>
+    </row>
+    <row r="39" spans="1:21" ht="15.75" customHeight="1">
       <c r="A39" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C39" s="14"/>
       <c r="D39" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E39" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G39" s="17"/>
       <c r="H39" s="16" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I39" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J39" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K39" s="17"/>
       <c r="L39" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M39" s="18"/>
       <c r="N39" s="19"/>
@@ -2949,45 +3035,46 @@
       <c r="Q39" s="17"/>
       <c r="R39" s="17"/>
       <c r="S39" s="18"/>
-      <c r="T39" s="13"/>
-    </row>
-    <row r="40" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T39" s="47"/>
+      <c r="U39" s="13"/>
+    </row>
+    <row r="40" spans="1:21" ht="15.75" customHeight="1">
       <c r="A40" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C40" s="14"/>
       <c r="D40" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E40" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F40" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G40" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H40" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I40" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J40" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K40" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L40" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M40" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N40" s="19"/>
       <c r="O40" s="17"/>
@@ -2995,43 +3082,44 @@
       <c r="Q40" s="17"/>
       <c r="R40" s="17"/>
       <c r="S40" s="18"/>
-      <c r="T40" s="13"/>
-    </row>
-    <row r="41" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T40" s="47"/>
+      <c r="U40" s="13"/>
+    </row>
+    <row r="41" spans="1:21" ht="15.75" customHeight="1">
       <c r="A41" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C41" s="14"/>
       <c r="D41" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F41" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G41" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H41" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I41" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J41" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K41" s="17"/>
       <c r="L41" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M41" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N41" s="19"/>
       <c r="O41" s="17"/>
@@ -3039,41 +3127,42 @@
       <c r="Q41" s="17"/>
       <c r="R41" s="17"/>
       <c r="S41" s="18"/>
-      <c r="T41" s="13"/>
-    </row>
-    <row r="42" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T41" s="47"/>
+      <c r="U41" s="13"/>
+    </row>
+    <row r="42" spans="1:21" ht="15.75" customHeight="1">
       <c r="A42" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C42" s="14"/>
       <c r="D42" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F42" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G42" s="17"/>
       <c r="H42" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I42" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J42" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K42" s="17"/>
       <c r="L42" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M42" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="N42" s="19"/>
       <c r="O42" s="17"/>
@@ -3081,38 +3170,39 @@
       <c r="Q42" s="17"/>
       <c r="R42" s="17"/>
       <c r="S42" s="18"/>
-      <c r="T42" s="13"/>
-    </row>
-    <row r="43" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T42" s="47"/>
+      <c r="U42" s="13"/>
+    </row>
+    <row r="43" spans="1:21" ht="15.75" customHeight="1">
       <c r="A43" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C43" s="14"/>
       <c r="D43" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G43" s="17"/>
       <c r="H43" s="16" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I43" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J43" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K43" s="17"/>
       <c r="L43" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M43" s="18"/>
       <c r="N43" s="19"/>
@@ -3121,38 +3211,39 @@
       <c r="Q43" s="17"/>
       <c r="R43" s="17"/>
       <c r="S43" s="18"/>
-      <c r="T43" s="13"/>
-    </row>
-    <row r="44" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T43" s="47"/>
+      <c r="U43" s="13"/>
+    </row>
+    <row r="44" spans="1:21" ht="15.75" customHeight="1">
       <c r="A44" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C44" s="14"/>
       <c r="D44" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F44" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G44" s="17"/>
       <c r="H44" s="16" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I44" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J44" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K44" s="17"/>
       <c r="L44" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M44" s="18"/>
       <c r="N44" s="19"/>
@@ -3161,38 +3252,39 @@
       <c r="Q44" s="17"/>
       <c r="R44" s="17"/>
       <c r="S44" s="18"/>
-      <c r="T44" s="13"/>
-    </row>
-    <row r="45" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T44" s="47"/>
+      <c r="U44" s="13"/>
+    </row>
+    <row r="45" spans="1:21" ht="15.75" customHeight="1">
       <c r="A45" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C45" s="14"/>
       <c r="D45" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E45" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F45" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G45" s="17"/>
       <c r="H45" s="16" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I45" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J45" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K45" s="17"/>
       <c r="L45" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M45" s="18"/>
       <c r="N45" s="19"/>
@@ -3201,45 +3293,46 @@
       <c r="Q45" s="17"/>
       <c r="R45" s="17"/>
       <c r="S45" s="18"/>
-      <c r="T45" s="13"/>
-    </row>
-    <row r="46" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T45" s="47"/>
+      <c r="U45" s="13"/>
+    </row>
+    <row r="46" spans="1:21" ht="15.75" customHeight="1">
       <c r="A46" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C46" s="14"/>
       <c r="D46" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E46" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F46" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G46" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H46" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I46" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J46" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K46" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L46" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M46" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N46" s="19"/>
       <c r="O46" s="17"/>
@@ -3247,255 +3340,260 @@
       <c r="Q46" s="17"/>
       <c r="R46" s="17"/>
       <c r="S46" s="18"/>
-      <c r="T46" s="13"/>
-    </row>
-    <row r="47" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T46" s="47"/>
+      <c r="U46" s="13"/>
+    </row>
+    <row r="47" spans="1:21" ht="15.75" customHeight="1">
       <c r="A47" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C47" s="14"/>
       <c r="D47" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F47" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G47" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H47" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I47" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J47" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K47" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L47" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M47" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N47" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="O47" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="P47" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q47" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="R47" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="S47" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="T47" s="27" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="48" spans="1:20" ht="15.75" customHeight="1">
+        <v>19</v>
+      </c>
+      <c r="T47" s="47"/>
+      <c r="U47" s="40" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" ht="15.75" customHeight="1">
       <c r="A48" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C48" s="14"/>
       <c r="D48" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E48" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F48" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G48" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H48" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I48" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J48" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K48" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L48" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M48" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N48" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="O48" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="P48" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q48" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="R48" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="S48" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="T48" s="28"/>
-    </row>
-    <row r="49" spans="1:20" ht="15.75" customHeight="1">
+        <v>19</v>
+      </c>
+      <c r="T48" s="47"/>
+      <c r="U48" s="41"/>
+    </row>
+    <row r="49" spans="1:21" ht="15.75" customHeight="1">
       <c r="A49" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C49" s="14"/>
       <c r="D49" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="E49" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G49" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H49" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I49" s="14" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="J49" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="K49" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L49" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M49" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N49" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="O49" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="P49" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q49" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="R49" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="S49" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="T49" s="13"/>
-    </row>
-    <row r="50" spans="1:20" ht="15.75" customHeight="1">
+        <v>19</v>
+      </c>
+      <c r="T49" s="47"/>
+      <c r="U49" s="13"/>
+    </row>
+    <row r="50" spans="1:21" ht="15.75" customHeight="1">
       <c r="A50" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C50" s="14"/>
       <c r="D50" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="E50" s="17"/>
       <c r="F50" s="17"/>
       <c r="G50" s="17"/>
       <c r="H50" s="18"/>
       <c r="I50" s="14" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="J50" s="17"/>
       <c r="K50" s="17"/>
       <c r="L50" s="17"/>
       <c r="M50" s="18"/>
       <c r="N50" s="14" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="O50" s="17"/>
       <c r="P50" s="17"/>
       <c r="Q50" s="17"/>
       <c r="R50" s="17"/>
       <c r="S50" s="18"/>
-      <c r="T50" s="20" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="51" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T50" s="47"/>
+      <c r="U50" s="20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" ht="15.75" customHeight="1">
       <c r="A51" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C51" s="14"/>
       <c r="D51" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F51" s="15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G51" s="15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H51" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I51" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J51" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K51" s="15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="L51" s="15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="M51" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="N51" s="19"/>
       <c r="O51" s="17"/>
@@ -3503,29 +3601,30 @@
       <c r="Q51" s="17"/>
       <c r="R51" s="17"/>
       <c r="S51" s="18"/>
-    </row>
-    <row r="52" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T51" s="47"/>
+    </row>
+    <row r="52" spans="1:21" ht="15.75" customHeight="1">
       <c r="A52" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="C52" s="14"/>
       <c r="D52" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="E52" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F52" s="17"/>
       <c r="G52" s="17"/>
       <c r="H52" s="18"/>
       <c r="I52" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J52" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K52" s="17"/>
       <c r="L52" s="17"/>
@@ -3536,29 +3635,30 @@
       <c r="Q52" s="17"/>
       <c r="R52" s="17"/>
       <c r="S52" s="18"/>
-    </row>
-    <row r="53" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T52" s="47"/>
+    </row>
+    <row r="53" spans="1:21" ht="15.75" customHeight="1">
       <c r="A53" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C53" s="14"/>
       <c r="D53" s="15" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="E53" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F53" s="17"/>
       <c r="G53" s="17"/>
       <c r="H53" s="18"/>
       <c r="I53" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J53" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K53" s="17"/>
       <c r="L53" s="17"/>
@@ -3569,17 +3669,18 @@
       <c r="Q53" s="17"/>
       <c r="R53" s="17"/>
       <c r="S53" s="18"/>
-    </row>
-    <row r="54" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T53" s="47"/>
+    </row>
+    <row r="54" spans="1:21" ht="15.75" customHeight="1">
       <c r="A54" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C54" s="21"/>
       <c r="D54" s="22" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="E54" s="23"/>
       <c r="F54" s="23"/>
@@ -3596,21 +3697,22 @@
       <c r="Q54" s="23"/>
       <c r="R54" s="23"/>
       <c r="S54" s="24"/>
-    </row>
-    <row r="55" spans="1:20" ht="15.75" customHeight="1">
+      <c r="T54" s="47"/>
+    </row>
+    <row r="55" spans="1:21" ht="15.75" customHeight="1">
       <c r="A55" s="26" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B55" s="26" t="s">
-        <v>120</v>
-      </c>
-      <c r="D55" s="42" t="s">
-        <v>20</v>
+        <v>116</v>
+      </c>
+      <c r="D55" s="39" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="T47:T48"/>
+    <mergeCell ref="U47:U48"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="I5:M5"/>
     <mergeCell ref="N5:S5"/>
@@ -3629,10 +3731,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -3640,277 +3742,298 @@
     <col min="1" max="1" width="29.6640625" customWidth="1"/>
     <col min="2" max="2" width="28.1640625" customWidth="1"/>
     <col min="3" max="3" width="42.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="14" thickBot="1">
+      <c r="A2" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="C2" s="31" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="14" thickBot="1">
+      <c r="A3" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="B3" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="C3" s="31" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="14" thickBot="1">
+      <c r="A4" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="14" thickBot="1">
+      <c r="A5" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="14" thickBot="1">
+      <c r="A6" s="29" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="14" thickBot="1">
-      <c r="A2" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" s="33" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" s="34" t="s">
+      <c r="B6" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="14" thickBot="1">
+      <c r="A7" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="14" thickBot="1">
+      <c r="A8" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="31" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="14" thickBot="1">
-      <c r="A3" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="B3" s="35" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3" s="34" t="s">
+      <c r="D8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="14" thickBot="1">
+      <c r="A9" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="14" thickBot="1">
+      <c r="A10" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="14" thickBot="1">
+      <c r="A11" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="14" thickBot="1">
+      <c r="A12" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="14" thickBot="1">
+      <c r="A13" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="14" thickBot="1">
+      <c r="A14" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="14" thickBot="1">
+      <c r="A15" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="31" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="14" thickBot="1">
-      <c r="A4" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="B4" s="36" t="s">
+      <c r="D15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="14" thickBot="1">
+      <c r="A16" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="B16" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="14" thickBot="1">
+      <c r="A17" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="14" thickBot="1">
+      <c r="A18" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="14" thickBot="1">
+      <c r="A19" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C19" s="31" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="14" thickBot="1">
-      <c r="A5" s="32" t="s">
-        <v>104</v>
-      </c>
-      <c r="B5" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="C5" s="37" t="s">
+      <c r="D19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="14" thickBot="1">
+      <c r="A20" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="14" thickBot="1">
-      <c r="A6" s="32" t="s">
-        <v>105</v>
-      </c>
-      <c r="B6" s="35" t="s">
-        <v>87</v>
-      </c>
-      <c r="C6" s="37" t="s">
+      <c r="D20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="13">
+      <c r="A21" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="B21" s="45" t="s">
+        <v>123</v>
+      </c>
+      <c r="C21" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="D6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="14" thickBot="1">
-      <c r="A7" s="38" t="s">
-        <v>106</v>
-      </c>
-      <c r="B7" s="35" t="s">
-        <v>88</v>
-      </c>
-      <c r="C7" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="14" thickBot="1">
-      <c r="A8" s="32" t="s">
-        <v>107</v>
-      </c>
-      <c r="B8" s="33" t="s">
-        <v>90</v>
-      </c>
-      <c r="C8" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="14" thickBot="1">
-      <c r="A9" s="40" t="s">
-        <v>117</v>
-      </c>
-      <c r="B9" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="C9" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="14" thickBot="1">
-      <c r="A10" s="40" t="s">
-        <v>116</v>
-      </c>
-      <c r="B10" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="C10" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="14" thickBot="1">
-      <c r="A11" s="40" t="s">
-        <v>115</v>
-      </c>
-      <c r="B11" s="35" t="s">
-        <v>93</v>
-      </c>
-      <c r="C11" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="14" thickBot="1">
-      <c r="A12" s="40" t="s">
-        <v>108</v>
-      </c>
-      <c r="B12" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="C12" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="14" thickBot="1">
-      <c r="A13" s="40" t="s">
-        <v>114</v>
-      </c>
-      <c r="B13" s="35" t="s">
-        <v>95</v>
-      </c>
-      <c r="C13" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="14" thickBot="1">
-      <c r="A14" s="38" t="s">
-        <v>109</v>
-      </c>
-      <c r="B14" s="35" t="s">
-        <v>96</v>
-      </c>
-      <c r="C14" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="14" thickBot="1">
-      <c r="A15" s="41" t="s">
-        <v>110</v>
-      </c>
-      <c r="B15" s="35" t="s">
-        <v>97</v>
-      </c>
-      <c r="C15" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="14" thickBot="1">
-      <c r="A16" s="32" t="s">
-        <v>111</v>
-      </c>
-      <c r="B16" s="35" t="s">
+      <c r="D21" t="s">
         <v>98</v>
       </c>
-      <c r="C16" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="14" thickBot="1">
-      <c r="A17" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="B17" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="14" thickBot="1">
-      <c r="A18" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="C18" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="14" thickBot="1">
-      <c r="A19" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="35" t="s">
-        <v>89</v>
-      </c>
-      <c r="C19" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="14" thickBot="1">
-      <c r="A20" s="32" t="s">
-        <v>113</v>
-      </c>
-      <c r="B20" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="C20" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" t="s">
-        <v>102</v>
+      <c r="E21" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tee oikeustarkistukset ja siisti ulkoasua
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="128">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -401,6 +401,9 @@
   </si>
   <si>
     <t>Liitteet</t>
+  </si>
+  <si>
+    <t>R,W,poista</t>
   </si>
 </sst>
 </file>
@@ -1168,7 +1171,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K33" sqref="K33"/>
+      <selection pane="bottomLeft" activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1538,7 +1541,7 @@
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="15" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>117</v>
@@ -2691,7 +2694,7 @@
         <v>117</v>
       </c>
       <c r="K30" s="15" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="L30" s="15" t="s">
         <v>18</v>
@@ -2865,7 +2868,7 @@
         <v>117</v>
       </c>
       <c r="K33" s="17" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="L33" s="17" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Näytä mobiililaadunseurannan linkki vain jos oikeus työkaluun
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26230"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markolau/projektit/harja/resources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20340" yWindow="60" windowWidth="18040" windowHeight="20500" tabRatio="500"/>
+    <workbookView xWindow="43500" yWindow="-18840" windowWidth="35320" windowHeight="22340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="134">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -413,6 +418,15 @@
   </si>
   <si>
     <t xml:space="preserve"> Yrityksen urakan laadunvalvoja</t>
+  </si>
+  <si>
+    <t>Laadunseuranta</t>
+  </si>
+  <si>
+    <t>Kirjaus</t>
+  </si>
+  <si>
+    <t>W</t>
   </si>
 </sst>
 </file>
@@ -550,7 +564,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -593,17 +607,20 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -622,6 +639,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -947,16 +969,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X56"/>
+  <dimension ref="A1:X57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="Q7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="S33" sqref="S33"/>
+      <selection pane="bottomRight" activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.5" bestFit="1" customWidth="1"/>
@@ -983,45 +1005,45 @@
     <col min="24" max="24" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" customHeight="1">
+    <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-    </row>
-    <row r="2" spans="1:24" ht="15.75" customHeight="1">
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+    </row>
+    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-    </row>
-    <row r="3" spans="1:24" ht="15.75" customHeight="1">
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+    </row>
+    <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -1036,39 +1058,39 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="15.75" customHeight="1">
+    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:24" ht="15.75" customHeight="1">
-      <c r="C5" s="28" t="s">
+    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C5" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="J5" s="28" t="s">
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="J5" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="27"/>
-      <c r="L5" s="27"/>
-      <c r="M5" s="27"/>
-      <c r="N5" s="27"/>
-      <c r="P5" s="28" t="s">
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="30"/>
+      <c r="P5" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="Q5" s="27"/>
-      <c r="R5" s="27"/>
-      <c r="S5" s="27"/>
-      <c r="T5" s="27"/>
-      <c r="U5" s="27"/>
-      <c r="V5" s="27"/>
+      <c r="Q5" s="30"/>
+      <c r="R5" s="30"/>
+      <c r="S5" s="30"/>
+      <c r="T5" s="30"/>
+      <c r="U5" s="30"/>
+      <c r="V5" s="30"/>
       <c r="X5" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="15.75" customHeight="1">
+    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -1137,7 +1159,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="15.75" customHeight="1">
+    <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="16" t="s">
         <v>15</v>
       </c>
@@ -1205,7 +1227,7 @@
       <c r="W7" s="17"/>
       <c r="X7" s="10"/>
     </row>
-    <row r="8" spans="1:24" ht="15.75" customHeight="1">
+    <row r="8" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="16" t="s">
         <v>15</v>
       </c>
@@ -1232,7 +1254,7 @@
         <v>116</v>
       </c>
       <c r="L8" s="21"/>
-      <c r="M8" s="30" t="s">
+      <c r="M8" s="26" t="s">
         <v>17</v>
       </c>
       <c r="N8" s="21"/>
@@ -1259,7 +1281,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="15.75" customHeight="1">
+    <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="16" t="s">
         <v>15</v>
       </c>
@@ -1286,7 +1308,7 @@
         <v>116</v>
       </c>
       <c r="L9" s="21"/>
-      <c r="M9" s="30" t="s">
+      <c r="M9" s="26" t="s">
         <v>17</v>
       </c>
       <c r="N9" s="21"/>
@@ -1307,7 +1329,7 @@
       <c r="W9" s="17"/>
       <c r="X9" s="10"/>
     </row>
-    <row r="10" spans="1:24" ht="15.75" customHeight="1">
+    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="16" t="s">
         <v>15</v>
       </c>
@@ -1334,7 +1356,7 @@
         <v>116</v>
       </c>
       <c r="L10" s="21"/>
-      <c r="M10" s="30" t="s">
+      <c r="M10" s="26" t="s">
         <v>17</v>
       </c>
       <c r="N10" s="21"/>
@@ -1355,7 +1377,7 @@
       <c r="W10" s="17"/>
       <c r="X10" s="10"/>
     </row>
-    <row r="11" spans="1:24" ht="15.75" customHeight="1">
+    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="16" t="s">
         <v>15</v>
       </c>
@@ -1417,7 +1439,7 @@
       <c r="W11" s="17"/>
       <c r="X11" s="10"/>
     </row>
-    <row r="12" spans="1:24" ht="15.75" customHeight="1">
+    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="16" t="s">
         <v>15</v>
       </c>
@@ -1479,7 +1501,7 @@
       <c r="W12" s="17"/>
       <c r="X12" s="10"/>
     </row>
-    <row r="13" spans="1:24" ht="15.75" customHeight="1">
+    <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="16" t="s">
         <v>15</v>
       </c>
@@ -1529,7 +1551,7 @@
       <c r="W13" s="17"/>
       <c r="X13" s="10"/>
     </row>
-    <row r="14" spans="1:24" ht="15.75" customHeight="1">
+    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="16" t="s">
         <v>15</v>
       </c>
@@ -1579,7 +1601,7 @@
       <c r="W14" s="17"/>
       <c r="X14" s="10"/>
     </row>
-    <row r="15" spans="1:24" ht="15.75" customHeight="1">
+    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="16" t="s">
         <v>15</v>
       </c>
@@ -1629,7 +1651,7 @@
       <c r="W15" s="17"/>
       <c r="X15" s="10"/>
     </row>
-    <row r="16" spans="1:24" ht="15.75" customHeight="1">
+    <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="16" t="s">
         <v>15</v>
       </c>
@@ -1691,7 +1713,7 @@
       <c r="W16" s="17"/>
       <c r="X16" s="10"/>
     </row>
-    <row r="17" spans="1:24" ht="15.75" customHeight="1">
+    <row r="17" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="16" t="s">
         <v>15</v>
       </c>
@@ -1753,7 +1775,7 @@
       <c r="W17" s="17"/>
       <c r="X17" s="10"/>
     </row>
-    <row r="18" spans="1:24" ht="15.75" customHeight="1">
+    <row r="18" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="16" t="s">
         <v>15</v>
       </c>
@@ -1803,7 +1825,7 @@
       <c r="W18" s="17"/>
       <c r="X18" s="10"/>
     </row>
-    <row r="19" spans="1:24" ht="15.75" customHeight="1">
+    <row r="19" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="16" t="s">
         <v>15</v>
       </c>
@@ -1865,7 +1887,7 @@
       <c r="W19" s="17"/>
       <c r="X19" s="10"/>
     </row>
-    <row r="20" spans="1:24" ht="15.75" customHeight="1">
+    <row r="20" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="16" t="s">
         <v>15</v>
       </c>
@@ -1931,11 +1953,11 @@
       <c r="W20" s="17"/>
       <c r="X20" s="10"/>
     </row>
-    <row r="21" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A21" s="31" t="s">
+    <row r="21" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="27" t="s">
         <v>30</v>
       </c>
       <c r="C21" s="21"/>
@@ -1999,11 +2021,11 @@
       <c r="W21" s="21"/>
       <c r="X21" s="10"/>
     </row>
-    <row r="22" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A22" s="31" t="s">
+    <row r="22" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="27" t="s">
         <v>31</v>
       </c>
       <c r="C22" s="21"/>
@@ -2065,11 +2087,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="23" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A23" s="31" t="s">
+    <row r="23" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="27" t="s">
         <v>32</v>
       </c>
       <c r="C23" s="21"/>
@@ -2131,11 +2153,11 @@
       <c r="W23" s="21"/>
       <c r="X23" s="10"/>
     </row>
-    <row r="24" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A24" s="31" t="s">
+    <row r="24" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="27" t="s">
         <v>33</v>
       </c>
       <c r="C24" s="21"/>
@@ -2193,11 +2215,11 @@
       <c r="W24" s="21"/>
       <c r="X24" s="10"/>
     </row>
-    <row r="25" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A25" s="31" t="s">
+    <row r="25" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="31" t="s">
+      <c r="B25" s="27" t="s">
         <v>34</v>
       </c>
       <c r="C25" s="21"/>
@@ -2234,7 +2256,7 @@
       <c r="R25" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="S25" s="32"/>
+      <c r="S25" s="28"/>
       <c r="T25" s="21"/>
       <c r="U25" s="21"/>
       <c r="V25" s="21" t="s">
@@ -2243,11 +2265,11 @@
       <c r="W25" s="21"/>
       <c r="X25" s="10"/>
     </row>
-    <row r="26" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A26" s="31" t="s">
+    <row r="26" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="31" t="s">
+      <c r="B26" s="27" t="s">
         <v>35</v>
       </c>
       <c r="C26" s="21"/>
@@ -2289,11 +2311,11 @@
       <c r="W26" s="21"/>
       <c r="X26" s="10"/>
     </row>
-    <row r="27" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A27" s="31" t="s">
+    <row r="27" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="31" t="s">
+      <c r="B27" s="27" t="s">
         <v>36</v>
       </c>
       <c r="C27" s="21"/>
@@ -2329,11 +2351,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A28" s="31" t="s">
+    <row r="28" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="27" t="s">
         <v>38</v>
       </c>
       <c r="C28" s="21"/>
@@ -2395,11 +2417,11 @@
         <v>128</v>
       </c>
     </row>
-    <row r="29" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A29" s="31" t="s">
+    <row r="29" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="31" t="s">
+      <c r="B29" s="27" t="s">
         <v>39</v>
       </c>
       <c r="C29" s="21"/>
@@ -2457,11 +2479,11 @@
       <c r="W29" s="21"/>
       <c r="X29" s="10"/>
     </row>
-    <row r="30" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A30" s="31" t="s">
+    <row r="30" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="31" t="s">
+      <c r="B30" s="27" t="s">
         <v>40</v>
       </c>
       <c r="C30" s="21"/>
@@ -2519,11 +2541,11 @@
       <c r="W30" s="21"/>
       <c r="X30" s="10"/>
     </row>
-    <row r="31" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A31" s="31" t="s">
+    <row r="31" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="31" t="s">
+      <c r="B31" s="27" t="s">
         <v>41</v>
       </c>
       <c r="C31" s="21"/>
@@ -2581,11 +2603,11 @@
       <c r="W31" s="21"/>
       <c r="X31" s="10"/>
     </row>
-    <row r="32" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A32" s="31" t="s">
+    <row r="32" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="31" t="s">
+      <c r="B32" s="27" t="s">
         <v>42</v>
       </c>
       <c r="C32" s="21"/>
@@ -2643,11 +2665,11 @@
       <c r="W32" s="21"/>
       <c r="X32" s="10"/>
     </row>
-    <row r="33" spans="1:24" s="13" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A33" s="31" t="s">
+    <row r="33" spans="1:24" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="31" t="s">
+      <c r="B33" s="27" t="s">
         <v>125</v>
       </c>
       <c r="C33" s="21"/>
@@ -2711,11 +2733,11 @@
       <c r="W33" s="21"/>
       <c r="X33" s="12"/>
     </row>
-    <row r="34" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A34" s="31" t="s">
+    <row r="34" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="31" t="s">
+      <c r="B34" s="27" t="s">
         <v>44</v>
       </c>
       <c r="C34" s="21"/>
@@ -2761,11 +2783,11 @@
       <c r="W34" s="21"/>
       <c r="X34" s="10"/>
     </row>
-    <row r="35" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A35" s="31" t="s">
+    <row r="35" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B35" s="31" t="s">
+      <c r="B35" s="27" t="s">
         <v>45</v>
       </c>
       <c r="C35" s="21"/>
@@ -2827,11 +2849,11 @@
       <c r="W35" s="21"/>
       <c r="X35" s="10"/>
     </row>
-    <row r="36" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A36" s="31" t="s">
+    <row r="36" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B36" s="31" t="s">
+      <c r="B36" s="27" t="s">
         <v>46</v>
       </c>
       <c r="C36" s="21"/>
@@ -2893,11 +2915,11 @@
       <c r="W36" s="21"/>
       <c r="X36" s="10"/>
     </row>
-    <row r="37" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A37" s="31" t="s">
+    <row r="37" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B37" s="31" t="s">
+      <c r="B37" s="27" t="s">
         <v>47</v>
       </c>
       <c r="C37" s="21"/>
@@ -2959,11 +2981,11 @@
       <c r="W37" s="21"/>
       <c r="X37" s="10"/>
     </row>
-    <row r="38" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A38" s="31" t="s">
+    <row r="38" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="31" t="s">
+      <c r="B38" s="27" t="s">
         <v>48</v>
       </c>
       <c r="C38" s="21"/>
@@ -3025,11 +3047,11 @@
       <c r="W38" s="21"/>
       <c r="X38" s="10"/>
     </row>
-    <row r="39" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A39" s="31" t="s">
+    <row r="39" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="31" t="s">
+      <c r="B39" s="27" t="s">
         <v>49</v>
       </c>
       <c r="C39" s="21"/>
@@ -3091,11 +3113,11 @@
       <c r="W39" s="21"/>
       <c r="X39" s="10"/>
     </row>
-    <row r="40" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A40" s="31" t="s">
+    <row r="40" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B40" s="31" t="s">
+      <c r="B40" s="27" t="s">
         <v>50</v>
       </c>
       <c r="C40" s="21"/>
@@ -3149,11 +3171,11 @@
       <c r="W40" s="21"/>
       <c r="X40" s="10"/>
     </row>
-    <row r="41" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A41" s="31" t="s">
+    <row r="41" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B41" s="31" t="s">
+      <c r="B41" s="27" t="s">
         <v>51</v>
       </c>
       <c r="C41" s="21"/>
@@ -3215,11 +3237,11 @@
       <c r="W41" s="21"/>
       <c r="X41" s="10"/>
     </row>
-    <row r="42" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A42" s="31" t="s">
+    <row r="42" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B42" s="31" t="s">
+      <c r="B42" s="27" t="s">
         <v>52</v>
       </c>
       <c r="C42" s="21"/>
@@ -3267,11 +3289,11 @@
       <c r="W42" s="21"/>
       <c r="X42" s="10"/>
     </row>
-    <row r="43" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A43" s="31" t="s">
+    <row r="43" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B43" s="31" t="s">
+      <c r="B43" s="27" t="s">
         <v>53</v>
       </c>
       <c r="C43" s="21"/>
@@ -3317,11 +3339,11 @@
       <c r="W43" s="21"/>
       <c r="X43" s="10"/>
     </row>
-    <row r="44" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A44" s="31" t="s">
+    <row r="44" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="31" t="s">
+      <c r="B44" s="27" t="s">
         <v>54</v>
       </c>
       <c r="C44" s="21"/>
@@ -3365,11 +3387,11 @@
       <c r="W44" s="21"/>
       <c r="X44" s="10"/>
     </row>
-    <row r="45" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A45" s="31" t="s">
+    <row r="45" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B45" s="31" t="s">
+      <c r="B45" s="27" t="s">
         <v>55</v>
       </c>
       <c r="C45" s="21"/>
@@ -3413,11 +3435,11 @@
       <c r="W45" s="21"/>
       <c r="X45" s="10"/>
     </row>
-    <row r="46" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A46" s="31" t="s">
+    <row r="46" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B46" s="31" t="s">
+      <c r="B46" s="27" t="s">
         <v>56</v>
       </c>
       <c r="C46" s="21"/>
@@ -3461,11 +3483,11 @@
       <c r="W46" s="21"/>
       <c r="X46" s="10"/>
     </row>
-    <row r="47" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A47" s="31" t="s">
+    <row r="47" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B47" s="31" t="s">
+      <c r="B47" s="27" t="s">
         <v>57</v>
       </c>
       <c r="C47" s="21"/>
@@ -3527,11 +3549,11 @@
       <c r="W47" s="21"/>
       <c r="X47" s="10"/>
     </row>
-    <row r="48" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A48" s="31" t="s">
+    <row r="48" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="B48" s="31" t="s">
+      <c r="B48" s="27" t="s">
         <v>59</v>
       </c>
       <c r="C48" s="21"/>
@@ -3593,15 +3615,15 @@
         <v>17</v>
       </c>
       <c r="W48" s="21"/>
-      <c r="X48" s="26" t="s">
+      <c r="X48" s="29" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A49" s="31" t="s">
+    <row r="49" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="B49" s="31" t="s">
+      <c r="B49" s="27" t="s">
         <v>61</v>
       </c>
       <c r="C49" s="21"/>
@@ -3663,13 +3685,13 @@
         <v>17</v>
       </c>
       <c r="W49" s="21"/>
-      <c r="X49" s="27"/>
-    </row>
-    <row r="50" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A50" s="31" t="s">
+      <c r="X49" s="30"/>
+    </row>
+    <row r="50" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="B50" s="31" t="s">
+      <c r="B50" s="27" t="s">
         <v>62</v>
       </c>
       <c r="C50" s="21"/>
@@ -3731,7 +3753,7 @@
       <c r="W50" s="21"/>
       <c r="X50" s="10"/>
     </row>
-    <row r="51" spans="1:24" s="15" customFormat="1" ht="15.75" customHeight="1">
+    <row r="51" spans="1:24" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="18" t="s">
         <v>63</v>
       </c>
@@ -3769,7 +3791,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="52" spans="1:24" ht="15.75" customHeight="1">
+    <row r="52" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="16" t="s">
         <v>63</v>
       </c>
@@ -3812,7 +3834,7 @@
       <c r="V52" s="17"/>
       <c r="W52" s="17"/>
     </row>
-    <row r="53" spans="1:24" ht="15.75" customHeight="1">
+    <row r="53" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="16" t="s">
         <v>63</v>
       </c>
@@ -3843,7 +3865,7 @@
       <c r="V53" s="17"/>
       <c r="W53" s="17"/>
     </row>
-    <row r="54" spans="1:24" ht="15.75" customHeight="1">
+    <row r="54" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="16" t="s">
         <v>63</v>
       </c>
@@ -3874,7 +3896,7 @@
       <c r="V54" s="17"/>
       <c r="W54" s="17"/>
     </row>
-    <row r="55" spans="1:24" ht="15.75" customHeight="1">
+    <row r="55" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="16" t="s">
         <v>63</v>
       </c>
@@ -3905,7 +3927,7 @@
       <c r="V55" s="17"/>
       <c r="W55" s="17"/>
     </row>
-    <row r="56" spans="1:24" ht="15.75" customHeight="1">
+    <row r="56" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="16" t="s">
         <v>112</v>
       </c>
@@ -3936,6 +3958,47 @@
       <c r="V56" s="20"/>
       <c r="W56" s="20"/>
     </row>
+    <row r="57" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A57" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="B57" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="C57" s="20"/>
+      <c r="D57" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="E57" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="F57" s="33"/>
+      <c r="G57" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="H57" s="33"/>
+      <c r="I57" s="33"/>
+      <c r="J57" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="K57" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="L57" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="M57" s="33"/>
+      <c r="N57" s="33"/>
+      <c r="O57" s="33"/>
+      <c r="P57" s="33"/>
+      <c r="Q57" s="33"/>
+      <c r="R57" s="33"/>
+      <c r="S57" s="33"/>
+      <c r="T57" s="33"/>
+      <c r="U57" s="33"/>
+      <c r="V57" s="33"/>
+      <c r="W57" s="33"/>
+    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="X48:X49"/>
@@ -3947,11 +4010,6 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3963,7 +4021,7 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="29.6640625" customWidth="1"/>
     <col min="2" max="2" width="28.1640625" customWidth="1"/>
@@ -3971,7 +4029,7 @@
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
         <v>70</v>
       </c>
@@ -3988,7 +4046,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15">
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
         <v>73</v>
       </c>
@@ -4001,7 +4059,7 @@
       <c r="D2" s="24"/>
       <c r="E2" s="24"/>
     </row>
-    <row r="3" spans="1:5" ht="15">
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
         <v>75</v>
       </c>
@@ -4014,7 +4072,7 @@
       <c r="D3" s="24"/>
       <c r="E3" s="24"/>
     </row>
-    <row r="4" spans="1:5" ht="15">
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
         <v>77</v>
       </c>
@@ -4027,7 +4085,7 @@
       <c r="D4" s="24"/>
       <c r="E4" s="24"/>
     </row>
-    <row r="5" spans="1:5" ht="15">
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
         <v>97</v>
       </c>
@@ -4042,7 +4100,7 @@
       </c>
       <c r="E5" s="24"/>
     </row>
-    <row r="6" spans="1:5" ht="15">
+    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
         <v>98</v>
       </c>
@@ -4057,7 +4115,7 @@
       </c>
       <c r="E6" s="24"/>
     </row>
-    <row r="7" spans="1:5" ht="15">
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
         <v>99</v>
       </c>
@@ -4072,7 +4130,7 @@
       </c>
       <c r="E7" s="24"/>
     </row>
-    <row r="8" spans="1:5" ht="15">
+    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
         <v>100</v>
       </c>
@@ -4087,7 +4145,7 @@
       </c>
       <c r="E8" s="24"/>
     </row>
-    <row r="9" spans="1:5" ht="15">
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
         <v>110</v>
       </c>
@@ -4102,7 +4160,7 @@
       </c>
       <c r="E9" s="24"/>
     </row>
-    <row r="10" spans="1:5" ht="15">
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
         <v>109</v>
       </c>
@@ -4117,7 +4175,7 @@
       </c>
       <c r="E10" s="24"/>
     </row>
-    <row r="11" spans="1:5" ht="15">
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
         <v>108</v>
       </c>
@@ -4132,7 +4190,7 @@
       </c>
       <c r="E11" s="24"/>
     </row>
-    <row r="12" spans="1:5" ht="15">
+    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
         <v>101</v>
       </c>
@@ -4147,7 +4205,7 @@
       </c>
       <c r="E12" s="24"/>
     </row>
-    <row r="13" spans="1:5" ht="15">
+    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
         <v>107</v>
       </c>
@@ -4162,7 +4220,7 @@
       </c>
       <c r="E13" s="24"/>
     </row>
-    <row r="14" spans="1:5" ht="15">
+    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
         <v>102</v>
       </c>
@@ -4177,7 +4235,7 @@
       </c>
       <c r="E14" s="24"/>
     </row>
-    <row r="15" spans="1:5" ht="15">
+    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
         <v>103</v>
       </c>
@@ -4192,7 +4250,7 @@
       </c>
       <c r="E15" s="24"/>
     </row>
-    <row r="16" spans="1:5" ht="15">
+    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
         <v>104</v>
       </c>
@@ -4207,7 +4265,7 @@
       </c>
       <c r="E16" s="24"/>
     </row>
-    <row r="17" spans="1:5" ht="15">
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
         <v>105</v>
       </c>
@@ -4222,7 +4280,7 @@
       </c>
       <c r="E17" s="24"/>
     </row>
-    <row r="18" spans="1:5" ht="15">
+    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
         <v>12</v>
       </c>
@@ -4237,7 +4295,7 @@
       </c>
       <c r="E18" s="24"/>
     </row>
-    <row r="19" spans="1:5" ht="15">
+    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
         <v>13</v>
       </c>
@@ -4252,7 +4310,7 @@
       </c>
       <c r="E19" s="24"/>
     </row>
-    <row r="20" spans="1:5" ht="15">
+    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
         <v>106</v>
       </c>
@@ -4267,7 +4325,7 @@
       </c>
       <c r="E20" s="24"/>
     </row>
-    <row r="21" spans="1:5" ht="15">
+    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
         <v>119</v>
       </c>
@@ -4286,10 +4344,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Päivitä uusi Sanktiorapsan nimi rooolit-Exceliin
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26812"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarihan/Desktop/Harja/harja/resources/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="8740" yWindow="1140" windowWidth="35320" windowHeight="22340" tabRatio="500"/>
   </bookViews>
@@ -429,7 +424,7 @@
     <t>W</t>
   </si>
   <si>
-    <t>Sanktioraportti</t>
+    <t>Sanktioiden yhteenveto</t>
   </si>
 </sst>
 </file>
@@ -552,8 +547,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -629,19 +628,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -982,10 +985,10 @@
       <pane xSplit="2" ySplit="6" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="H42" sqref="H42"/>
+      <selection pane="bottomRight" activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.5" bestFit="1" customWidth="1"/>
@@ -1012,7 +1015,7 @@
     <col min="24" max="24" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:24" ht="15.75" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1032,7 +1035,7 @@
       <c r="M1" s="33"/>
       <c r="N1" s="33"/>
     </row>
-    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:24" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="35" t="s">
@@ -1050,7 +1053,7 @@
       <c r="M2" s="33"/>
       <c r="N2" s="33"/>
     </row>
-    <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:24" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -1065,10 +1068,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:24" ht="15.75" customHeight="1">
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:24" ht="15.75" customHeight="1">
       <c r="C5" s="34" t="s">
         <v>6</v>
       </c>
@@ -1097,7 +1100,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:24" ht="15.75" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -1166,7 +1169,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:24" ht="15.75" customHeight="1">
       <c r="A7" s="16" t="s">
         <v>15</v>
       </c>
@@ -1234,7 +1237,7 @@
       <c r="W7" s="17"/>
       <c r="X7" s="10"/>
     </row>
-    <row r="8" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:24" ht="15.75" customHeight="1">
       <c r="A8" s="16" t="s">
         <v>15</v>
       </c>
@@ -1288,7 +1291,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:24" ht="15.75" customHeight="1">
       <c r="A9" s="16" t="s">
         <v>15</v>
       </c>
@@ -1336,7 +1339,7 @@
       <c r="W9" s="17"/>
       <c r="X9" s="10"/>
     </row>
-    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:24" ht="15.75" customHeight="1">
       <c r="A10" s="16" t="s">
         <v>15</v>
       </c>
@@ -1384,7 +1387,7 @@
       <c r="W10" s="17"/>
       <c r="X10" s="10"/>
     </row>
-    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:24" ht="15.75" customHeight="1">
       <c r="A11" s="16" t="s">
         <v>15</v>
       </c>
@@ -1446,7 +1449,7 @@
       <c r="W11" s="17"/>
       <c r="X11" s="10"/>
     </row>
-    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:24" ht="15.75" customHeight="1">
       <c r="A12" s="16" t="s">
         <v>15</v>
       </c>
@@ -1508,7 +1511,7 @@
       <c r="W12" s="17"/>
       <c r="X12" s="10"/>
     </row>
-    <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:24" ht="15.75" customHeight="1">
       <c r="A13" s="16" t="s">
         <v>15</v>
       </c>
@@ -1558,7 +1561,7 @@
       <c r="W13" s="17"/>
       <c r="X13" s="10"/>
     </row>
-    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:24" ht="15.75" customHeight="1">
       <c r="A14" s="16" t="s">
         <v>15</v>
       </c>
@@ -1608,7 +1611,7 @@
       <c r="W14" s="17"/>
       <c r="X14" s="10"/>
     </row>
-    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:24" ht="15.75" customHeight="1">
       <c r="A15" s="16" t="s">
         <v>15</v>
       </c>
@@ -1658,7 +1661,7 @@
       <c r="W15" s="17"/>
       <c r="X15" s="10"/>
     </row>
-    <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:24" ht="15.75" customHeight="1">
       <c r="A16" s="16" t="s">
         <v>15</v>
       </c>
@@ -1720,7 +1723,7 @@
       <c r="W16" s="17"/>
       <c r="X16" s="10"/>
     </row>
-    <row r="17" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:24" ht="15.75" customHeight="1">
       <c r="A17" s="16" t="s">
         <v>15</v>
       </c>
@@ -1782,7 +1785,7 @@
       <c r="W17" s="17"/>
       <c r="X17" s="10"/>
     </row>
-    <row r="18" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:24" ht="15.75" customHeight="1">
       <c r="A18" s="16" t="s">
         <v>15</v>
       </c>
@@ -1832,7 +1835,7 @@
       <c r="W18" s="17"/>
       <c r="X18" s="10"/>
     </row>
-    <row r="19" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:24" ht="15.75" customHeight="1">
       <c r="A19" s="16" t="s">
         <v>15</v>
       </c>
@@ -1894,7 +1897,7 @@
       <c r="W19" s="17"/>
       <c r="X19" s="10"/>
     </row>
-    <row r="20" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:24" ht="15.75" customHeight="1">
       <c r="A20" s="16" t="s">
         <v>15</v>
       </c>
@@ -1960,7 +1963,7 @@
       <c r="W20" s="17"/>
       <c r="X20" s="10"/>
     </row>
-    <row r="21" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:24" ht="15.75" customHeight="1">
       <c r="A21" s="27" t="s">
         <v>15</v>
       </c>
@@ -2028,7 +2031,7 @@
       <c r="W21" s="21"/>
       <c r="X21" s="10"/>
     </row>
-    <row r="22" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:24" ht="15.75" customHeight="1">
       <c r="A22" s="27" t="s">
         <v>15</v>
       </c>
@@ -2094,7 +2097,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="23" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:24" ht="15.75" customHeight="1">
       <c r="A23" s="27" t="s">
         <v>15</v>
       </c>
@@ -2160,7 +2163,7 @@
       <c r="W23" s="21"/>
       <c r="X23" s="10"/>
     </row>
-    <row r="24" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:24" ht="15.75" customHeight="1">
       <c r="A24" s="27" t="s">
         <v>15</v>
       </c>
@@ -2222,7 +2225,7 @@
       <c r="W24" s="21"/>
       <c r="X24" s="10"/>
     </row>
-    <row r="25" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:24" ht="15.75" customHeight="1">
       <c r="A25" s="27" t="s">
         <v>15</v>
       </c>
@@ -2272,7 +2275,7 @@
       <c r="W25" s="21"/>
       <c r="X25" s="10"/>
     </row>
-    <row r="26" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:24" ht="15.75" customHeight="1">
       <c r="A26" s="27" t="s">
         <v>15</v>
       </c>
@@ -2318,7 +2321,7 @@
       <c r="W26" s="21"/>
       <c r="X26" s="10"/>
     </row>
-    <row r="27" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:24" ht="15.75" customHeight="1">
       <c r="A27" s="27" t="s">
         <v>15</v>
       </c>
@@ -2358,7 +2361,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:24" ht="15.75" customHeight="1">
       <c r="A28" s="27" t="s">
         <v>15</v>
       </c>
@@ -2424,7 +2427,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="29" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:24" ht="15.75" customHeight="1">
       <c r="A29" s="27" t="s">
         <v>15</v>
       </c>
@@ -2486,7 +2489,7 @@
       <c r="W29" s="21"/>
       <c r="X29" s="10"/>
     </row>
-    <row r="30" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:24" ht="15.75" customHeight="1">
       <c r="A30" s="27" t="s">
         <v>15</v>
       </c>
@@ -2548,7 +2551,7 @@
       <c r="W30" s="21"/>
       <c r="X30" s="10"/>
     </row>
-    <row r="31" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:24" ht="15.75" customHeight="1">
       <c r="A31" s="27" t="s">
         <v>15</v>
       </c>
@@ -2610,7 +2613,7 @@
       <c r="W31" s="21"/>
       <c r="X31" s="10"/>
     </row>
-    <row r="32" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:24" ht="15.75" customHeight="1">
       <c r="A32" s="27" t="s">
         <v>15</v>
       </c>
@@ -2672,7 +2675,7 @@
       <c r="W32" s="21"/>
       <c r="X32" s="10"/>
     </row>
-    <row r="33" spans="1:24" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:24" s="13" customFormat="1" ht="15.75" customHeight="1">
       <c r="A33" s="27" t="s">
         <v>15</v>
       </c>
@@ -2740,7 +2743,7 @@
       <c r="W33" s="21"/>
       <c r="X33" s="12"/>
     </row>
-    <row r="34" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:24" ht="15.75" customHeight="1">
       <c r="A34" s="27" t="s">
         <v>43</v>
       </c>
@@ -2790,7 +2793,7 @@
       <c r="W34" s="21"/>
       <c r="X34" s="10"/>
     </row>
-    <row r="35" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:24" ht="15.75" customHeight="1">
       <c r="A35" s="27" t="s">
         <v>43</v>
       </c>
@@ -2856,7 +2859,7 @@
       <c r="W35" s="21"/>
       <c r="X35" s="10"/>
     </row>
-    <row r="36" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:24" ht="15.75" customHeight="1">
       <c r="A36" s="27" t="s">
         <v>43</v>
       </c>
@@ -2922,7 +2925,7 @@
       <c r="W36" s="21"/>
       <c r="X36" s="10"/>
     </row>
-    <row r="37" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:24" ht="15.75" customHeight="1">
       <c r="A37" s="27" t="s">
         <v>43</v>
       </c>
@@ -2988,7 +2991,7 @@
       <c r="W37" s="21"/>
       <c r="X37" s="10"/>
     </row>
-    <row r="38" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:24" ht="15.75" customHeight="1">
       <c r="A38" s="27" t="s">
         <v>43</v>
       </c>
@@ -3054,7 +3057,7 @@
       <c r="W38" s="21"/>
       <c r="X38" s="10"/>
     </row>
-    <row r="39" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:24" ht="15.75" customHeight="1">
       <c r="A39" s="27" t="s">
         <v>43</v>
       </c>
@@ -3120,7 +3123,7 @@
       <c r="W39" s="21"/>
       <c r="X39" s="10"/>
     </row>
-    <row r="40" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:24" ht="15.75" customHeight="1">
       <c r="A40" s="27" t="s">
         <v>43</v>
       </c>
@@ -3178,7 +3181,7 @@
       <c r="W40" s="21"/>
       <c r="X40" s="10"/>
     </row>
-    <row r="41" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:24" ht="15.75" customHeight="1">
       <c r="A41" s="27" t="s">
         <v>43</v>
       </c>
@@ -3244,7 +3247,7 @@
       <c r="W41" s="21"/>
       <c r="X41" s="10"/>
     </row>
-    <row r="42" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:24" ht="15.75" customHeight="1">
       <c r="A42" s="27" t="s">
         <v>43</v>
       </c>
@@ -3296,7 +3299,7 @@
       <c r="W42" s="21"/>
       <c r="X42" s="10"/>
     </row>
-    <row r="43" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:24" ht="15.75" customHeight="1">
       <c r="A43" s="27" t="s">
         <v>43</v>
       </c>
@@ -3346,7 +3349,7 @@
       <c r="W43" s="21"/>
       <c r="X43" s="10"/>
     </row>
-    <row r="44" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:24" ht="15.75" customHeight="1">
       <c r="A44" s="27" t="s">
         <v>43</v>
       </c>
@@ -3394,7 +3397,7 @@
       <c r="W44" s="21"/>
       <c r="X44" s="10"/>
     </row>
-    <row r="45" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:24" ht="15.75" customHeight="1">
       <c r="A45" s="27" t="s">
         <v>43</v>
       </c>
@@ -3442,7 +3445,7 @@
       <c r="W45" s="21"/>
       <c r="X45" s="10"/>
     </row>
-    <row r="46" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:24" ht="15.75" customHeight="1">
       <c r="A46" s="27" t="s">
         <v>43</v>
       </c>
@@ -3490,7 +3493,7 @@
       <c r="W46" s="21"/>
       <c r="X46" s="10"/>
     </row>
-    <row r="47" spans="1:24" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:24" s="30" customFormat="1" ht="15.75" customHeight="1">
       <c r="A47" s="27" t="s">
         <v>43</v>
       </c>
@@ -3548,7 +3551,7 @@
       <c r="W47" s="21"/>
       <c r="X47" s="29"/>
     </row>
-    <row r="48" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:24" ht="15.75" customHeight="1">
       <c r="A48" s="27" t="s">
         <v>43</v>
       </c>
@@ -3614,7 +3617,7 @@
       <c r="W48" s="21"/>
       <c r="X48" s="10"/>
     </row>
-    <row r="49" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:24" ht="15.75" customHeight="1">
       <c r="A49" s="27" t="s">
         <v>58</v>
       </c>
@@ -3684,7 +3687,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:24" ht="15.75" customHeight="1">
       <c r="A50" s="27" t="s">
         <v>58</v>
       </c>
@@ -3752,7 +3755,7 @@
       <c r="W50" s="21"/>
       <c r="X50" s="33"/>
     </row>
-    <row r="51" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:24" ht="15.75" customHeight="1">
       <c r="A51" s="27" t="s">
         <v>62</v>
       </c>
@@ -3818,7 +3821,7 @@
       <c r="W51" s="21"/>
       <c r="X51" s="10"/>
     </row>
-    <row r="52" spans="1:24" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:24" s="15" customFormat="1" ht="15.75" customHeight="1">
       <c r="A52" s="18" t="s">
         <v>63</v>
       </c>
@@ -3856,7 +3859,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="53" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:24" ht="15.75" customHeight="1">
       <c r="A53" s="16" t="s">
         <v>63</v>
       </c>
@@ -3899,7 +3902,7 @@
       <c r="V53" s="17"/>
       <c r="W53" s="17"/>
     </row>
-    <row r="54" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:24" ht="15.75" customHeight="1">
       <c r="A54" s="16" t="s">
         <v>63</v>
       </c>
@@ -3930,7 +3933,7 @@
       <c r="V54" s="17"/>
       <c r="W54" s="17"/>
     </row>
-    <row r="55" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:24" ht="15.75" customHeight="1">
       <c r="A55" s="16" t="s">
         <v>63</v>
       </c>
@@ -3961,7 +3964,7 @@
       <c r="V55" s="17"/>
       <c r="W55" s="17"/>
     </row>
-    <row r="56" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:24" ht="15.75" customHeight="1">
       <c r="A56" s="16" t="s">
         <v>63</v>
       </c>
@@ -3992,7 +3995,7 @@
       <c r="V56" s="17"/>
       <c r="W56" s="17"/>
     </row>
-    <row r="57" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:24" ht="15.75" customHeight="1">
       <c r="A57" s="16" t="s">
         <v>112</v>
       </c>
@@ -4023,7 +4026,7 @@
       <c r="V57" s="20"/>
       <c r="W57" s="20"/>
     </row>
-    <row r="58" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:24" ht="15.75" customHeight="1">
       <c r="A58" s="16" t="s">
         <v>131</v>
       </c>
@@ -4075,6 +4078,11 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4086,7 +4094,7 @@
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="29.6640625" customWidth="1"/>
     <col min="2" max="2" width="28.1640625" customWidth="1"/>
@@ -4094,7 +4102,7 @@
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="15">
       <c r="A1" s="22" t="s">
         <v>70</v>
       </c>
@@ -4111,7 +4119,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15">
       <c r="A2" s="23" t="s">
         <v>73</v>
       </c>
@@ -4124,7 +4132,7 @@
       <c r="D2" s="24"/>
       <c r="E2" s="24"/>
     </row>
-    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15">
       <c r="A3" s="23" t="s">
         <v>75</v>
       </c>
@@ -4137,7 +4145,7 @@
       <c r="D3" s="24"/>
       <c r="E3" s="24"/>
     </row>
-    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="15">
       <c r="A4" s="23" t="s">
         <v>77</v>
       </c>
@@ -4150,7 +4158,7 @@
       <c r="D4" s="24"/>
       <c r="E4" s="24"/>
     </row>
-    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="15">
       <c r="A5" s="23" t="s">
         <v>97</v>
       </c>
@@ -4165,7 +4173,7 @@
       </c>
       <c r="E5" s="24"/>
     </row>
-    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="15">
       <c r="A6" s="23" t="s">
         <v>98</v>
       </c>
@@ -4180,7 +4188,7 @@
       </c>
       <c r="E6" s="24"/>
     </row>
-    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="15">
       <c r="A7" s="23" t="s">
         <v>99</v>
       </c>
@@ -4195,7 +4203,7 @@
       </c>
       <c r="E7" s="24"/>
     </row>
-    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="15">
       <c r="A8" s="23" t="s">
         <v>100</v>
       </c>
@@ -4210,7 +4218,7 @@
       </c>
       <c r="E8" s="24"/>
     </row>
-    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="15">
       <c r="A9" s="23" t="s">
         <v>110</v>
       </c>
@@ -4225,7 +4233,7 @@
       </c>
       <c r="E9" s="24"/>
     </row>
-    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="15">
       <c r="A10" s="23" t="s">
         <v>109</v>
       </c>
@@ -4240,7 +4248,7 @@
       </c>
       <c r="E10" s="24"/>
     </row>
-    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="15">
       <c r="A11" s="23" t="s">
         <v>108</v>
       </c>
@@ -4255,7 +4263,7 @@
       </c>
       <c r="E11" s="24"/>
     </row>
-    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="15">
       <c r="A12" s="23" t="s">
         <v>101</v>
       </c>
@@ -4270,7 +4278,7 @@
       </c>
       <c r="E12" s="24"/>
     </row>
-    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="15">
       <c r="A13" s="23" t="s">
         <v>107</v>
       </c>
@@ -4285,7 +4293,7 @@
       </c>
       <c r="E13" s="24"/>
     </row>
-    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="15">
       <c r="A14" s="23" t="s">
         <v>102</v>
       </c>
@@ -4300,7 +4308,7 @@
       </c>
       <c r="E14" s="24"/>
     </row>
-    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="15">
       <c r="A15" s="23" t="s">
         <v>103</v>
       </c>
@@ -4315,7 +4323,7 @@
       </c>
       <c r="E15" s="24"/>
     </row>
-    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="15">
       <c r="A16" s="23" t="s">
         <v>104</v>
       </c>
@@ -4330,7 +4338,7 @@
       </c>
       <c r="E16" s="24"/>
     </row>
-    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="15">
       <c r="A17" s="23" t="s">
         <v>105</v>
       </c>
@@ -4345,7 +4353,7 @@
       </c>
       <c r="E17" s="24"/>
     </row>
-    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="15">
       <c r="A18" s="23" t="s">
         <v>12</v>
       </c>
@@ -4360,7 +4368,7 @@
       </c>
       <c r="E18" s="24"/>
     </row>
-    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="15">
       <c r="A19" s="23" t="s">
         <v>13</v>
       </c>
@@ -4375,7 +4383,7 @@
       </c>
       <c r="E19" s="24"/>
     </row>
-    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="15">
       <c r="A20" s="23" t="s">
         <v>106</v>
       </c>
@@ -4390,7 +4398,7 @@
       </c>
       <c r="E20" s="24"/>
     </row>
-    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="15">
       <c r="A21" s="23" t="s">
         <v>119</v>
       </c>
@@ -4409,5 +4417,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Nimeä vastuuhenkilö pienellä v:llä
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8740" yWindow="1140" windowWidth="35320" windowHeight="22340" tabRatio="500"/>
+    <workbookView xWindow="8740" yWindow="1140" windowWidth="35320" windowHeight="22340" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -337,9 +337,6 @@
     <t>Kayttaja</t>
   </si>
   <si>
-    <t>Vastuuhenkilo</t>
-  </si>
-  <si>
     <t>Paivystaja</t>
   </si>
   <si>
@@ -425,6 +422,9 @@
   </si>
   <si>
     <t>Sanktioiden yhteenveto</t>
+  </si>
+  <si>
+    <t>vastuuhenkilo</t>
   </si>
 </sst>
 </file>
@@ -981,7 +981,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane xSplit="2" ySplit="6" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
@@ -1021,7 +1021,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D1" s="33"/>
       <c r="E1" s="33"/>
@@ -1154,7 +1154,7 @@
         <v>90</v>
       </c>
       <c r="S6" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="T6" s="9" t="s">
         <v>91</v>
@@ -1166,7 +1166,7 @@
         <v>82</v>
       </c>
       <c r="W6" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:24" ht="15.75" customHeight="1">
@@ -1178,10 +1178,10 @@
       </c>
       <c r="C7" s="17"/>
       <c r="D7" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F7" s="17" t="s">
         <v>17</v>
@@ -1196,10 +1196,10 @@
         <v>17</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K7" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L7" s="17" t="s">
         <v>17</v>
@@ -1214,10 +1214,10 @@
         <v>17</v>
       </c>
       <c r="P7" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q7" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="R7" s="17" t="s">
         <v>17</v>
@@ -1246,10 +1246,10 @@
       </c>
       <c r="C8" s="17"/>
       <c r="D8" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F8" s="17" t="s">
         <v>17</v>
@@ -1258,10 +1258,10 @@
       <c r="H8" s="21"/>
       <c r="I8" s="21"/>
       <c r="J8" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K8" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L8" s="21"/>
       <c r="M8" s="26" t="s">
@@ -1288,7 +1288,7 @@
       </c>
       <c r="W8" s="17"/>
       <c r="X8" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="15.75" customHeight="1">
@@ -1300,10 +1300,10 @@
       </c>
       <c r="C9" s="17"/>
       <c r="D9" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F9" s="17" t="s">
         <v>17</v>
@@ -1312,10 +1312,10 @@
       <c r="H9" s="21"/>
       <c r="I9" s="21"/>
       <c r="J9" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K9" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L9" s="21"/>
       <c r="M9" s="26" t="s">
@@ -1344,14 +1344,14 @@
         <v>15</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C10" s="17"/>
       <c r="D10" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F10" s="17" t="s">
         <v>17</v>
@@ -1360,10 +1360,10 @@
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
       <c r="J10" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K10" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L10" s="21"/>
       <c r="M10" s="26" t="s">
@@ -1396,10 +1396,10 @@
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>17</v>
@@ -1414,10 +1414,10 @@
         <v>17</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K11" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L11" s="17" t="s">
         <v>17</v>
@@ -1430,10 +1430,10 @@
       </c>
       <c r="O11" s="17"/>
       <c r="P11" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q11" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="R11" s="17" t="s">
         <v>17</v>
@@ -1458,10 +1458,10 @@
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F12" s="17" t="s">
         <v>17</v>
@@ -1476,10 +1476,10 @@
         <v>17</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K12" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L12" s="17" t="s">
         <v>17</v>
@@ -1492,10 +1492,10 @@
       </c>
       <c r="O12" s="17"/>
       <c r="P12" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q12" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="R12" s="17" t="s">
         <v>17</v>
@@ -1520,7 +1520,7 @@
       </c>
       <c r="C13" s="17"/>
       <c r="D13" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E13" s="17" t="s">
         <v>17</v>
@@ -1532,7 +1532,7 @@
       <c r="H13" s="21"/>
       <c r="I13" s="21"/>
       <c r="J13" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K13" s="17" t="s">
         <v>17</v>
@@ -1546,10 +1546,10 @@
       <c r="N13" s="21"/>
       <c r="O13" s="17"/>
       <c r="P13" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q13" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="R13" s="21"/>
       <c r="S13" s="17"/>
@@ -1570,7 +1570,7 @@
       </c>
       <c r="C14" s="17"/>
       <c r="D14" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E14" s="17" t="s">
         <v>17</v>
@@ -1582,7 +1582,7 @@
       <c r="H14" s="21"/>
       <c r="I14" s="21"/>
       <c r="J14" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K14" s="17" t="s">
         <v>17</v>
@@ -1596,10 +1596,10 @@
       <c r="N14" s="21"/>
       <c r="O14" s="17"/>
       <c r="P14" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q14" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="R14" s="21"/>
       <c r="S14" s="17"/>
@@ -1616,11 +1616,11 @@
         <v>15</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E15" s="17" t="s">
         <v>17</v>
@@ -1632,7 +1632,7 @@
       <c r="H15" s="21"/>
       <c r="I15" s="21"/>
       <c r="J15" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K15" s="17" t="s">
         <v>17</v>
@@ -1646,10 +1646,10 @@
       <c r="N15" s="21"/>
       <c r="O15" s="17"/>
       <c r="P15" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q15" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="R15" s="21"/>
       <c r="S15" s="17"/>
@@ -1670,7 +1670,7 @@
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E16" s="17" t="s">
         <v>17</v>
@@ -1688,7 +1688,7 @@
         <v>17</v>
       </c>
       <c r="J16" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K16" s="17" t="s">
         <v>17</v>
@@ -1704,10 +1704,10 @@
       </c>
       <c r="O16" s="17"/>
       <c r="P16" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q16" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="R16" s="17" t="s">
         <v>17</v>
@@ -1732,7 +1732,7 @@
       </c>
       <c r="C17" s="17"/>
       <c r="D17" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E17" s="17" t="s">
         <v>17</v>
@@ -1750,7 +1750,7 @@
         <v>17</v>
       </c>
       <c r="J17" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K17" s="17" t="s">
         <v>17</v>
@@ -1766,10 +1766,10 @@
       </c>
       <c r="O17" s="17"/>
       <c r="P17" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q17" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="R17" s="17" t="s">
         <v>17</v>
@@ -1794,7 +1794,7 @@
       </c>
       <c r="C18" s="17"/>
       <c r="D18" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E18" s="17" t="s">
         <v>17</v>
@@ -1806,10 +1806,10 @@
       <c r="H18" s="21"/>
       <c r="I18" s="21"/>
       <c r="J18" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K18" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L18" s="17" t="s">
         <v>17</v>
@@ -1820,10 +1820,10 @@
       <c r="N18" s="21"/>
       <c r="O18" s="17"/>
       <c r="P18" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q18" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="R18" s="21"/>
       <c r="S18" s="21"/>
@@ -1844,7 +1844,7 @@
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E19" s="17" t="s">
         <v>17</v>
@@ -1862,7 +1862,7 @@
         <v>17</v>
       </c>
       <c r="J19" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K19" s="17" t="s">
         <v>17</v>
@@ -1878,10 +1878,10 @@
       </c>
       <c r="O19" s="17"/>
       <c r="P19" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q19" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="R19" s="17" t="s">
         <v>17</v>
@@ -1906,16 +1906,16 @@
       </c>
       <c r="C20" s="17"/>
       <c r="D20" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F20" s="17" t="s">
         <v>17</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H20" s="17" t="s">
         <v>17</v>
@@ -1924,13 +1924,13 @@
         <v>17</v>
       </c>
       <c r="J20" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K20" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L20" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M20" s="17" t="s">
         <v>17</v>
@@ -1942,16 +1942,16 @@
         <v>17</v>
       </c>
       <c r="P20" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q20" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="R20" s="17" t="s">
         <v>17</v>
       </c>
       <c r="S20" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="T20" s="17" t="s">
         <v>17</v>
@@ -1972,16 +1972,16 @@
       </c>
       <c r="C21" s="21"/>
       <c r="D21" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E21" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F21" s="21" t="s">
         <v>17</v>
       </c>
       <c r="G21" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H21" s="21" t="s">
         <v>17</v>
@@ -1990,13 +1990,13 @@
         <v>17</v>
       </c>
       <c r="J21" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K21" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L21" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M21" s="21" t="s">
         <v>17</v>
@@ -2008,16 +2008,16 @@
         <v>17</v>
       </c>
       <c r="P21" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q21" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="R21" s="21" t="s">
         <v>17</v>
       </c>
       <c r="S21" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="T21" s="21" t="s">
         <v>17</v>
@@ -2040,10 +2040,10 @@
       </c>
       <c r="C22" s="21"/>
       <c r="D22" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F22" s="21" t="s">
         <v>17</v>
@@ -2058,10 +2058,10 @@
         <v>17</v>
       </c>
       <c r="J22" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K22" s="21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L22" s="21" t="s">
         <v>17</v>
@@ -2094,7 +2094,7 @@
       </c>
       <c r="W22" s="21"/>
       <c r="X22" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="23" spans="1:24" ht="15.75" customHeight="1">
@@ -2106,10 +2106,10 @@
       </c>
       <c r="C23" s="21"/>
       <c r="D23" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F23" s="21" t="s">
         <v>17</v>
@@ -2124,13 +2124,13 @@
         <v>17</v>
       </c>
       <c r="J23" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K23" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L23" s="21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M23" s="21" t="s">
         <v>17</v>
@@ -2142,16 +2142,16 @@
         <v>17</v>
       </c>
       <c r="P23" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q23" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="R23" s="21" t="s">
         <v>17</v>
       </c>
       <c r="S23" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="T23" s="21" t="s">
         <v>17</v>
@@ -2172,10 +2172,10 @@
       </c>
       <c r="C24" s="21"/>
       <c r="D24" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F24" s="21" t="s">
         <v>17</v>
@@ -2190,10 +2190,10 @@
         <v>17</v>
       </c>
       <c r="J24" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K24" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L24" s="21" t="s">
         <v>17</v>
@@ -2234,34 +2234,34 @@
       </c>
       <c r="C25" s="21"/>
       <c r="D25" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F25" s="21"/>
       <c r="G25" s="21"/>
       <c r="H25" s="21"/>
       <c r="I25" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J25" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K25" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L25" s="21"/>
       <c r="M25" s="21"/>
       <c r="N25" s="21"/>
       <c r="O25" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P25" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q25" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="R25" s="21" t="s">
         <v>17</v>
@@ -2270,7 +2270,7 @@
       <c r="T25" s="21"/>
       <c r="U25" s="21"/>
       <c r="V25" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W25" s="21"/>
       <c r="X25" s="10"/>
@@ -2284,10 +2284,10 @@
       </c>
       <c r="C26" s="21"/>
       <c r="D26" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F26" s="21" t="s">
         <v>17</v>
@@ -2296,10 +2296,10 @@
       <c r="H26" s="21"/>
       <c r="I26" s="21"/>
       <c r="J26" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K26" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L26" s="21"/>
       <c r="M26" s="21" t="s">
@@ -2330,20 +2330,20 @@
       </c>
       <c r="C27" s="21"/>
       <c r="D27" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F27" s="21"/>
       <c r="G27" s="21"/>
       <c r="H27" s="21"/>
       <c r="I27" s="21"/>
       <c r="J27" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K27" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L27" s="21"/>
       <c r="M27" s="21"/>
@@ -2370,10 +2370,10 @@
       </c>
       <c r="C28" s="21"/>
       <c r="D28" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F28" s="21" t="s">
         <v>17</v>
@@ -2388,10 +2388,10 @@
         <v>17</v>
       </c>
       <c r="J28" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K28" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L28" s="21" t="s">
         <v>17</v>
@@ -2404,10 +2404,10 @@
       </c>
       <c r="O28" s="21"/>
       <c r="P28" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q28" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="R28" s="21" t="s">
         <v>17</v>
@@ -2421,10 +2421,10 @@
       <c r="U28" s="21"/>
       <c r="V28" s="21"/>
       <c r="W28" s="21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="X28" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:24" ht="15.75" customHeight="1">
@@ -2436,10 +2436,10 @@
       </c>
       <c r="C29" s="21"/>
       <c r="D29" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F29" s="21" t="s">
         <v>17</v>
@@ -2454,10 +2454,10 @@
         <v>17</v>
       </c>
       <c r="J29" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K29" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L29" s="21" t="s">
         <v>17</v>
@@ -2470,10 +2470,10 @@
       </c>
       <c r="O29" s="21"/>
       <c r="P29" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q29" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="R29" s="21" t="s">
         <v>17</v>
@@ -2498,10 +2498,10 @@
       </c>
       <c r="C30" s="21"/>
       <c r="D30" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E30" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F30" s="21" t="s">
         <v>17</v>
@@ -2516,10 +2516,10 @@
         <v>17</v>
       </c>
       <c r="J30" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K30" s="21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L30" s="21" t="s">
         <v>17</v>
@@ -2532,10 +2532,10 @@
       </c>
       <c r="O30" s="21"/>
       <c r="P30" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q30" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="R30" s="21" t="s">
         <v>17</v>
@@ -2560,10 +2560,10 @@
       </c>
       <c r="C31" s="21"/>
       <c r="D31" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F31" s="21" t="s">
         <v>17</v>
@@ -2578,10 +2578,10 @@
         <v>17</v>
       </c>
       <c r="J31" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K31" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L31" s="21" t="s">
         <v>17</v>
@@ -2594,10 +2594,10 @@
       </c>
       <c r="O31" s="21"/>
       <c r="P31" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q31" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="R31" s="21" t="s">
         <v>17</v>
@@ -2622,10 +2622,10 @@
       </c>
       <c r="C32" s="21"/>
       <c r="D32" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E32" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F32" s="21" t="s">
         <v>17</v>
@@ -2640,10 +2640,10 @@
         <v>17</v>
       </c>
       <c r="J32" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K32" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L32" s="21" t="s">
         <v>17</v>
@@ -2656,10 +2656,10 @@
       </c>
       <c r="O32" s="21"/>
       <c r="P32" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q32" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="R32" s="21" t="s">
         <v>17</v>
@@ -2680,35 +2680,35 @@
         <v>15</v>
       </c>
       <c r="B33" s="27" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C33" s="21"/>
       <c r="D33" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E33" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F33" s="21" t="s">
         <v>17</v>
       </c>
       <c r="G33" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H33" s="21" t="s">
         <v>17</v>
       </c>
       <c r="I33" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J33" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K33" s="21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L33" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M33" s="21" t="s">
         <v>17</v>
@@ -2720,16 +2720,16 @@
         <v>17</v>
       </c>
       <c r="P33" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q33" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="R33" s="21" t="s">
         <v>17</v>
       </c>
       <c r="S33" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="T33" s="21" t="s">
         <v>17</v>
@@ -3498,7 +3498,7 @@
         <v>43</v>
       </c>
       <c r="B47" s="27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C47" s="21"/>
       <c r="D47" s="21" t="s">
@@ -3764,10 +3764,10 @@
       </c>
       <c r="C51" s="21"/>
       <c r="D51" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E51" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F51" s="21" t="s">
         <v>17</v>
@@ -3782,10 +3782,10 @@
         <v>17</v>
       </c>
       <c r="J51" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K51" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L51" s="21" t="s">
         <v>17</v>
@@ -3800,10 +3800,10 @@
         <v>17</v>
       </c>
       <c r="P51" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q51" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="R51" s="21" t="s">
         <v>17</v>
@@ -3813,7 +3813,7 @@
         <v>17</v>
       </c>
       <c r="U51" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="V51" s="21" t="s">
         <v>17</v>
@@ -3830,7 +3830,7 @@
       </c>
       <c r="C52" s="19"/>
       <c r="D52" s="19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E52" s="19"/>
       <c r="F52" s="19"/>
@@ -3838,7 +3838,7 @@
       <c r="H52" s="19"/>
       <c r="I52" s="19"/>
       <c r="J52" s="19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K52" s="19"/>
       <c r="L52" s="19"/>
@@ -3846,7 +3846,7 @@
       <c r="N52" s="19"/>
       <c r="O52" s="19"/>
       <c r="P52" s="19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q52" s="19"/>
       <c r="R52" s="19"/>
@@ -3868,7 +3868,7 @@
       </c>
       <c r="C53" s="17"/>
       <c r="D53" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E53" s="17"/>
       <c r="F53" s="17" t="s">
@@ -3911,7 +3911,7 @@
       </c>
       <c r="C54" s="17"/>
       <c r="D54" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E54" s="17"/>
       <c r="F54" s="17"/>
@@ -3942,7 +3942,7 @@
       </c>
       <c r="C55" s="17"/>
       <c r="D55" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E55" s="17"/>
       <c r="F55" s="17"/>
@@ -3973,7 +3973,7 @@
       </c>
       <c r="C56" s="17"/>
       <c r="D56" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E56" s="17"/>
       <c r="F56" s="17"/>
@@ -3997,14 +3997,14 @@
     </row>
     <row r="57" spans="1:24" ht="15.75" customHeight="1">
       <c r="A57" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="B57" s="16" t="s">
         <v>112</v>
-      </c>
-      <c r="B57" s="16" t="s">
-        <v>113</v>
       </c>
       <c r="C57" s="20"/>
       <c r="D57" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E57" s="20"/>
       <c r="F57" s="20"/>
@@ -4028,32 +4028,32 @@
     </row>
     <row r="58" spans="1:24" ht="15.75" customHeight="1">
       <c r="A58" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="B58" s="16" t="s">
         <v>131</v>
-      </c>
-      <c r="B58" s="16" t="s">
-        <v>132</v>
       </c>
       <c r="C58" s="20"/>
       <c r="D58" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E58" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F58" s="31"/>
       <c r="G58" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H58" s="31"/>
       <c r="I58" s="31"/>
       <c r="J58" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K58" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L58" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M58" s="31"/>
       <c r="N58" s="31"/>
@@ -4090,8 +4090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -4116,7 +4116,7 @@
         <v>94</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15">
@@ -4220,7 +4220,7 @@
     </row>
     <row r="9" spans="1:5" ht="15">
       <c r="A9" s="23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B9" s="23" t="s">
         <v>84</v>
@@ -4229,13 +4229,13 @@
         <v>5</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E9" s="24"/>
     </row>
     <row r="10" spans="1:5" ht="15">
       <c r="A10" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B10" s="23" t="s">
         <v>85</v>
@@ -4244,13 +4244,13 @@
         <v>5</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E10" s="24"/>
     </row>
     <row r="11" spans="1:5" ht="15">
       <c r="A11" s="23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B11" s="23" t="s">
         <v>86</v>
@@ -4259,7 +4259,7 @@
         <v>5</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E11" s="24"/>
     </row>
@@ -4280,7 +4280,7 @@
     </row>
     <row r="13" spans="1:5" ht="15">
       <c r="A13" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B13" s="23" t="s">
         <v>88</v>
@@ -4340,7 +4340,7 @@
     </row>
     <row r="17" spans="1:5" ht="15">
       <c r="A17" s="23" t="s">
-        <v>105</v>
+        <v>134</v>
       </c>
       <c r="B17" s="23" t="s">
         <v>11</v>
@@ -4385,7 +4385,7 @@
     </row>
     <row r="20" spans="1:5" ht="15">
       <c r="A20" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B20" s="23" t="s">
         <v>93</v>
@@ -4400,10 +4400,10 @@
     </row>
     <row r="21" spans="1:5" ht="15">
       <c r="A21" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="B21" s="23" t="s">
         <v>119</v>
-      </c>
-      <c r="B21" s="23" t="s">
-        <v>120</v>
       </c>
       <c r="C21" s="23" t="s">
         <v>4</v>
@@ -4412,7 +4412,7 @@
         <v>95</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lisää Raportit Laskutusyhteenveto rooli-Exceliin
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8740" yWindow="1140" windowWidth="35320" windowHeight="22340" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="8740" yWindow="1140" windowWidth="35320" windowHeight="22340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="136">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -425,6 +425,9 @@
   </si>
   <si>
     <t>vastuuhenkilo</t>
+  </si>
+  <si>
+    <t>Laskutusyhteenveto</t>
   </si>
 </sst>
 </file>
@@ -547,7 +550,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -565,8 +568,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -625,10 +632,14 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -637,6 +648,8 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -645,6 +658,8 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -979,13 +994,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X58"/>
+  <dimension ref="A1:X59"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane xSplit="2" ySplit="6" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B48" sqref="B48"/>
+      <selection pane="bottomRight" activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1020,38 +1035,38 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="37" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
     </row>
     <row r="2" spans="1:24" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
     </row>
     <row r="3" spans="1:24" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
@@ -1072,30 +1087,30 @@
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:24" ht="15.75" customHeight="1">
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="J5" s="34" t="s">
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="J5" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
-      <c r="P5" s="34" t="s">
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
+      <c r="P5" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="Q5" s="33"/>
-      <c r="R5" s="33"/>
-      <c r="S5" s="33"/>
-      <c r="T5" s="33"/>
-      <c r="U5" s="33"/>
-      <c r="V5" s="33"/>
+      <c r="Q5" s="35"/>
+      <c r="R5" s="35"/>
+      <c r="S5" s="35"/>
+      <c r="T5" s="35"/>
+      <c r="U5" s="35"/>
+      <c r="V5" s="35"/>
       <c r="X5" s="5" t="s">
         <v>14</v>
       </c>
@@ -2743,33 +2758,31 @@
       <c r="W33" s="21"/>
       <c r="X33" s="12"/>
     </row>
-    <row r="34" spans="1:24" ht="15.75" customHeight="1">
+    <row r="34" spans="1:24" s="33" customFormat="1" ht="15.75" customHeight="1">
       <c r="A34" s="27" t="s">
         <v>43</v>
       </c>
       <c r="B34" s="27" t="s">
-        <v>44</v>
+        <v>135</v>
       </c>
       <c r="C34" s="21"/>
       <c r="D34" s="21" t="s">
-        <v>17</v>
+        <v>115</v>
       </c>
       <c r="E34" s="21" t="s">
-        <v>17</v>
+        <v>115</v>
       </c>
       <c r="F34" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="G34" s="21" t="s">
-        <v>19</v>
-      </c>
+      <c r="G34" s="21"/>
       <c r="H34" s="21"/>
       <c r="I34" s="21"/>
       <c r="J34" s="21" t="s">
-        <v>17</v>
+        <v>115</v>
       </c>
       <c r="K34" s="21" t="s">
-        <v>17</v>
+        <v>115</v>
       </c>
       <c r="L34" s="21"/>
       <c r="M34" s="21" t="s">
@@ -2785,20 +2798,18 @@
       </c>
       <c r="R34" s="21"/>
       <c r="S34" s="21"/>
-      <c r="T34" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="T34" s="21"/>
       <c r="U34" s="21"/>
       <c r="V34" s="21"/>
       <c r="W34" s="21"/>
-      <c r="X34" s="10"/>
+      <c r="X34" s="32"/>
     </row>
     <row r="35" spans="1:24" ht="15.75" customHeight="1">
       <c r="A35" s="27" t="s">
         <v>43</v>
       </c>
       <c r="B35" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C35" s="21"/>
       <c r="D35" s="21" t="s">
@@ -2811,51 +2822,35 @@
         <v>17</v>
       </c>
       <c r="G35" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="H35" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="I35" s="21" t="s">
-        <v>17</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="H35" s="21"/>
+      <c r="I35" s="21"/>
       <c r="J35" s="21" t="s">
         <v>17</v>
       </c>
       <c r="K35" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="L35" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="L35" s="21"/>
       <c r="M35" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="N35" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="O35" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="N35" s="21"/>
+      <c r="O35" s="21"/>
       <c r="P35" s="21" t="s">
         <v>17</v>
       </c>
       <c r="Q35" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="R35" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="S35" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="R35" s="21"/>
+      <c r="S35" s="21"/>
       <c r="T35" s="21" t="s">
         <v>17</v>
       </c>
       <c r="U35" s="21"/>
-      <c r="V35" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="V35" s="21"/>
       <c r="W35" s="21"/>
       <c r="X35" s="10"/>
     </row>
@@ -2864,7 +2859,7 @@
         <v>43</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C36" s="21"/>
       <c r="D36" s="21" t="s">
@@ -2930,7 +2925,7 @@
         <v>43</v>
       </c>
       <c r="B37" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C37" s="21"/>
       <c r="D37" s="21" t="s">
@@ -2996,7 +2991,7 @@
         <v>43</v>
       </c>
       <c r="B38" s="27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C38" s="21"/>
       <c r="D38" s="21" t="s">
@@ -3062,7 +3057,7 @@
         <v>43</v>
       </c>
       <c r="B39" s="27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C39" s="21"/>
       <c r="D39" s="21" t="s">
@@ -3128,7 +3123,7 @@
         <v>43</v>
       </c>
       <c r="B40" s="27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C40" s="21"/>
       <c r="D40" s="21" t="s">
@@ -3155,12 +3150,18 @@
       <c r="K40" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="L40" s="21"/>
+      <c r="L40" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="M40" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="N40" s="21"/>
-      <c r="O40" s="21"/>
+      <c r="N40" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="O40" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="P40" s="21" t="s">
         <v>17</v>
       </c>
@@ -3170,7 +3171,9 @@
       <c r="R40" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="S40" s="21"/>
+      <c r="S40" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="T40" s="21" t="s">
         <v>17</v>
       </c>
@@ -3186,7 +3189,7 @@
         <v>43</v>
       </c>
       <c r="B41" s="27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C41" s="21"/>
       <c r="D41" s="21" t="s">
@@ -3213,18 +3216,12 @@
       <c r="K41" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="L41" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="L41" s="21"/>
       <c r="M41" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="N41" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="O41" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="N41" s="21"/>
+      <c r="O41" s="21"/>
       <c r="P41" s="21" t="s">
         <v>17</v>
       </c>
@@ -3234,9 +3231,7 @@
       <c r="R41" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="S41" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="S41" s="21"/>
       <c r="T41" s="21" t="s">
         <v>17</v>
       </c>
@@ -3252,7 +3247,7 @@
         <v>43</v>
       </c>
       <c r="B42" s="27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C42" s="21"/>
       <c r="D42" s="21" t="s">
@@ -3261,11 +3256,15 @@
       <c r="E42" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="F42" s="21"/>
+      <c r="F42" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="G42" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="H42" s="21"/>
+      <c r="H42" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="I42" s="21" t="s">
         <v>17</v>
       </c>
@@ -3275,9 +3274,15 @@
       <c r="K42" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="L42" s="21"/>
-      <c r="M42" s="21"/>
-      <c r="N42" s="21"/>
+      <c r="L42" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="M42" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="N42" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="O42" s="21" t="s">
         <v>17</v>
       </c>
@@ -3287,8 +3292,12 @@
       <c r="Q42" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="R42" s="21"/>
-      <c r="S42" s="21"/>
+      <c r="R42" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="S42" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="T42" s="21" t="s">
         <v>17</v>
       </c>
@@ -3304,7 +3313,7 @@
         <v>43</v>
       </c>
       <c r="B43" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C43" s="21"/>
       <c r="D43" s="21" t="s">
@@ -3313,14 +3322,14 @@
       <c r="E43" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="F43" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="G43" s="21"/>
-      <c r="H43" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="I43" s="21"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H43" s="21"/>
+      <c r="I43" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="J43" s="21" t="s">
         <v>17</v>
       </c>
@@ -3328,13 +3337,11 @@
         <v>17</v>
       </c>
       <c r="L43" s="21"/>
-      <c r="M43" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="N43" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="O43" s="21"/>
+      <c r="M43" s="21"/>
+      <c r="N43" s="21"/>
+      <c r="O43" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="P43" s="21" t="s">
         <v>17</v>
       </c>
@@ -3343,9 +3350,13 @@
       </c>
       <c r="R43" s="21"/>
       <c r="S43" s="21"/>
-      <c r="T43" s="21"/>
+      <c r="T43" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="U43" s="21"/>
-      <c r="V43" s="21"/>
+      <c r="V43" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="W43" s="21"/>
       <c r="X43" s="10"/>
     </row>
@@ -3354,7 +3365,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C44" s="21"/>
       <c r="D44" s="21" t="s">
@@ -3367,7 +3378,9 @@
         <v>17</v>
       </c>
       <c r="G44" s="21"/>
-      <c r="H44" s="21"/>
+      <c r="H44" s="21" t="s">
+        <v>19</v>
+      </c>
       <c r="I44" s="21"/>
       <c r="J44" s="21" t="s">
         <v>17</v>
@@ -3379,7 +3392,9 @@
       <c r="M44" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="N44" s="21"/>
+      <c r="N44" s="21" t="s">
+        <v>19</v>
+      </c>
       <c r="O44" s="21"/>
       <c r="P44" s="21" t="s">
         <v>17</v>
@@ -3389,9 +3404,7 @@
       </c>
       <c r="R44" s="21"/>
       <c r="S44" s="21"/>
-      <c r="T44" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="T44" s="21"/>
       <c r="U44" s="21"/>
       <c r="V44" s="21"/>
       <c r="W44" s="21"/>
@@ -3402,7 +3415,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C45" s="21"/>
       <c r="D45" s="21" t="s">
@@ -3450,7 +3463,7 @@
         <v>43</v>
       </c>
       <c r="B46" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C46" s="21"/>
       <c r="D46" s="21" t="s">
@@ -3493,12 +3506,12 @@
       <c r="W46" s="21"/>
       <c r="X46" s="10"/>
     </row>
-    <row r="47" spans="1:24" s="30" customFormat="1" ht="15.75" customHeight="1">
+    <row r="47" spans="1:24" ht="15.75" customHeight="1">
       <c r="A47" s="27" t="s">
         <v>43</v>
       </c>
       <c r="B47" s="27" t="s">
-        <v>133</v>
+        <v>56</v>
       </c>
       <c r="C47" s="21"/>
       <c r="D47" s="21" t="s">
@@ -3510,15 +3523,9 @@
       <c r="F47" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="G47" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="H47" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="I47" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="G47" s="21"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="21"/>
       <c r="J47" s="21" t="s">
         <v>17</v>
       </c>
@@ -3537,26 +3544,22 @@
       <c r="Q47" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="R47" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="R47" s="21"/>
       <c r="S47" s="21"/>
       <c r="T47" s="21" t="s">
         <v>17</v>
       </c>
       <c r="U47" s="21"/>
-      <c r="V47" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="V47" s="21"/>
       <c r="W47" s="21"/>
-      <c r="X47" s="29"/>
-    </row>
-    <row r="48" spans="1:24" ht="15.75" customHeight="1">
+      <c r="X47" s="10"/>
+    </row>
+    <row r="48" spans="1:24" s="30" customFormat="1" ht="15.75" customHeight="1">
       <c r="A48" s="27" t="s">
         <v>43</v>
       </c>
       <c r="B48" s="27" t="s">
-        <v>57</v>
+        <v>133</v>
       </c>
       <c r="C48" s="21"/>
       <c r="D48" s="21" t="s">
@@ -3583,18 +3586,12 @@
       <c r="K48" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="L48" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="L48" s="21"/>
       <c r="M48" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="N48" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="O48" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="N48" s="21"/>
+      <c r="O48" s="21"/>
       <c r="P48" s="21" t="s">
         <v>17</v>
       </c>
@@ -3604,9 +3601,7 @@
       <c r="R48" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="S48" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="S48" s="21"/>
       <c r="T48" s="21" t="s">
         <v>17</v>
       </c>
@@ -3615,14 +3610,14 @@
         <v>17</v>
       </c>
       <c r="W48" s="21"/>
-      <c r="X48" s="10"/>
+      <c r="X48" s="29"/>
     </row>
     <row r="49" spans="1:24" ht="15.75" customHeight="1">
       <c r="A49" s="27" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B49" s="27" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C49" s="21"/>
       <c r="D49" s="21" t="s">
@@ -3676,23 +3671,19 @@
       <c r="T49" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="U49" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="U49" s="21"/>
       <c r="V49" s="21" t="s">
         <v>17</v>
       </c>
       <c r="W49" s="21"/>
-      <c r="X49" s="32" t="s">
-        <v>60</v>
-      </c>
+      <c r="X49" s="10"/>
     </row>
     <row r="50" spans="1:24" ht="15.75" customHeight="1">
       <c r="A50" s="27" t="s">
         <v>58</v>
       </c>
       <c r="B50" s="27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C50" s="21"/>
       <c r="D50" s="21" t="s">
@@ -3753,21 +3744,23 @@
         <v>17</v>
       </c>
       <c r="W50" s="21"/>
-      <c r="X50" s="33"/>
+      <c r="X50" s="34" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="51" spans="1:24" ht="15.75" customHeight="1">
       <c r="A51" s="27" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B51" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C51" s="21"/>
       <c r="D51" s="21" t="s">
-        <v>115</v>
+        <v>17</v>
       </c>
       <c r="E51" s="21" t="s">
-        <v>115</v>
+        <v>17</v>
       </c>
       <c r="F51" s="21" t="s">
         <v>17</v>
@@ -3782,10 +3775,10 @@
         <v>17</v>
       </c>
       <c r="J51" s="21" t="s">
-        <v>115</v>
+        <v>17</v>
       </c>
       <c r="K51" s="21" t="s">
-        <v>115</v>
+        <v>17</v>
       </c>
       <c r="L51" s="21" t="s">
         <v>17</v>
@@ -3800,129 +3793,166 @@
         <v>17</v>
       </c>
       <c r="P51" s="21" t="s">
-        <v>115</v>
+        <v>17</v>
       </c>
       <c r="Q51" s="21" t="s">
-        <v>115</v>
+        <v>17</v>
       </c>
       <c r="R51" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="S51" s="21"/>
+      <c r="S51" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="T51" s="21" t="s">
         <v>17</v>
       </c>
       <c r="U51" s="21" t="s">
-        <v>115</v>
+        <v>17</v>
       </c>
       <c r="V51" s="21" t="s">
         <v>17</v>
       </c>
       <c r="W51" s="21"/>
-      <c r="X51" s="10"/>
-    </row>
-    <row r="52" spans="1:24" s="15" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A52" s="18" t="s">
+      <c r="X51" s="35"/>
+    </row>
+    <row r="52" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A52" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B52" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="C52" s="21"/>
+      <c r="D52" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E52" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F52" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="G52" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H52" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="I52" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="J52" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="K52" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="L52" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="M52" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="N52" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="O52" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="P52" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q52" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="R52" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="S52" s="21"/>
+      <c r="T52" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="U52" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="V52" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="W52" s="21"/>
+      <c r="X52" s="10"/>
+    </row>
+    <row r="53" spans="1:24" s="15" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A53" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="B52" s="18" t="s">
+      <c r="B53" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="C52" s="19"/>
-      <c r="D52" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="E52" s="19"/>
-      <c r="F52" s="19"/>
-      <c r="G52" s="19"/>
-      <c r="H52" s="19"/>
-      <c r="I52" s="19"/>
-      <c r="J52" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="K52" s="19"/>
-      <c r="L52" s="19"/>
-      <c r="M52" s="19"/>
-      <c r="N52" s="19"/>
-      <c r="O52" s="19"/>
-      <c r="P52" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q52" s="19"/>
-      <c r="R52" s="19"/>
-      <c r="S52" s="19"/>
-      <c r="T52" s="19"/>
-      <c r="U52" s="19"/>
-      <c r="V52" s="19"/>
-      <c r="W52" s="19"/>
-      <c r="X52" s="14" t="s">
+      <c r="C53" s="19"/>
+      <c r="D53" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="E53" s="19"/>
+      <c r="F53" s="19"/>
+      <c r="G53" s="19"/>
+      <c r="H53" s="19"/>
+      <c r="I53" s="19"/>
+      <c r="J53" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="K53" s="19"/>
+      <c r="L53" s="19"/>
+      <c r="M53" s="19"/>
+      <c r="N53" s="19"/>
+      <c r="O53" s="19"/>
+      <c r="P53" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q53" s="19"/>
+      <c r="R53" s="19"/>
+      <c r="S53" s="19"/>
+      <c r="T53" s="19"/>
+      <c r="U53" s="19"/>
+      <c r="V53" s="19"/>
+      <c r="W53" s="19"/>
+      <c r="X53" s="14" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="53" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A53" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="B53" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="C53" s="17"/>
-      <c r="D53" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="E53" s="17"/>
-      <c r="F53" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="G53" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="H53" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="I53" s="17"/>
-      <c r="J53" s="17"/>
-      <c r="K53" s="17"/>
-      <c r="L53" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="M53" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="N53" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="O53" s="17"/>
-      <c r="P53" s="17"/>
-      <c r="Q53" s="17"/>
-      <c r="R53" s="17"/>
-      <c r="S53" s="17"/>
-      <c r="T53" s="17"/>
-      <c r="U53" s="17"/>
-      <c r="V53" s="17"/>
-      <c r="W53" s="17"/>
     </row>
     <row r="54" spans="1:24" ht="15.75" customHeight="1">
       <c r="A54" s="16" t="s">
         <v>63</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C54" s="17"/>
       <c r="D54" s="17" t="s">
         <v>115</v>
       </c>
       <c r="E54" s="17"/>
-      <c r="F54" s="17"/>
-      <c r="G54" s="17"/>
-      <c r="H54" s="17"/>
+      <c r="F54" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G54" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H54" s="17" t="s">
+        <v>19</v>
+      </c>
       <c r="I54" s="17"/>
       <c r="J54" s="17"/>
       <c r="K54" s="17"/>
-      <c r="L54" s="17"/>
-      <c r="M54" s="17"/>
-      <c r="N54" s="17"/>
+      <c r="L54" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="M54" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="N54" s="17" t="s">
+        <v>19</v>
+      </c>
       <c r="O54" s="17"/>
       <c r="P54" s="17"/>
       <c r="Q54" s="17"/>
@@ -3938,7 +3968,7 @@
         <v>63</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C55" s="17"/>
       <c r="D55" s="17" t="s">
@@ -3969,7 +3999,7 @@
         <v>63</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C56" s="17"/>
       <c r="D56" s="17" t="s">
@@ -3997,79 +4027,110 @@
     </row>
     <row r="57" spans="1:24" ht="15.75" customHeight="1">
       <c r="A57" s="16" t="s">
-        <v>111</v>
+        <v>63</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="C57" s="20"/>
-      <c r="D57" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="E57" s="20"/>
-      <c r="F57" s="20"/>
-      <c r="G57" s="20"/>
-      <c r="H57" s="20"/>
-      <c r="I57" s="20"/>
-      <c r="J57" s="20"/>
-      <c r="K57" s="20"/>
-      <c r="L57" s="20"/>
-      <c r="M57" s="20"/>
-      <c r="N57" s="20"/>
-      <c r="O57" s="20"/>
-      <c r="P57" s="20"/>
-      <c r="Q57" s="20"/>
-      <c r="R57" s="20"/>
-      <c r="S57" s="20"/>
-      <c r="T57" s="20"/>
-      <c r="U57" s="20"/>
-      <c r="V57" s="20"/>
-      <c r="W57" s="20"/>
+        <v>69</v>
+      </c>
+      <c r="C57" s="17"/>
+      <c r="D57" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="E57" s="17"/>
+      <c r="F57" s="17"/>
+      <c r="G57" s="17"/>
+      <c r="H57" s="17"/>
+      <c r="I57" s="17"/>
+      <c r="J57" s="17"/>
+      <c r="K57" s="17"/>
+      <c r="L57" s="17"/>
+      <c r="M57" s="17"/>
+      <c r="N57" s="17"/>
+      <c r="O57" s="17"/>
+      <c r="P57" s="17"/>
+      <c r="Q57" s="17"/>
+      <c r="R57" s="17"/>
+      <c r="S57" s="17"/>
+      <c r="T57" s="17"/>
+      <c r="U57" s="17"/>
+      <c r="V57" s="17"/>
+      <c r="W57" s="17"/>
     </row>
     <row r="58" spans="1:24" ht="15.75" customHeight="1">
       <c r="A58" s="16" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="B58" s="16" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="C58" s="20"/>
       <c r="D58" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E58" s="20"/>
+      <c r="F58" s="20"/>
+      <c r="G58" s="20"/>
+      <c r="H58" s="20"/>
+      <c r="I58" s="20"/>
+      <c r="J58" s="20"/>
+      <c r="K58" s="20"/>
+      <c r="L58" s="20"/>
+      <c r="M58" s="20"/>
+      <c r="N58" s="20"/>
+      <c r="O58" s="20"/>
+      <c r="P58" s="20"/>
+      <c r="Q58" s="20"/>
+      <c r="R58" s="20"/>
+      <c r="S58" s="20"/>
+      <c r="T58" s="20"/>
+      <c r="U58" s="20"/>
+      <c r="V58" s="20"/>
+      <c r="W58" s="20"/>
+    </row>
+    <row r="59" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A59" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="B59" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="C59" s="20"/>
+      <c r="D59" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="E58" s="31" t="s">
+      <c r="E59" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="F58" s="31"/>
-      <c r="G58" s="31" t="s">
+      <c r="F59" s="31"/>
+      <c r="G59" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="H58" s="31"/>
-      <c r="I58" s="31"/>
-      <c r="J58" s="31" t="s">
+      <c r="H59" s="31"/>
+      <c r="I59" s="31"/>
+      <c r="J59" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="K58" s="31" t="s">
+      <c r="K59" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="L58" s="31" t="s">
+      <c r="L59" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="M58" s="31"/>
-      <c r="N58" s="31"/>
-      <c r="O58" s="31"/>
-      <c r="P58" s="31"/>
-      <c r="Q58" s="31"/>
-      <c r="R58" s="31"/>
-      <c r="S58" s="31"/>
-      <c r="T58" s="31"/>
-      <c r="U58" s="31"/>
-      <c r="V58" s="31"/>
-      <c r="W58" s="31"/>
+      <c r="M59" s="31"/>
+      <c r="N59" s="31"/>
+      <c r="O59" s="31"/>
+      <c r="P59" s="31"/>
+      <c r="Q59" s="31"/>
+      <c r="R59" s="31"/>
+      <c r="S59" s="31"/>
+      <c r="T59" s="31"/>
+      <c r="U59" s="31"/>
+      <c r="V59" s="31"/>
+      <c r="W59" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="X49:X50"/>
+    <mergeCell ref="X50:X51"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="J5:N5"/>
     <mergeCell ref="P5:V5"/>
@@ -4090,7 +4151,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Lisää alustava UI kohdeluettelon päivitykselle & uusi oikeus sitoa paikkausurakka
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1008,7 +1008,7 @@
       <pane xSplit="2" ySplit="6" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E29" sqref="E29"/>
+      <selection pane="bottomRight" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2583,10 +2583,10 @@
       </c>
       <c r="C31" s="21"/>
       <c r="D31" s="21" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="F31" s="21" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
LIsää oma oikeustarkistus paikkauskohteiden sidonnalle
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1008,7 +1008,7 @@
       <pane xSplit="2" ySplit="6" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E29" sqref="E29"/>
+      <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2583,10 +2583,10 @@
       </c>
       <c r="C31" s="21"/>
       <c r="D31" s="21" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="F31" s="21" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
orjKorjaa testit vastaamaan uutta tietomallia
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8000" yWindow="1160" windowWidth="35320" windowHeight="22340" tabRatio="500"/>
+    <workbookView xWindow="8880" yWindow="2160" windowWidth="35320" windowHeight="22340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -435,7 +435,7 @@
     <t>Laskutusyhteenveto</t>
   </si>
   <si>
-    <t>R,W,sidonta</t>
+    <t>R,W,sido</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Lisää API-järjestelmätunnukset osio oikeuksiin
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26812"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarihan/Desktop/Harja/harja/resources/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="8000" yWindow="1160" windowWidth="35320" windowHeight="22340" tabRatio="500"/>
   </bookViews>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="138">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -436,6 +431,9 @@
   </si>
   <si>
     <t>R,W,sidonta</t>
+  </si>
+  <si>
+    <t>API-järjestelmätunnukset</t>
   </si>
 </sst>
 </file>
@@ -581,7 +579,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -639,6 +637,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1002,16 +1001,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X59"/>
+  <dimension ref="A1:X60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
+      <selection pane="bottomRight" activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.5" bestFit="1" customWidth="1"/>
@@ -1038,45 +1037,45 @@
     <col min="24" max="24" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:24" ht="15.75" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-    </row>
-    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+    </row>
+    <row r="2" spans="1:24" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-    </row>
-    <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+    </row>
+    <row r="3" spans="1:24" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -1091,39 +1090,39 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:24" ht="15.75" customHeight="1">
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C5" s="36" t="s">
+    <row r="5" spans="1:24" ht="15.75" customHeight="1">
+      <c r="C5" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="J5" s="36" t="s">
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="J5" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
-      <c r="M5" s="35"/>
-      <c r="N5" s="35"/>
-      <c r="P5" s="36" t="s">
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="36"/>
+      <c r="N5" s="36"/>
+      <c r="P5" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="Q5" s="35"/>
-      <c r="R5" s="35"/>
-      <c r="S5" s="35"/>
-      <c r="T5" s="35"/>
-      <c r="U5" s="35"/>
-      <c r="V5" s="35"/>
+      <c r="Q5" s="36"/>
+      <c r="R5" s="36"/>
+      <c r="S5" s="36"/>
+      <c r="T5" s="36"/>
+      <c r="U5" s="36"/>
+      <c r="V5" s="36"/>
       <c r="X5" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:24" ht="15.75" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -1192,7 +1191,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:24" ht="15.75" customHeight="1">
       <c r="A7" s="16" t="s">
         <v>15</v>
       </c>
@@ -1260,7 +1259,7 @@
       <c r="W7" s="17"/>
       <c r="X7" s="10"/>
     </row>
-    <row r="8" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:24" ht="15.75" customHeight="1">
       <c r="A8" s="16" t="s">
         <v>15</v>
       </c>
@@ -1314,7 +1313,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:24" ht="15.75" customHeight="1">
       <c r="A9" s="16" t="s">
         <v>15</v>
       </c>
@@ -1362,7 +1361,7 @@
       <c r="W9" s="17"/>
       <c r="X9" s="10"/>
     </row>
-    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:24" ht="15.75" customHeight="1">
       <c r="A10" s="16" t="s">
         <v>15</v>
       </c>
@@ -1410,7 +1409,7 @@
       <c r="W10" s="17"/>
       <c r="X10" s="10"/>
     </row>
-    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:24" ht="15.75" customHeight="1">
       <c r="A11" s="16" t="s">
         <v>15</v>
       </c>
@@ -1472,7 +1471,7 @@
       <c r="W11" s="17"/>
       <c r="X11" s="10"/>
     </row>
-    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:24" ht="15.75" customHeight="1">
       <c r="A12" s="16" t="s">
         <v>15</v>
       </c>
@@ -1534,7 +1533,7 @@
       <c r="W12" s="17"/>
       <c r="X12" s="10"/>
     </row>
-    <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:24" ht="15.75" customHeight="1">
       <c r="A13" s="16" t="s">
         <v>15</v>
       </c>
@@ -1584,7 +1583,7 @@
       <c r="W13" s="17"/>
       <c r="X13" s="10"/>
     </row>
-    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:24" ht="15.75" customHeight="1">
       <c r="A14" s="16" t="s">
         <v>15</v>
       </c>
@@ -1634,7 +1633,7 @@
       <c r="W14" s="17"/>
       <c r="X14" s="10"/>
     </row>
-    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:24" ht="15.75" customHeight="1">
       <c r="A15" s="16" t="s">
         <v>15</v>
       </c>
@@ -1684,7 +1683,7 @@
       <c r="W15" s="17"/>
       <c r="X15" s="10"/>
     </row>
-    <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:24" ht="15.75" customHeight="1">
       <c r="A16" s="16" t="s">
         <v>15</v>
       </c>
@@ -1746,7 +1745,7 @@
       <c r="W16" s="17"/>
       <c r="X16" s="10"/>
     </row>
-    <row r="17" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:24" ht="15.75" customHeight="1">
       <c r="A17" s="16" t="s">
         <v>15</v>
       </c>
@@ -1808,7 +1807,7 @@
       <c r="W17" s="17"/>
       <c r="X17" s="10"/>
     </row>
-    <row r="18" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:24" ht="15.75" customHeight="1">
       <c r="A18" s="16" t="s">
         <v>15</v>
       </c>
@@ -1858,7 +1857,7 @@
       <c r="W18" s="17"/>
       <c r="X18" s="10"/>
     </row>
-    <row r="19" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:24" ht="15.75" customHeight="1">
       <c r="A19" s="16" t="s">
         <v>15</v>
       </c>
@@ -1920,7 +1919,7 @@
       <c r="W19" s="17"/>
       <c r="X19" s="10"/>
     </row>
-    <row r="20" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:24" ht="15.75" customHeight="1">
       <c r="A20" s="16" t="s">
         <v>15</v>
       </c>
@@ -1986,7 +1985,7 @@
       <c r="W20" s="17"/>
       <c r="X20" s="10"/>
     </row>
-    <row r="21" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:24" ht="15.75" customHeight="1">
       <c r="A21" s="27" t="s">
         <v>15</v>
       </c>
@@ -2054,7 +2053,7 @@
       <c r="W21" s="21"/>
       <c r="X21" s="10"/>
     </row>
-    <row r="22" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:24" ht="15.75" customHeight="1">
       <c r="A22" s="27" t="s">
         <v>15</v>
       </c>
@@ -2120,7 +2119,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="23" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:24" ht="15.75" customHeight="1">
       <c r="A23" s="27" t="s">
         <v>15</v>
       </c>
@@ -2186,7 +2185,7 @@
       <c r="W23" s="21"/>
       <c r="X23" s="10"/>
     </row>
-    <row r="24" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:24" ht="15.75" customHeight="1">
       <c r="A24" s="27" t="s">
         <v>15</v>
       </c>
@@ -2248,7 +2247,7 @@
       <c r="W24" s="21"/>
       <c r="X24" s="10"/>
     </row>
-    <row r="25" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:24" ht="15.75" customHeight="1">
       <c r="A25" s="27" t="s">
         <v>15</v>
       </c>
@@ -2298,7 +2297,7 @@
       <c r="W25" s="21"/>
       <c r="X25" s="10"/>
     </row>
-    <row r="26" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:24" ht="15.75" customHeight="1">
       <c r="A26" s="27" t="s">
         <v>15</v>
       </c>
@@ -2344,7 +2343,7 @@
       <c r="W26" s="21"/>
       <c r="X26" s="10"/>
     </row>
-    <row r="27" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:24" ht="15.75" customHeight="1">
       <c r="A27" s="27" t="s">
         <v>15</v>
       </c>
@@ -2384,7 +2383,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:24" ht="15.75" customHeight="1">
       <c r="A28" s="27" t="s">
         <v>15</v>
       </c>
@@ -2450,7 +2449,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="29" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:24" ht="15.75" customHeight="1">
       <c r="A29" s="27" t="s">
         <v>15</v>
       </c>
@@ -2512,7 +2511,7 @@
       <c r="W29" s="21"/>
       <c r="X29" s="10"/>
     </row>
-    <row r="30" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:24" ht="15.75" customHeight="1">
       <c r="A30" s="27" t="s">
         <v>15</v>
       </c>
@@ -2574,7 +2573,7 @@
       <c r="W30" s="21"/>
       <c r="X30" s="10"/>
     </row>
-    <row r="31" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:24" ht="15.75" customHeight="1">
       <c r="A31" s="27" t="s">
         <v>15</v>
       </c>
@@ -2636,7 +2635,7 @@
       <c r="W31" s="21"/>
       <c r="X31" s="10"/>
     </row>
-    <row r="32" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:24" ht="15.75" customHeight="1">
       <c r="A32" s="27" t="s">
         <v>15</v>
       </c>
@@ -2698,7 +2697,7 @@
       <c r="W32" s="21"/>
       <c r="X32" s="10"/>
     </row>
-    <row r="33" spans="1:24" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:24" s="13" customFormat="1" ht="15.75" customHeight="1">
       <c r="A33" s="27" t="s">
         <v>15</v>
       </c>
@@ -2766,7 +2765,7 @@
       <c r="W33" s="21"/>
       <c r="X33" s="12"/>
     </row>
-    <row r="34" spans="1:24" s="33" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:24" s="33" customFormat="1" ht="15.75" customHeight="1">
       <c r="A34" s="27" t="s">
         <v>43</v>
       </c>
@@ -2812,7 +2811,7 @@
       <c r="W34" s="21"/>
       <c r="X34" s="32"/>
     </row>
-    <row r="35" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:24" ht="15.75" customHeight="1">
       <c r="A35" s="27" t="s">
         <v>43</v>
       </c>
@@ -2862,7 +2861,7 @@
       <c r="W35" s="21"/>
       <c r="X35" s="10"/>
     </row>
-    <row r="36" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:24" ht="15.75" customHeight="1">
       <c r="A36" s="27" t="s">
         <v>43</v>
       </c>
@@ -2928,7 +2927,7 @@
       <c r="W36" s="21"/>
       <c r="X36" s="10"/>
     </row>
-    <row r="37" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:24" ht="15.75" customHeight="1">
       <c r="A37" s="27" t="s">
         <v>43</v>
       </c>
@@ -2994,7 +2993,7 @@
       <c r="W37" s="21"/>
       <c r="X37" s="10"/>
     </row>
-    <row r="38" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:24" ht="15.75" customHeight="1">
       <c r="A38" s="27" t="s">
         <v>43</v>
       </c>
@@ -3060,7 +3059,7 @@
       <c r="W38" s="21"/>
       <c r="X38" s="10"/>
     </row>
-    <row r="39" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:24" ht="15.75" customHeight="1">
       <c r="A39" s="27" t="s">
         <v>43</v>
       </c>
@@ -3126,7 +3125,7 @@
       <c r="W39" s="21"/>
       <c r="X39" s="10"/>
     </row>
-    <row r="40" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:24" ht="15.75" customHeight="1">
       <c r="A40" s="27" t="s">
         <v>43</v>
       </c>
@@ -3192,7 +3191,7 @@
       <c r="W40" s="21"/>
       <c r="X40" s="10"/>
     </row>
-    <row r="41" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:24" ht="15.75" customHeight="1">
       <c r="A41" s="27" t="s">
         <v>43</v>
       </c>
@@ -3250,7 +3249,7 @@
       <c r="W41" s="21"/>
       <c r="X41" s="10"/>
     </row>
-    <row r="42" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:24" ht="15.75" customHeight="1">
       <c r="A42" s="27" t="s">
         <v>43</v>
       </c>
@@ -3316,7 +3315,7 @@
       <c r="W42" s="21"/>
       <c r="X42" s="10"/>
     </row>
-    <row r="43" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:24" ht="15.75" customHeight="1">
       <c r="A43" s="27" t="s">
         <v>43</v>
       </c>
@@ -3368,7 +3367,7 @@
       <c r="W43" s="21"/>
       <c r="X43" s="10"/>
     </row>
-    <row r="44" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:24" ht="15.75" customHeight="1">
       <c r="A44" s="27" t="s">
         <v>43</v>
       </c>
@@ -3418,7 +3417,7 @@
       <c r="W44" s="21"/>
       <c r="X44" s="10"/>
     </row>
-    <row r="45" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:24" ht="15.75" customHeight="1">
       <c r="A45" s="27" t="s">
         <v>43</v>
       </c>
@@ -3466,7 +3465,7 @@
       <c r="W45" s="21"/>
       <c r="X45" s="10"/>
     </row>
-    <row r="46" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:24" ht="15.75" customHeight="1">
       <c r="A46" s="27" t="s">
         <v>43</v>
       </c>
@@ -3514,7 +3513,7 @@
       <c r="W46" s="21"/>
       <c r="X46" s="10"/>
     </row>
-    <row r="47" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:24" ht="15.75" customHeight="1">
       <c r="A47" s="27" t="s">
         <v>43</v>
       </c>
@@ -3562,7 +3561,7 @@
       <c r="W47" s="21"/>
       <c r="X47" s="10"/>
     </row>
-    <row r="48" spans="1:24" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:24" s="30" customFormat="1" ht="15.75" customHeight="1">
       <c r="A48" s="27" t="s">
         <v>43</v>
       </c>
@@ -3620,7 +3619,7 @@
       <c r="W48" s="21"/>
       <c r="X48" s="29"/>
     </row>
-    <row r="49" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:24" ht="15.75" customHeight="1">
       <c r="A49" s="27" t="s">
         <v>43</v>
       </c>
@@ -3686,7 +3685,7 @@
       <c r="W49" s="21"/>
       <c r="X49" s="10"/>
     </row>
-    <row r="50" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:24" ht="15.75" customHeight="1">
       <c r="A50" s="27" t="s">
         <v>58</v>
       </c>
@@ -3752,11 +3751,11 @@
         <v>17</v>
       </c>
       <c r="W50" s="21"/>
-      <c r="X50" s="34" t="s">
+      <c r="X50" s="35" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:24" ht="15.75" customHeight="1">
       <c r="A51" s="27" t="s">
         <v>58</v>
       </c>
@@ -3822,9 +3821,9 @@
         <v>17</v>
       </c>
       <c r="W51" s="21"/>
-      <c r="X51" s="35"/>
-    </row>
-    <row r="52" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="X51" s="36"/>
+    </row>
+    <row r="52" spans="1:24" ht="15.75" customHeight="1">
       <c r="A52" s="27" t="s">
         <v>62</v>
       </c>
@@ -3890,7 +3889,7 @@
       <c r="W52" s="21"/>
       <c r="X52" s="10"/>
     </row>
-    <row r="53" spans="1:24" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:24" s="15" customFormat="1" ht="15.75" customHeight="1">
       <c r="A53" s="18" t="s">
         <v>63</v>
       </c>
@@ -3928,7 +3927,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="54" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:24" ht="15.75" customHeight="1">
       <c r="A54" s="16" t="s">
         <v>63</v>
       </c>
@@ -3971,7 +3970,7 @@
       <c r="V54" s="17"/>
       <c r="W54" s="17"/>
     </row>
-    <row r="55" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:24" ht="15.75" customHeight="1">
       <c r="A55" s="16" t="s">
         <v>63</v>
       </c>
@@ -4002,7 +4001,7 @@
       <c r="V55" s="17"/>
       <c r="W55" s="17"/>
     </row>
-    <row r="56" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:24" ht="15.75" customHeight="1">
       <c r="A56" s="16" t="s">
         <v>63</v>
       </c>
@@ -4033,7 +4032,7 @@
       <c r="V56" s="17"/>
       <c r="W56" s="17"/>
     </row>
-    <row r="57" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:24" ht="15.75" customHeight="1">
       <c r="A57" s="16" t="s">
         <v>63</v>
       </c>
@@ -4064,77 +4063,108 @@
       <c r="V57" s="17"/>
       <c r="W57" s="17"/>
     </row>
-    <row r="58" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:24" s="34" customFormat="1" ht="15.75" customHeight="1">
       <c r="A58" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B58" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="C58" s="17"/>
+      <c r="D58" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="E58" s="17"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="17"/>
+      <c r="H58" s="17"/>
+      <c r="I58" s="17"/>
+      <c r="J58" s="17"/>
+      <c r="K58" s="17"/>
+      <c r="L58" s="17"/>
+      <c r="M58" s="17"/>
+      <c r="N58" s="17"/>
+      <c r="O58" s="17"/>
+      <c r="P58" s="17"/>
+      <c r="Q58" s="17"/>
+      <c r="R58" s="17"/>
+      <c r="S58" s="17"/>
+      <c r="T58" s="17"/>
+      <c r="U58" s="17"/>
+      <c r="V58" s="17"/>
+      <c r="W58" s="17"/>
+    </row>
+    <row r="59" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A59" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="B58" s="16" t="s">
+      <c r="B59" s="16" t="s">
         <v>112</v>
-      </c>
-      <c r="C58" s="20"/>
-      <c r="D58" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="E58" s="20"/>
-      <c r="F58" s="20"/>
-      <c r="G58" s="20"/>
-      <c r="H58" s="20"/>
-      <c r="I58" s="20"/>
-      <c r="J58" s="20"/>
-      <c r="K58" s="20"/>
-      <c r="L58" s="20"/>
-      <c r="M58" s="20"/>
-      <c r="N58" s="20"/>
-      <c r="O58" s="20"/>
-      <c r="P58" s="20"/>
-      <c r="Q58" s="20"/>
-      <c r="R58" s="20"/>
-      <c r="S58" s="20"/>
-      <c r="T58" s="20"/>
-      <c r="U58" s="20"/>
-      <c r="V58" s="20"/>
-      <c r="W58" s="20"/>
-    </row>
-    <row r="59" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="B59" s="16" t="s">
-        <v>131</v>
       </c>
       <c r="C59" s="20"/>
       <c r="D59" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E59" s="20"/>
+      <c r="F59" s="20"/>
+      <c r="G59" s="20"/>
+      <c r="H59" s="20"/>
+      <c r="I59" s="20"/>
+      <c r="J59" s="20"/>
+      <c r="K59" s="20"/>
+      <c r="L59" s="20"/>
+      <c r="M59" s="20"/>
+      <c r="N59" s="20"/>
+      <c r="O59" s="20"/>
+      <c r="P59" s="20"/>
+      <c r="Q59" s="20"/>
+      <c r="R59" s="20"/>
+      <c r="S59" s="20"/>
+      <c r="T59" s="20"/>
+      <c r="U59" s="20"/>
+      <c r="V59" s="20"/>
+      <c r="W59" s="20"/>
+    </row>
+    <row r="60" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A60" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="B60" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="C60" s="20"/>
+      <c r="D60" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="E59" s="31" t="s">
+      <c r="E60" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="F59" s="31"/>
-      <c r="G59" s="31" t="s">
+      <c r="F60" s="31"/>
+      <c r="G60" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="H59" s="31"/>
-      <c r="I59" s="31"/>
-      <c r="J59" s="31" t="s">
+      <c r="H60" s="31"/>
+      <c r="I60" s="31"/>
+      <c r="J60" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="K59" s="31" t="s">
+      <c r="K60" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="L59" s="31" t="s">
+      <c r="L60" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="M59" s="31"/>
-      <c r="N59" s="31"/>
-      <c r="O59" s="31"/>
-      <c r="P59" s="31"/>
-      <c r="Q59" s="31"/>
-      <c r="R59" s="31"/>
-      <c r="S59" s="31"/>
-      <c r="T59" s="31"/>
-      <c r="U59" s="31"/>
-      <c r="V59" s="31"/>
-      <c r="W59" s="31"/>
+      <c r="M60" s="31"/>
+      <c r="N60" s="31"/>
+      <c r="O60" s="31"/>
+      <c r="P60" s="31"/>
+      <c r="Q60" s="31"/>
+      <c r="R60" s="31"/>
+      <c r="S60" s="31"/>
+      <c r="T60" s="31"/>
+      <c r="U60" s="31"/>
+      <c r="V60" s="31"/>
+      <c r="W60" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -4147,6 +4177,11 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4158,7 +4193,7 @@
       <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="29.6640625" customWidth="1"/>
     <col min="2" max="2" width="28.1640625" customWidth="1"/>
@@ -4166,7 +4201,7 @@
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="15">
       <c r="A1" s="22" t="s">
         <v>70</v>
       </c>
@@ -4183,7 +4218,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15">
       <c r="A2" s="23" t="s">
         <v>73</v>
       </c>
@@ -4196,7 +4231,7 @@
       <c r="D2" s="24"/>
       <c r="E2" s="24"/>
     </row>
-    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15">
       <c r="A3" s="23" t="s">
         <v>75</v>
       </c>
@@ -4209,7 +4244,7 @@
       <c r="D3" s="24"/>
       <c r="E3" s="24"/>
     </row>
-    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="15">
       <c r="A4" s="23" t="s">
         <v>77</v>
       </c>
@@ -4222,7 +4257,7 @@
       <c r="D4" s="24"/>
       <c r="E4" s="24"/>
     </row>
-    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="15">
       <c r="A5" s="23" t="s">
         <v>97</v>
       </c>
@@ -4237,7 +4272,7 @@
       </c>
       <c r="E5" s="24"/>
     </row>
-    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="15">
       <c r="A6" s="23" t="s">
         <v>98</v>
       </c>
@@ -4252,7 +4287,7 @@
       </c>
       <c r="E6" s="24"/>
     </row>
-    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="15">
       <c r="A7" s="23" t="s">
         <v>99</v>
       </c>
@@ -4267,7 +4302,7 @@
       </c>
       <c r="E7" s="24"/>
     </row>
-    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="15">
       <c r="A8" s="23" t="s">
         <v>100</v>
       </c>
@@ -4282,7 +4317,7 @@
       </c>
       <c r="E8" s="24"/>
     </row>
-    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="15">
       <c r="A9" s="23" t="s">
         <v>109</v>
       </c>
@@ -4297,7 +4332,7 @@
       </c>
       <c r="E9" s="24"/>
     </row>
-    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="15">
       <c r="A10" s="23" t="s">
         <v>108</v>
       </c>
@@ -4312,7 +4347,7 @@
       </c>
       <c r="E10" s="24"/>
     </row>
-    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="15">
       <c r="A11" s="23" t="s">
         <v>107</v>
       </c>
@@ -4327,7 +4362,7 @@
       </c>
       <c r="E11" s="24"/>
     </row>
-    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="15">
       <c r="A12" s="23" t="s">
         <v>101</v>
       </c>
@@ -4342,7 +4377,7 @@
       </c>
       <c r="E12" s="24"/>
     </row>
-    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="15">
       <c r="A13" s="23" t="s">
         <v>106</v>
       </c>
@@ -4357,7 +4392,7 @@
       </c>
       <c r="E13" s="24"/>
     </row>
-    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="15">
       <c r="A14" s="23" t="s">
         <v>102</v>
       </c>
@@ -4372,7 +4407,7 @@
       </c>
       <c r="E14" s="24"/>
     </row>
-    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="15">
       <c r="A15" s="23" t="s">
         <v>103</v>
       </c>
@@ -4387,7 +4422,7 @@
       </c>
       <c r="E15" s="24"/>
     </row>
-    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="15">
       <c r="A16" s="23" t="s">
         <v>104</v>
       </c>
@@ -4402,7 +4437,7 @@
       </c>
       <c r="E16" s="24"/>
     </row>
-    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="15">
       <c r="A17" s="23" t="s">
         <v>134</v>
       </c>
@@ -4417,7 +4452,7 @@
       </c>
       <c r="E17" s="24"/>
     </row>
-    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="15">
       <c r="A18" s="23" t="s">
         <v>12</v>
       </c>
@@ -4432,7 +4467,7 @@
       </c>
       <c r="E18" s="24"/>
     </row>
-    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="15">
       <c r="A19" s="23" t="s">
         <v>13</v>
       </c>
@@ -4447,7 +4482,7 @@
       </c>
       <c r="E19" s="24"/>
     </row>
-    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="15">
       <c r="A20" s="23" t="s">
         <v>105</v>
       </c>
@@ -4462,7 +4497,7 @@
       </c>
       <c r="E20" s="24"/>
     </row>
-    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="15">
       <c r="A21" s="23" t="s">
         <v>118</v>
       </c>
@@ -4481,5 +4516,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Lisää toimenpiteiden ajoittuminen oikeuksiin
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8000" yWindow="1160" windowWidth="35320" windowHeight="22340" tabRatio="500"/>
+    <workbookView xWindow="3860" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="139">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -434,6 +434,9 @@
   </si>
   <si>
     <t>API-järjestelmätunnukset</t>
+  </si>
+  <si>
+    <t>Toimenpiteiden ajoittuminen</t>
   </si>
 </sst>
 </file>
@@ -579,7 +582,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -638,6 +641,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1001,13 +1008,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X60"/>
+  <dimension ref="A1:X61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C37" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D62" sqref="D62"/>
+      <selection pane="bottomRight" activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1042,38 +1049,38 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
     </row>
     <row r="2" spans="1:24" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
     </row>
     <row r="3" spans="1:24" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
@@ -1094,30 +1101,30 @@
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:24" ht="15.75" customHeight="1">
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="J5" s="37" t="s">
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="J5" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36"/>
-      <c r="N5" s="36"/>
-      <c r="P5" s="37" t="s">
+      <c r="K5" s="38"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="38"/>
+      <c r="N5" s="38"/>
+      <c r="P5" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="Q5" s="36"/>
-      <c r="R5" s="36"/>
-      <c r="S5" s="36"/>
-      <c r="T5" s="36"/>
-      <c r="U5" s="36"/>
-      <c r="V5" s="36"/>
+      <c r="Q5" s="38"/>
+      <c r="R5" s="38"/>
+      <c r="S5" s="38"/>
+      <c r="T5" s="38"/>
+      <c r="U5" s="38"/>
+      <c r="V5" s="38"/>
       <c r="X5" s="5" t="s">
         <v>14</v>
       </c>
@@ -3685,12 +3692,12 @@
       <c r="W49" s="21"/>
       <c r="X49" s="10"/>
     </row>
-    <row r="50" spans="1:24" ht="15.75" customHeight="1">
+    <row r="50" spans="1:24" s="36" customFormat="1" ht="15.75" customHeight="1">
       <c r="A50" s="27" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B50" s="27" t="s">
-        <v>59</v>
+        <v>138</v>
       </c>
       <c r="C50" s="21"/>
       <c r="D50" s="21" t="s">
@@ -3729,38 +3736,22 @@
       <c r="O50" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="P50" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q50" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="R50" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="S50" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="T50" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="U50" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="V50" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="P50" s="21"/>
+      <c r="Q50" s="21"/>
+      <c r="R50" s="21"/>
+      <c r="S50" s="21"/>
+      <c r="T50" s="21"/>
+      <c r="U50" s="21"/>
+      <c r="V50" s="21"/>
       <c r="W50" s="21"/>
-      <c r="X50" s="35" t="s">
-        <v>60</v>
-      </c>
+      <c r="X50" s="35"/>
     </row>
     <row r="51" spans="1:24" ht="15.75" customHeight="1">
       <c r="A51" s="27" t="s">
         <v>58</v>
       </c>
       <c r="B51" s="27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C51" s="21"/>
       <c r="D51" s="21" t="s">
@@ -3821,21 +3812,23 @@
         <v>17</v>
       </c>
       <c r="W51" s="21"/>
-      <c r="X51" s="36"/>
+      <c r="X51" s="37" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="52" spans="1:24" ht="15.75" customHeight="1">
       <c r="A52" s="27" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B52" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C52" s="21"/>
       <c r="D52" s="21" t="s">
-        <v>115</v>
+        <v>17</v>
       </c>
       <c r="E52" s="21" t="s">
-        <v>115</v>
+        <v>17</v>
       </c>
       <c r="F52" s="21" t="s">
         <v>17</v>
@@ -3850,10 +3843,10 @@
         <v>17</v>
       </c>
       <c r="J52" s="21" t="s">
-        <v>115</v>
+        <v>17</v>
       </c>
       <c r="K52" s="21" t="s">
-        <v>115</v>
+        <v>17</v>
       </c>
       <c r="L52" s="21" t="s">
         <v>17</v>
@@ -3868,129 +3861,166 @@
         <v>17</v>
       </c>
       <c r="P52" s="21" t="s">
-        <v>115</v>
+        <v>17</v>
       </c>
       <c r="Q52" s="21" t="s">
-        <v>115</v>
+        <v>17</v>
       </c>
       <c r="R52" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="S52" s="21"/>
+      <c r="S52" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="T52" s="21" t="s">
         <v>17</v>
       </c>
       <c r="U52" s="21" t="s">
-        <v>115</v>
+        <v>17</v>
       </c>
       <c r="V52" s="21" t="s">
         <v>17</v>
       </c>
       <c r="W52" s="21"/>
-      <c r="X52" s="10"/>
-    </row>
-    <row r="53" spans="1:24" s="15" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A53" s="18" t="s">
+      <c r="X52" s="38"/>
+    </row>
+    <row r="53" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A53" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B53" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="C53" s="21"/>
+      <c r="D53" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E53" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F53" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="G53" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H53" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="I53" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="J53" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="K53" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="L53" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="M53" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="N53" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="O53" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="P53" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q53" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="R53" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="S53" s="21"/>
+      <c r="T53" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="U53" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="V53" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="W53" s="21"/>
+      <c r="X53" s="10"/>
+    </row>
+    <row r="54" spans="1:24" s="15" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A54" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="B53" s="18" t="s">
+      <c r="B54" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="C53" s="19"/>
-      <c r="D53" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="E53" s="19"/>
-      <c r="F53" s="19"/>
-      <c r="G53" s="19"/>
-      <c r="H53" s="19"/>
-      <c r="I53" s="19"/>
-      <c r="J53" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="K53" s="19"/>
-      <c r="L53" s="19"/>
-      <c r="M53" s="19"/>
-      <c r="N53" s="19"/>
-      <c r="O53" s="19"/>
-      <c r="P53" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q53" s="19"/>
-      <c r="R53" s="19"/>
-      <c r="S53" s="19"/>
-      <c r="T53" s="19"/>
-      <c r="U53" s="19"/>
-      <c r="V53" s="19"/>
-      <c r="W53" s="19"/>
-      <c r="X53" s="14" t="s">
+      <c r="C54" s="19"/>
+      <c r="D54" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="E54" s="19"/>
+      <c r="F54" s="19"/>
+      <c r="G54" s="19"/>
+      <c r="H54" s="19"/>
+      <c r="I54" s="19"/>
+      <c r="J54" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="K54" s="19"/>
+      <c r="L54" s="19"/>
+      <c r="M54" s="19"/>
+      <c r="N54" s="19"/>
+      <c r="O54" s="19"/>
+      <c r="P54" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q54" s="19"/>
+      <c r="R54" s="19"/>
+      <c r="S54" s="19"/>
+      <c r="T54" s="19"/>
+      <c r="U54" s="19"/>
+      <c r="V54" s="19"/>
+      <c r="W54" s="19"/>
+      <c r="X54" s="14" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="54" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A54" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="B54" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="C54" s="17"/>
-      <c r="D54" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="E54" s="17"/>
-      <c r="F54" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="G54" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="H54" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="I54" s="17"/>
-      <c r="J54" s="17"/>
-      <c r="K54" s="17"/>
-      <c r="L54" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="M54" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="N54" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="O54" s="17"/>
-      <c r="P54" s="17"/>
-      <c r="Q54" s="17"/>
-      <c r="R54" s="17"/>
-      <c r="S54" s="17"/>
-      <c r="T54" s="17"/>
-      <c r="U54" s="17"/>
-      <c r="V54" s="17"/>
-      <c r="W54" s="17"/>
     </row>
     <row r="55" spans="1:24" ht="15.75" customHeight="1">
       <c r="A55" s="16" t="s">
         <v>63</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C55" s="17"/>
       <c r="D55" s="17" t="s">
         <v>115</v>
       </c>
       <c r="E55" s="17"/>
-      <c r="F55" s="17"/>
-      <c r="G55" s="17"/>
-      <c r="H55" s="17"/>
+      <c r="F55" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G55" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H55" s="17" t="s">
+        <v>19</v>
+      </c>
       <c r="I55" s="17"/>
       <c r="J55" s="17"/>
       <c r="K55" s="17"/>
-      <c r="L55" s="17"/>
-      <c r="M55" s="17"/>
-      <c r="N55" s="17"/>
+      <c r="L55" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="M55" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="N55" s="17" t="s">
+        <v>19</v>
+      </c>
       <c r="O55" s="17"/>
       <c r="P55" s="17"/>
       <c r="Q55" s="17"/>
@@ -4006,7 +4036,7 @@
         <v>63</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C56" s="17"/>
       <c r="D56" s="17" t="s">
@@ -4037,7 +4067,7 @@
         <v>63</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C57" s="17"/>
       <c r="D57" s="17" t="s">
@@ -4063,12 +4093,12 @@
       <c r="V57" s="17"/>
       <c r="W57" s="17"/>
     </row>
-    <row r="58" spans="1:24" s="34" customFormat="1" ht="15.75" customHeight="1">
+    <row r="58" spans="1:24" ht="15.75" customHeight="1">
       <c r="A58" s="16" t="s">
         <v>63</v>
       </c>
       <c r="B58" s="16" t="s">
-        <v>137</v>
+        <v>69</v>
       </c>
       <c r="C58" s="17"/>
       <c r="D58" s="17" t="s">
@@ -4094,81 +4124,112 @@
       <c r="V58" s="17"/>
       <c r="W58" s="17"/>
     </row>
-    <row r="59" spans="1:24" ht="15.75" customHeight="1">
+    <row r="59" spans="1:24" s="34" customFormat="1" ht="15.75" customHeight="1">
       <c r="A59" s="16" t="s">
-        <v>111</v>
+        <v>63</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="C59" s="20"/>
-      <c r="D59" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="E59" s="20"/>
-      <c r="F59" s="20"/>
-      <c r="G59" s="20"/>
-      <c r="H59" s="20"/>
-      <c r="I59" s="20"/>
-      <c r="J59" s="20"/>
-      <c r="K59" s="20"/>
-      <c r="L59" s="20"/>
-      <c r="M59" s="20"/>
-      <c r="N59" s="20"/>
-      <c r="O59" s="20"/>
-      <c r="P59" s="20"/>
-      <c r="Q59" s="20"/>
-      <c r="R59" s="20"/>
-      <c r="S59" s="20"/>
-      <c r="T59" s="20"/>
-      <c r="U59" s="20"/>
-      <c r="V59" s="20"/>
-      <c r="W59" s="20"/>
+        <v>137</v>
+      </c>
+      <c r="C59" s="17"/>
+      <c r="D59" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="E59" s="17"/>
+      <c r="F59" s="17"/>
+      <c r="G59" s="17"/>
+      <c r="H59" s="17"/>
+      <c r="I59" s="17"/>
+      <c r="J59" s="17"/>
+      <c r="K59" s="17"/>
+      <c r="L59" s="17"/>
+      <c r="M59" s="17"/>
+      <c r="N59" s="17"/>
+      <c r="O59" s="17"/>
+      <c r="P59" s="17"/>
+      <c r="Q59" s="17"/>
+      <c r="R59" s="17"/>
+      <c r="S59" s="17"/>
+      <c r="T59" s="17"/>
+      <c r="U59" s="17"/>
+      <c r="V59" s="17"/>
+      <c r="W59" s="17"/>
     </row>
     <row r="60" spans="1:24" ht="15.75" customHeight="1">
       <c r="A60" s="16" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="C60" s="20"/>
       <c r="D60" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E60" s="20"/>
+      <c r="F60" s="20"/>
+      <c r="G60" s="20"/>
+      <c r="H60" s="20"/>
+      <c r="I60" s="20"/>
+      <c r="J60" s="20"/>
+      <c r="K60" s="20"/>
+      <c r="L60" s="20"/>
+      <c r="M60" s="20"/>
+      <c r="N60" s="20"/>
+      <c r="O60" s="20"/>
+      <c r="P60" s="20"/>
+      <c r="Q60" s="20"/>
+      <c r="R60" s="20"/>
+      <c r="S60" s="20"/>
+      <c r="T60" s="20"/>
+      <c r="U60" s="20"/>
+      <c r="V60" s="20"/>
+      <c r="W60" s="20"/>
+    </row>
+    <row r="61" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A61" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="B61" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="C61" s="20"/>
+      <c r="D61" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="E60" s="31" t="s">
+      <c r="E61" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="F60" s="31"/>
-      <c r="G60" s="31" t="s">
+      <c r="F61" s="31"/>
+      <c r="G61" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="H60" s="31"/>
-      <c r="I60" s="31"/>
-      <c r="J60" s="31" t="s">
+      <c r="H61" s="31"/>
+      <c r="I61" s="31"/>
+      <c r="J61" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="K60" s="31" t="s">
+      <c r="K61" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="L60" s="31" t="s">
+      <c r="L61" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="M60" s="31"/>
-      <c r="N60" s="31"/>
-      <c r="O60" s="31"/>
-      <c r="P60" s="31"/>
-      <c r="Q60" s="31"/>
-      <c r="R60" s="31"/>
-      <c r="S60" s="31"/>
-      <c r="T60" s="31"/>
-      <c r="U60" s="31"/>
-      <c r="V60" s="31"/>
-      <c r="W60" s="31"/>
+      <c r="M61" s="31"/>
+      <c r="N61" s="31"/>
+      <c r="O61" s="31"/>
+      <c r="P61" s="31"/>
+      <c r="Q61" s="31"/>
+      <c r="R61" s="31"/>
+      <c r="S61" s="31"/>
+      <c r="T61" s="31"/>
+      <c r="U61" s="31"/>
+      <c r="V61" s="31"/>
+      <c r="W61" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="X50:X51"/>
+    <mergeCell ref="X51:X52"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="J5:N5"/>
     <mergeCell ref="P5:V5"/>

</xml_diff>

<commit_message>
Käytä oikeaa sido-oikeustermiä roolit-excelissä päällystys- ja paikkauskohteille
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26812"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarihan/Desktop/Harja/harja/resources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3860" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="8580" yWindow="3840" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -430,13 +435,13 @@
     <t>Laskutusyhteenveto</t>
   </si>
   <si>
-    <t>R,W,sidonta</t>
-  </si>
-  <si>
     <t>API-järjestelmätunnukset</t>
   </si>
   <si>
     <t>Toimenpiteiden ajoittuminen</t>
+  </si>
+  <si>
+    <t>R,W,sido</t>
   </si>
 </sst>
 </file>
@@ -1011,13 +1016,13 @@
   <dimension ref="A1:X61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B52" sqref="B52"/>
+      <selection pane="bottomRight" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.5" bestFit="1" customWidth="1"/>
@@ -1044,7 +1049,7 @@
     <col min="24" max="24" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" customHeight="1">
+    <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1064,7 +1069,7 @@
       <c r="M1" s="38"/>
       <c r="N1" s="38"/>
     </row>
-    <row r="2" spans="1:24" ht="15.75" customHeight="1">
+    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="40" t="s">
@@ -1082,7 +1087,7 @@
       <c r="M2" s="38"/>
       <c r="N2" s="38"/>
     </row>
-    <row r="3" spans="1:24" ht="15.75" customHeight="1">
+    <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -1097,10 +1102,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="15.75" customHeight="1">
+    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:24" ht="15.75" customHeight="1">
+    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C5" s="39" t="s">
         <v>6</v>
       </c>
@@ -1129,7 +1134,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="15.75" customHeight="1">
+    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -1198,7 +1203,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="15.75" customHeight="1">
+    <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="16" t="s">
         <v>15</v>
       </c>
@@ -1266,7 +1271,7 @@
       <c r="W7" s="17"/>
       <c r="X7" s="10"/>
     </row>
-    <row r="8" spans="1:24" ht="15.75" customHeight="1">
+    <row r="8" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="16" t="s">
         <v>15</v>
       </c>
@@ -1320,7 +1325,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="15.75" customHeight="1">
+    <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="16" t="s">
         <v>15</v>
       </c>
@@ -1368,7 +1373,7 @@
       <c r="W9" s="17"/>
       <c r="X9" s="10"/>
     </row>
-    <row r="10" spans="1:24" ht="15.75" customHeight="1">
+    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="16" t="s">
         <v>15</v>
       </c>
@@ -1416,7 +1421,7 @@
       <c r="W10" s="17"/>
       <c r="X10" s="10"/>
     </row>
-    <row r="11" spans="1:24" ht="15.75" customHeight="1">
+    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="16" t="s">
         <v>15</v>
       </c>
@@ -1478,7 +1483,7 @@
       <c r="W11" s="17"/>
       <c r="X11" s="10"/>
     </row>
-    <row r="12" spans="1:24" ht="15.75" customHeight="1">
+    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="16" t="s">
         <v>15</v>
       </c>
@@ -1540,7 +1545,7 @@
       <c r="W12" s="17"/>
       <c r="X12" s="10"/>
     </row>
-    <row r="13" spans="1:24" ht="15.75" customHeight="1">
+    <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="16" t="s">
         <v>15</v>
       </c>
@@ -1590,7 +1595,7 @@
       <c r="W13" s="17"/>
       <c r="X13" s="10"/>
     </row>
-    <row r="14" spans="1:24" ht="15.75" customHeight="1">
+    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="16" t="s">
         <v>15</v>
       </c>
@@ -1640,7 +1645,7 @@
       <c r="W14" s="17"/>
       <c r="X14" s="10"/>
     </row>
-    <row r="15" spans="1:24" ht="15.75" customHeight="1">
+    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="16" t="s">
         <v>15</v>
       </c>
@@ -1690,7 +1695,7 @@
       <c r="W15" s="17"/>
       <c r="X15" s="10"/>
     </row>
-    <row r="16" spans="1:24" ht="15.75" customHeight="1">
+    <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="16" t="s">
         <v>15</v>
       </c>
@@ -1752,7 +1757,7 @@
       <c r="W16" s="17"/>
       <c r="X16" s="10"/>
     </row>
-    <row r="17" spans="1:24" ht="15.75" customHeight="1">
+    <row r="17" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="16" t="s">
         <v>15</v>
       </c>
@@ -1814,7 +1819,7 @@
       <c r="W17" s="17"/>
       <c r="X17" s="10"/>
     </row>
-    <row r="18" spans="1:24" ht="15.75" customHeight="1">
+    <row r="18" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="16" t="s">
         <v>15</v>
       </c>
@@ -1864,7 +1869,7 @@
       <c r="W18" s="17"/>
       <c r="X18" s="10"/>
     </row>
-    <row r="19" spans="1:24" ht="15.75" customHeight="1">
+    <row r="19" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="16" t="s">
         <v>15</v>
       </c>
@@ -1926,7 +1931,7 @@
       <c r="W19" s="17"/>
       <c r="X19" s="10"/>
     </row>
-    <row r="20" spans="1:24" ht="15.75" customHeight="1">
+    <row r="20" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="16" t="s">
         <v>15</v>
       </c>
@@ -1992,7 +1997,7 @@
       <c r="W20" s="17"/>
       <c r="X20" s="10"/>
     </row>
-    <row r="21" spans="1:24" ht="15.75" customHeight="1">
+    <row r="21" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="27" t="s">
         <v>15</v>
       </c>
@@ -2060,7 +2065,7 @@
       <c r="W21" s="21"/>
       <c r="X21" s="10"/>
     </row>
-    <row r="22" spans="1:24" ht="15.75" customHeight="1">
+    <row r="22" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="27" t="s">
         <v>15</v>
       </c>
@@ -2126,7 +2131,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="23" spans="1:24" ht="15.75" customHeight="1">
+    <row r="23" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="27" t="s">
         <v>15</v>
       </c>
@@ -2192,7 +2197,7 @@
       <c r="W23" s="21"/>
       <c r="X23" s="10"/>
     </row>
-    <row r="24" spans="1:24" ht="15.75" customHeight="1">
+    <row r="24" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="27" t="s">
         <v>15</v>
       </c>
@@ -2254,7 +2259,7 @@
       <c r="W24" s="21"/>
       <c r="X24" s="10"/>
     </row>
-    <row r="25" spans="1:24" ht="15.75" customHeight="1">
+    <row r="25" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="27" t="s">
         <v>15</v>
       </c>
@@ -2304,7 +2309,7 @@
       <c r="W25" s="21"/>
       <c r="X25" s="10"/>
     </row>
-    <row r="26" spans="1:24" ht="15.75" customHeight="1">
+    <row r="26" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="27" t="s">
         <v>15</v>
       </c>
@@ -2350,7 +2355,7 @@
       <c r="W26" s="21"/>
       <c r="X26" s="10"/>
     </row>
-    <row r="27" spans="1:24" ht="15.75" customHeight="1">
+    <row r="27" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="27" t="s">
         <v>15</v>
       </c>
@@ -2390,7 +2395,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:24" ht="15.75" customHeight="1">
+    <row r="28" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="27" t="s">
         <v>15</v>
       </c>
@@ -2456,7 +2461,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="29" spans="1:24" ht="15.75" customHeight="1">
+    <row r="29" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="27" t="s">
         <v>15</v>
       </c>
@@ -2465,10 +2470,10 @@
       </c>
       <c r="C29" s="21"/>
       <c r="D29" s="21" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F29" s="21" t="s">
         <v>17</v>
@@ -2518,7 +2523,7 @@
       <c r="W29" s="21"/>
       <c r="X29" s="10"/>
     </row>
-    <row r="30" spans="1:24" ht="15.75" customHeight="1">
+    <row r="30" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="27" t="s">
         <v>15</v>
       </c>
@@ -2580,7 +2585,7 @@
       <c r="W30" s="21"/>
       <c r="X30" s="10"/>
     </row>
-    <row r="31" spans="1:24" ht="15.75" customHeight="1">
+    <row r="31" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="27" t="s">
         <v>15</v>
       </c>
@@ -2589,10 +2594,10 @@
       </c>
       <c r="C31" s="21"/>
       <c r="D31" s="21" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F31" s="21" t="s">
         <v>17</v>
@@ -2642,7 +2647,7 @@
       <c r="W31" s="21"/>
       <c r="X31" s="10"/>
     </row>
-    <row r="32" spans="1:24" ht="15.75" customHeight="1">
+    <row r="32" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="27" t="s">
         <v>15</v>
       </c>
@@ -2704,7 +2709,7 @@
       <c r="W32" s="21"/>
       <c r="X32" s="10"/>
     </row>
-    <row r="33" spans="1:24" s="13" customFormat="1" ht="15.75" customHeight="1">
+    <row r="33" spans="1:24" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="27" t="s">
         <v>15</v>
       </c>
@@ -2772,7 +2777,7 @@
       <c r="W33" s="21"/>
       <c r="X33" s="12"/>
     </row>
-    <row r="34" spans="1:24" s="33" customFormat="1" ht="15.75" customHeight="1">
+    <row r="34" spans="1:24" s="33" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="27" t="s">
         <v>43</v>
       </c>
@@ -2818,7 +2823,7 @@
       <c r="W34" s="21"/>
       <c r="X34" s="32"/>
     </row>
-    <row r="35" spans="1:24" ht="15.75" customHeight="1">
+    <row r="35" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="27" t="s">
         <v>43</v>
       </c>
@@ -2868,7 +2873,7 @@
       <c r="W35" s="21"/>
       <c r="X35" s="10"/>
     </row>
-    <row r="36" spans="1:24" ht="15.75" customHeight="1">
+    <row r="36" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="27" t="s">
         <v>43</v>
       </c>
@@ -2934,7 +2939,7 @@
       <c r="W36" s="21"/>
       <c r="X36" s="10"/>
     </row>
-    <row r="37" spans="1:24" ht="15.75" customHeight="1">
+    <row r="37" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="27" t="s">
         <v>43</v>
       </c>
@@ -3000,7 +3005,7 @@
       <c r="W37" s="21"/>
       <c r="X37" s="10"/>
     </row>
-    <row r="38" spans="1:24" ht="15.75" customHeight="1">
+    <row r="38" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="27" t="s">
         <v>43</v>
       </c>
@@ -3066,7 +3071,7 @@
       <c r="W38" s="21"/>
       <c r="X38" s="10"/>
     </row>
-    <row r="39" spans="1:24" ht="15.75" customHeight="1">
+    <row r="39" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="27" t="s">
         <v>43</v>
       </c>
@@ -3132,7 +3137,7 @@
       <c r="W39" s="21"/>
       <c r="X39" s="10"/>
     </row>
-    <row r="40" spans="1:24" ht="15.75" customHeight="1">
+    <row r="40" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="27" t="s">
         <v>43</v>
       </c>
@@ -3198,7 +3203,7 @@
       <c r="W40" s="21"/>
       <c r="X40" s="10"/>
     </row>
-    <row r="41" spans="1:24" ht="15.75" customHeight="1">
+    <row r="41" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="27" t="s">
         <v>43</v>
       </c>
@@ -3256,7 +3261,7 @@
       <c r="W41" s="21"/>
       <c r="X41" s="10"/>
     </row>
-    <row r="42" spans="1:24" ht="15.75" customHeight="1">
+    <row r="42" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="27" t="s">
         <v>43</v>
       </c>
@@ -3322,7 +3327,7 @@
       <c r="W42" s="21"/>
       <c r="X42" s="10"/>
     </row>
-    <row r="43" spans="1:24" ht="15.75" customHeight="1">
+    <row r="43" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="27" t="s">
         <v>43</v>
       </c>
@@ -3374,7 +3379,7 @@
       <c r="W43" s="21"/>
       <c r="X43" s="10"/>
     </row>
-    <row r="44" spans="1:24" ht="15.75" customHeight="1">
+    <row r="44" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="27" t="s">
         <v>43</v>
       </c>
@@ -3424,7 +3429,7 @@
       <c r="W44" s="21"/>
       <c r="X44" s="10"/>
     </row>
-    <row r="45" spans="1:24" ht="15.75" customHeight="1">
+    <row r="45" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="27" t="s">
         <v>43</v>
       </c>
@@ -3472,7 +3477,7 @@
       <c r="W45" s="21"/>
       <c r="X45" s="10"/>
     </row>
-    <row r="46" spans="1:24" ht="15.75" customHeight="1">
+    <row r="46" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="27" t="s">
         <v>43</v>
       </c>
@@ -3520,7 +3525,7 @@
       <c r="W46" s="21"/>
       <c r="X46" s="10"/>
     </row>
-    <row r="47" spans="1:24" ht="15.75" customHeight="1">
+    <row r="47" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="27" t="s">
         <v>43</v>
       </c>
@@ -3568,7 +3573,7 @@
       <c r="W47" s="21"/>
       <c r="X47" s="10"/>
     </row>
-    <row r="48" spans="1:24" s="30" customFormat="1" ht="15.75" customHeight="1">
+    <row r="48" spans="1:24" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="27" t="s">
         <v>43</v>
       </c>
@@ -3626,7 +3631,7 @@
       <c r="W48" s="21"/>
       <c r="X48" s="29"/>
     </row>
-    <row r="49" spans="1:24" ht="15.75" customHeight="1">
+    <row r="49" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="27" t="s">
         <v>43</v>
       </c>
@@ -3692,12 +3697,12 @@
       <c r="W49" s="21"/>
       <c r="X49" s="10"/>
     </row>
-    <row r="50" spans="1:24" s="36" customFormat="1" ht="15.75" customHeight="1">
+    <row r="50" spans="1:24" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="27" t="s">
         <v>43</v>
       </c>
       <c r="B50" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C50" s="21"/>
       <c r="D50" s="21" t="s">
@@ -3746,7 +3751,7 @@
       <c r="W50" s="21"/>
       <c r="X50" s="35"/>
     </row>
-    <row r="51" spans="1:24" ht="15.75" customHeight="1">
+    <row r="51" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="27" t="s">
         <v>58</v>
       </c>
@@ -3816,7 +3821,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="1:24" ht="15.75" customHeight="1">
+    <row r="52" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="27" t="s">
         <v>58</v>
       </c>
@@ -3884,7 +3889,7 @@
       <c r="W52" s="21"/>
       <c r="X52" s="38"/>
     </row>
-    <row r="53" spans="1:24" ht="15.75" customHeight="1">
+    <row r="53" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="27" t="s">
         <v>62</v>
       </c>
@@ -3950,7 +3955,7 @@
       <c r="W53" s="21"/>
       <c r="X53" s="10"/>
     </row>
-    <row r="54" spans="1:24" s="15" customFormat="1" ht="15.75" customHeight="1">
+    <row r="54" spans="1:24" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="18" t="s">
         <v>63</v>
       </c>
@@ -3988,7 +3993,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="55" spans="1:24" ht="15.75" customHeight="1">
+    <row r="55" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="16" t="s">
         <v>63</v>
       </c>
@@ -4031,7 +4036,7 @@
       <c r="V55" s="17"/>
       <c r="W55" s="17"/>
     </row>
-    <row r="56" spans="1:24" ht="15.75" customHeight="1">
+    <row r="56" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="16" t="s">
         <v>63</v>
       </c>
@@ -4062,7 +4067,7 @@
       <c r="V56" s="17"/>
       <c r="W56" s="17"/>
     </row>
-    <row r="57" spans="1:24" ht="15.75" customHeight="1">
+    <row r="57" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="16" t="s">
         <v>63</v>
       </c>
@@ -4093,7 +4098,7 @@
       <c r="V57" s="17"/>
       <c r="W57" s="17"/>
     </row>
-    <row r="58" spans="1:24" ht="15.75" customHeight="1">
+    <row r="58" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="16" t="s">
         <v>63</v>
       </c>
@@ -4124,12 +4129,12 @@
       <c r="V58" s="17"/>
       <c r="W58" s="17"/>
     </row>
-    <row r="59" spans="1:24" s="34" customFormat="1" ht="15.75" customHeight="1">
+    <row r="59" spans="1:24" s="34" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="16" t="s">
         <v>63</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C59" s="17"/>
       <c r="D59" s="17" t="s">
@@ -4155,7 +4160,7 @@
       <c r="V59" s="17"/>
       <c r="W59" s="17"/>
     </row>
-    <row r="60" spans="1:24" ht="15.75" customHeight="1">
+    <row r="60" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="16" t="s">
         <v>111</v>
       </c>
@@ -4186,7 +4191,7 @@
       <c r="V60" s="20"/>
       <c r="W60" s="20"/>
     </row>
-    <row r="61" spans="1:24" ht="15.75" customHeight="1">
+    <row r="61" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="16" t="s">
         <v>130</v>
       </c>
@@ -4238,11 +4243,6 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4254,7 +4254,7 @@
       <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="29.6640625" customWidth="1"/>
     <col min="2" max="2" width="28.1640625" customWidth="1"/>
@@ -4262,7 +4262,7 @@
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
         <v>70</v>
       </c>
@@ -4279,7 +4279,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15">
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
         <v>73</v>
       </c>
@@ -4292,7 +4292,7 @@
       <c r="D2" s="24"/>
       <c r="E2" s="24"/>
     </row>
-    <row r="3" spans="1:5" ht="15">
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
         <v>75</v>
       </c>
@@ -4305,7 +4305,7 @@
       <c r="D3" s="24"/>
       <c r="E3" s="24"/>
     </row>
-    <row r="4" spans="1:5" ht="15">
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
         <v>77</v>
       </c>
@@ -4318,7 +4318,7 @@
       <c r="D4" s="24"/>
       <c r="E4" s="24"/>
     </row>
-    <row r="5" spans="1:5" ht="15">
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
         <v>97</v>
       </c>
@@ -4333,7 +4333,7 @@
       </c>
       <c r="E5" s="24"/>
     </row>
-    <row r="6" spans="1:5" ht="15">
+    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
         <v>98</v>
       </c>
@@ -4348,7 +4348,7 @@
       </c>
       <c r="E6" s="24"/>
     </row>
-    <row r="7" spans="1:5" ht="15">
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
         <v>99</v>
       </c>
@@ -4363,7 +4363,7 @@
       </c>
       <c r="E7" s="24"/>
     </row>
-    <row r="8" spans="1:5" ht="15">
+    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
         <v>100</v>
       </c>
@@ -4378,7 +4378,7 @@
       </c>
       <c r="E8" s="24"/>
     </row>
-    <row r="9" spans="1:5" ht="15">
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
         <v>109</v>
       </c>
@@ -4393,7 +4393,7 @@
       </c>
       <c r="E9" s="24"/>
     </row>
-    <row r="10" spans="1:5" ht="15">
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
         <v>108</v>
       </c>
@@ -4408,7 +4408,7 @@
       </c>
       <c r="E10" s="24"/>
     </row>
-    <row r="11" spans="1:5" ht="15">
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
         <v>107</v>
       </c>
@@ -4423,7 +4423,7 @@
       </c>
       <c r="E11" s="24"/>
     </row>
-    <row r="12" spans="1:5" ht="15">
+    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
         <v>101</v>
       </c>
@@ -4438,7 +4438,7 @@
       </c>
       <c r="E12" s="24"/>
     </row>
-    <row r="13" spans="1:5" ht="15">
+    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
         <v>106</v>
       </c>
@@ -4453,7 +4453,7 @@
       </c>
       <c r="E13" s="24"/>
     </row>
-    <row r="14" spans="1:5" ht="15">
+    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
         <v>102</v>
       </c>
@@ -4468,7 +4468,7 @@
       </c>
       <c r="E14" s="24"/>
     </row>
-    <row r="15" spans="1:5" ht="15">
+    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
         <v>103</v>
       </c>
@@ -4483,7 +4483,7 @@
       </c>
       <c r="E15" s="24"/>
     </row>
-    <row r="16" spans="1:5" ht="15">
+    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
         <v>104</v>
       </c>
@@ -4498,7 +4498,7 @@
       </c>
       <c r="E16" s="24"/>
     </row>
-    <row r="17" spans="1:5" ht="15">
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
         <v>134</v>
       </c>
@@ -4513,7 +4513,7 @@
       </c>
       <c r="E17" s="24"/>
     </row>
-    <row r="18" spans="1:5" ht="15">
+    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
         <v>12</v>
       </c>
@@ -4528,7 +4528,7 @@
       </c>
       <c r="E18" s="24"/>
     </row>
-    <row r="19" spans="1:5" ht="15">
+    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
         <v>13</v>
       </c>
@@ -4543,7 +4543,7 @@
       </c>
       <c r="E19" s="24"/>
     </row>
-    <row r="20" spans="1:5" ht="15">
+    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
         <v>105</v>
       </c>
@@ -4558,7 +4558,7 @@
       </c>
       <c r="E20" s="24"/>
     </row>
-    <row r="21" spans="1:5" ht="15">
+    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
         <v>118</v>
       </c>
@@ -4577,10 +4577,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Roolit: poista suolan ja mater. suunnitteluoikeus urakoitsijalta
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8580" yWindow="3840" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="8580" yWindow="300" windowWidth="29820" windowHeight="20840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -1011,10 +1011,10 @@
   <dimension ref="A1:X61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="H47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="J7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="M61" sqref="M61"/>
+      <selection pane="bottomRight" activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1459,10 +1459,10 @@
       </c>
       <c r="O11" s="17"/>
       <c r="P11" s="17" t="s">
-        <v>115</v>
+        <v>17</v>
       </c>
       <c r="Q11" s="17" t="s">
-        <v>115</v>
+        <v>17</v>
       </c>
       <c r="R11" s="17" t="s">
         <v>17</v>
@@ -1521,10 +1521,10 @@
       </c>
       <c r="O12" s="17"/>
       <c r="P12" s="17" t="s">
-        <v>115</v>
+        <v>17</v>
       </c>
       <c r="Q12" s="17" t="s">
-        <v>115</v>
+        <v>17</v>
       </c>
       <c r="R12" s="17" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Roolit: poista urakoitsijalta oikeus kirjata erilliskustannuksia
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8580" yWindow="300" windowWidth="29820" windowHeight="20840" tabRatio="500"/>
+    <workbookView xWindow="19500" yWindow="300" windowWidth="18900" windowHeight="20840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -1011,10 +1011,10 @@
   <dimension ref="A1:X61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="J7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="N7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="Q11" sqref="Q11"/>
+      <selection pane="bottomRight" activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1849,10 +1849,10 @@
       <c r="N18" s="21"/>
       <c r="O18" s="17"/>
       <c r="P18" s="17" t="s">
-        <v>115</v>
+        <v>17</v>
       </c>
       <c r="Q18" s="17" t="s">
-        <v>115</v>
+        <v>17</v>
       </c>
       <c r="R18" s="21"/>
       <c r="S18" s="21"/>

</xml_diff>

<commit_message>
Roolit: Poista til.laadunvalv. oikeus nähdä turv.rap
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="139">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -1011,10 +1011,10 @@
   <dimension ref="A1:X61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="N7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A18" sqref="A18:XFD18"/>
+      <selection pane="bottomRight" activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -3337,9 +3337,7 @@
         <v>17</v>
       </c>
       <c r="F43" s="21"/>
-      <c r="G43" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="G43" s="21"/>
       <c r="H43" s="21"/>
       <c r="I43" s="21" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Lisää tuki periytyville oikeuksille
Oikeus voidaan merkitä Exceliin esim R+, jolloin se on voimassa kaikissa
oman organisaation urakoissa. R* tarkoittaa kaikkia urakoita. Pelkkä R
on vain siihen urakkaan annettu oikeus. Sama myös W oikeuksille.
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="19500" yWindow="300" windowWidth="18900" windowHeight="20840" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28700" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="144">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -382,45 +382,27 @@
     <t>Tiemerkitsijä</t>
   </si>
   <si>
-    <t>R = lukuoikeus, R,W = luku- ja kirjoitusoikeus, tyhjä = ei näe osiota, muut erikoisoikeuksia</t>
-  </si>
-  <si>
     <t>R,TM-valmis</t>
   </si>
   <si>
     <t>Sallitaanko urakoitsijalle hintojen syöttö?</t>
   </si>
   <si>
-    <t>R,W,päätös</t>
-  </si>
-  <si>
     <t>Liitteet</t>
   </si>
   <si>
-    <t>R,W,poista</t>
-  </si>
-  <si>
     <t>päätös tarkoittaa päätöksen tekemisoikeutta</t>
   </si>
   <si>
     <t>TM-valmis oikeus voi kirjata tiemerkinnän valmistumispäivämäärän, ei muita kenttiä</t>
   </si>
   <si>
-    <t xml:space="preserve">R </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Yrityksen urakan laadunvalvoja</t>
-  </si>
-  <si>
     <t>Laadunseuranta</t>
   </si>
   <si>
     <t>Kirjaus</t>
   </si>
   <si>
-    <t>W</t>
-  </si>
-  <si>
     <t>Sanktioiden yhteenveto</t>
   </si>
   <si>
@@ -436,7 +418,40 @@
     <t>Toimenpiteiden ajoittuminen</t>
   </si>
   <si>
-    <t>R,W,sido</t>
+    <t>R = lukuoikeus, R,W = luku- ja kirjoitusoikeus, tyhjä = ei näe osiota, muut erikoisoikeuksia, * R/W perässä tarkoittaa kaikkiin urakoihin, + tarkoittaa oman organisaation urakoihin</t>
+  </si>
+  <si>
+    <t>R*,W*</t>
+  </si>
+  <si>
+    <t>R*,W*,poista</t>
+  </si>
+  <si>
+    <t>R*,W*,sido</t>
+  </si>
+  <si>
+    <t>R*</t>
+  </si>
+  <si>
+    <t>W*</t>
+  </si>
+  <si>
+    <t>R*,W+</t>
+  </si>
+  <si>
+    <t>R*,W</t>
+  </si>
+  <si>
+    <t>R+</t>
+  </si>
+  <si>
+    <t>R+,W+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Urakan laadunvalvoja</t>
+  </si>
+  <si>
+    <t>R*,W,päätös</t>
   </si>
 </sst>
 </file>
@@ -491,7 +506,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -528,12 +543,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -559,7 +568,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -581,8 +590,48 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -625,9 +674,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -653,7 +699,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="61">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -664,6 +710,26 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -674,6 +740,26 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1011,10 +1097,10 @@
   <dimension ref="A1:X61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="S27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="G45" sqref="G45"/>
+      <selection pane="bottomRight" activeCell="S44" sqref="S44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1036,7 +1122,7 @@
     <col min="16" max="16" width="11.6640625" customWidth="1"/>
     <col min="17" max="17" width="10.6640625" customWidth="1"/>
     <col min="18" max="18" width="12.5" customWidth="1"/>
-    <col min="19" max="19" width="12.5" style="25" customWidth="1"/>
+    <col min="19" max="19" width="17.6640625" style="25" customWidth="1"/>
     <col min="20" max="20" width="11.5" customWidth="1"/>
     <col min="21" max="21" width="10.6640625" customWidth="1"/>
     <col min="22" max="22" width="11.1640625" customWidth="1"/>
@@ -1049,38 +1135,38 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="40" t="s">
-        <v>120</v>
-      </c>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
+      <c r="C1" s="39" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
     </row>
     <row r="2" spans="1:24" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
     </row>
     <row r="3" spans="1:24" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
@@ -1101,30 +1187,30 @@
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:24" ht="15.75" customHeight="1">
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="J5" s="39" t="s">
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="J5" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
-      <c r="M5" s="38"/>
-      <c r="N5" s="38"/>
-      <c r="P5" s="39" t="s">
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="37"/>
+      <c r="P5" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="Q5" s="38"/>
-      <c r="R5" s="38"/>
-      <c r="S5" s="38"/>
-      <c r="T5" s="38"/>
-      <c r="U5" s="38"/>
-      <c r="V5" s="38"/>
+      <c r="Q5" s="37"/>
+      <c r="R5" s="37"/>
+      <c r="S5" s="37"/>
+      <c r="T5" s="37"/>
+      <c r="U5" s="37"/>
+      <c r="V5" s="37"/>
       <c r="X5" s="5" t="s">
         <v>14</v>
       </c>
@@ -1183,7 +1269,7 @@
         <v>90</v>
       </c>
       <c r="S6" s="9" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="T6" s="9" t="s">
         <v>91</v>
@@ -1207,55 +1293,55 @@
       </c>
       <c r="C7" s="17"/>
       <c r="D7" s="17" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="K7" s="17" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="L7" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="M7" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="N7" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="O7" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
+      </c>
+      <c r="M7" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="N7" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="O7" s="21" t="s">
+        <v>136</v>
       </c>
       <c r="P7" s="17" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="Q7" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="R7" s="17" t="s">
-        <v>17</v>
+      <c r="R7" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="S7" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T7" s="17" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="U7" s="17" t="s">
         <v>17</v>
@@ -1275,31 +1361,31 @@
       </c>
       <c r="C8" s="17"/>
       <c r="D8" s="17" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G8" s="21"/>
       <c r="H8" s="21"/>
       <c r="I8" s="21"/>
       <c r="J8" s="17" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="K8" s="17" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="L8" s="21"/>
-      <c r="M8" s="26" t="s">
-        <v>17</v>
+      <c r="M8" s="21" t="s">
+        <v>136</v>
       </c>
       <c r="N8" s="21"/>
       <c r="O8" s="17"/>
       <c r="P8" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="Q8" s="21" t="s">
         <v>17</v>
@@ -1307,7 +1393,7 @@
       <c r="R8" s="17"/>
       <c r="S8" s="17"/>
       <c r="T8" s="17" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="U8" s="17" t="s">
         <v>19</v>
@@ -1317,7 +1403,7 @@
       </c>
       <c r="W8" s="17"/>
       <c r="X8" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="15.75" customHeight="1">
@@ -1329,31 +1415,31 @@
       </c>
       <c r="C9" s="17"/>
       <c r="D9" s="17" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G9" s="21"/>
       <c r="H9" s="21"/>
       <c r="I9" s="21"/>
       <c r="J9" s="17" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="K9" s="17" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="L9" s="21"/>
-      <c r="M9" s="26" t="s">
-        <v>17</v>
+      <c r="M9" s="21" t="s">
+        <v>136</v>
       </c>
       <c r="N9" s="21"/>
       <c r="O9" s="17"/>
       <c r="P9" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="Q9" s="21" t="s">
         <v>17</v>
@@ -1361,7 +1447,7 @@
       <c r="R9" s="17"/>
       <c r="S9" s="17"/>
       <c r="T9" s="17" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="U9" s="17"/>
       <c r="V9" s="17"/>
@@ -1377,31 +1463,31 @@
       </c>
       <c r="C10" s="17"/>
       <c r="D10" s="17" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G10" s="21"/>
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
       <c r="J10" s="17" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="K10" s="17" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="L10" s="21"/>
-      <c r="M10" s="26" t="s">
-        <v>17</v>
+      <c r="M10" s="21" t="s">
+        <v>136</v>
       </c>
       <c r="N10" s="21"/>
       <c r="O10" s="17"/>
       <c r="P10" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="Q10" s="21" t="s">
         <v>17</v>
@@ -1409,7 +1495,7 @@
       <c r="R10" s="17"/>
       <c r="S10" s="17"/>
       <c r="T10" s="17" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="U10" s="17"/>
       <c r="V10" s="17"/>
@@ -1425,53 +1511,53 @@
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="17" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="I11" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="K11" s="17" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="L11" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="M11" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="N11" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
+      </c>
+      <c r="M11" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="N11" s="21" t="s">
+        <v>136</v>
       </c>
       <c r="O11" s="17"/>
       <c r="P11" s="17" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="Q11" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="R11" s="17" t="s">
-        <v>17</v>
+      <c r="R11" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="S11" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T11" s="17" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="U11" s="17"/>
       <c r="V11" s="17"/>
@@ -1487,53 +1573,53 @@
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="17" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="K12" s="17" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="L12" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="M12" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="N12" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
+      </c>
+      <c r="M12" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="N12" s="21" t="s">
+        <v>136</v>
       </c>
       <c r="O12" s="17"/>
       <c r="P12" s="17" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="Q12" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="R12" s="17" t="s">
-        <v>17</v>
+      <c r="R12" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="S12" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T12" s="17" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="U12" s="17"/>
       <c r="V12" s="17"/>
@@ -1549,33 +1635,33 @@
       </c>
       <c r="C13" s="17"/>
       <c r="D13" s="17" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G13" s="21"/>
       <c r="H13" s="21"/>
       <c r="I13" s="21"/>
       <c r="J13" s="17" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="K13" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="L13" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="M13" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
+      </c>
+      <c r="M13" s="21" t="s">
+        <v>136</v>
       </c>
       <c r="N13" s="21"/>
       <c r="O13" s="17"/>
       <c r="P13" s="17" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="Q13" s="17" t="s">
         <v>115</v>
@@ -1583,7 +1669,7 @@
       <c r="R13" s="21"/>
       <c r="S13" s="17"/>
       <c r="T13" s="17" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="U13" s="17"/>
       <c r="V13" s="17"/>
@@ -1599,33 +1685,33 @@
       </c>
       <c r="C14" s="17"/>
       <c r="D14" s="17" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
       <c r="I14" s="21"/>
       <c r="J14" s="17" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="K14" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="L14" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="M14" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
+      </c>
+      <c r="M14" s="21" t="s">
+        <v>136</v>
       </c>
       <c r="N14" s="21"/>
       <c r="O14" s="17"/>
       <c r="P14" s="17" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="Q14" s="17" t="s">
         <v>115</v>
@@ -1633,7 +1719,7 @@
       <c r="R14" s="21"/>
       <c r="S14" s="17"/>
       <c r="T14" s="17" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="U14" s="17"/>
       <c r="V14" s="17"/>
@@ -1649,33 +1735,33 @@
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="17" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G15" s="21"/>
       <c r="H15" s="21"/>
       <c r="I15" s="21"/>
       <c r="J15" s="17" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="K15" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="L15" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="M15" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
+      </c>
+      <c r="M15" s="21" t="s">
+        <v>136</v>
       </c>
       <c r="N15" s="21"/>
       <c r="O15" s="17"/>
       <c r="P15" s="17" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="Q15" s="17" t="s">
         <v>115</v>
@@ -1683,7 +1769,7 @@
       <c r="R15" s="21"/>
       <c r="S15" s="17"/>
       <c r="T15" s="17" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="U15" s="17"/>
       <c r="V15" s="17"/>
@@ -1699,53 +1785,53 @@
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="17" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="J16" s="17" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="K16" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="L16" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="M16" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="N16" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
+      </c>
+      <c r="M16" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="N16" s="21" t="s">
+        <v>136</v>
       </c>
       <c r="O16" s="17"/>
       <c r="P16" s="17" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="Q16" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="R16" s="17" t="s">
-        <v>17</v>
+      <c r="R16" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="S16" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T16" s="17" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="U16" s="17"/>
       <c r="V16" s="17"/>
@@ -1761,53 +1847,53 @@
       </c>
       <c r="C17" s="17"/>
       <c r="D17" s="17" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="I17" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="J17" s="17" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="K17" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="L17" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="M17" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="N17" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
+      </c>
+      <c r="M17" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="N17" s="21" t="s">
+        <v>136</v>
       </c>
       <c r="O17" s="17"/>
       <c r="P17" s="17" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="Q17" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="R17" s="17" t="s">
-        <v>17</v>
+      <c r="R17" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="S17" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T17" s="17" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="U17" s="17"/>
       <c r="V17" s="17"/>
@@ -1823,33 +1909,33 @@
       </c>
       <c r="C18" s="17"/>
       <c r="D18" s="17" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G18" s="21"/>
       <c r="H18" s="21"/>
       <c r="I18" s="21"/>
       <c r="J18" s="17" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="K18" s="17" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="L18" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="M18" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
+      </c>
+      <c r="M18" s="21" t="s">
+        <v>136</v>
       </c>
       <c r="N18" s="21"/>
       <c r="O18" s="17"/>
       <c r="P18" s="17" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="Q18" s="17" t="s">
         <v>17</v>
@@ -1857,7 +1943,7 @@
       <c r="R18" s="21"/>
       <c r="S18" s="21"/>
       <c r="T18" s="17" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="U18" s="17"/>
       <c r="V18" s="17"/>
@@ -1873,53 +1959,53 @@
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="17" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="I19" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="J19" s="17" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="K19" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="L19" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="M19" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="N19" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
+      </c>
+      <c r="M19" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="N19" s="21" t="s">
+        <v>136</v>
       </c>
       <c r="O19" s="17"/>
       <c r="P19" s="17" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="Q19" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="R19" s="17" t="s">
-        <v>17</v>
+      <c r="R19" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="S19" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T19" s="17" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="U19" s="17"/>
       <c r="V19" s="17"/>
@@ -1935,55 +2021,55 @@
       </c>
       <c r="C20" s="17"/>
       <c r="D20" s="17" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="J20" s="17" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="K20" s="17" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="L20" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="M20" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="N20" s="17" t="s">
-        <v>17</v>
+        <v>138</v>
+      </c>
+      <c r="M20" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="N20" s="21" t="s">
+        <v>136</v>
       </c>
       <c r="O20" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="P20" s="17" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="Q20" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="R20" s="17" t="s">
-        <v>17</v>
+      <c r="R20" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="S20" s="21" t="s">
         <v>115</v>
       </c>
       <c r="T20" s="17" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="U20" s="17"/>
       <c r="V20" s="21" t="s">
@@ -1993,63 +2079,63 @@
       <c r="X20" s="10"/>
     </row>
     <row r="21" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="26" t="s">
         <v>30</v>
       </c>
       <c r="C21" s="21"/>
-      <c r="D21" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="E21" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="F21" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="H21" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="I21" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="J21" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="K21" s="21" t="s">
-        <v>115</v>
+      <c r="D21" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="I21" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="J21" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="K21" s="17" t="s">
+        <v>139</v>
       </c>
       <c r="L21" s="21" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="M21" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="N21" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="O21" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="P21" s="21" t="s">
-        <v>115</v>
+        <v>136</v>
+      </c>
+      <c r="P21" s="17" t="s">
+        <v>141</v>
       </c>
       <c r="Q21" s="21" t="s">
         <v>115</v>
       </c>
       <c r="R21" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="S21" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="T21" s="21" t="s">
-        <v>17</v>
+      <c r="T21" s="17" t="s">
+        <v>140</v>
       </c>
       <c r="U21" s="21" t="s">
         <v>17</v>
@@ -2061,61 +2147,61 @@
       <c r="X21" s="10"/>
     </row>
     <row r="22" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A22" s="27" t="s">
+      <c r="A22" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="27" t="s">
+      <c r="B22" s="26" t="s">
         <v>31</v>
       </c>
       <c r="C22" s="21"/>
-      <c r="D22" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="F22" s="21" t="s">
-        <v>17</v>
+      <c r="D22" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>136</v>
       </c>
       <c r="G22" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="H22" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="I22" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="J22" s="21" t="s">
-        <v>115</v>
+        <v>136</v>
+      </c>
+      <c r="H22" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="I22" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="J22" s="17" t="s">
+        <v>138</v>
       </c>
       <c r="K22" s="21" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="L22" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="M22" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="N22" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="O22" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="P22" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="Q22" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R22" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="S22" s="21"/>
-      <c r="T22" s="21" t="s">
-        <v>17</v>
+      <c r="T22" s="17" t="s">
+        <v>140</v>
       </c>
       <c r="U22" s="21"/>
       <c r="V22" s="21" t="s">
@@ -2123,67 +2209,67 @@
       </c>
       <c r="W22" s="21"/>
       <c r="X22" s="10" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A23" s="27" t="s">
+      <c r="A23" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="27" t="s">
+      <c r="B23" s="26" t="s">
         <v>32</v>
       </c>
       <c r="C23" s="21"/>
-      <c r="D23" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="F23" s="21" t="s">
-        <v>17</v>
+      <c r="D23" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>136</v>
       </c>
       <c r="G23" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="H23" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="I23" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="J23" s="21" t="s">
-        <v>115</v>
+        <v>136</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="I23" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="J23" s="17" t="s">
+        <v>138</v>
       </c>
       <c r="K23" s="21" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="L23" s="21" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="M23" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="N23" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="O23" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="P23" s="21" t="s">
-        <v>115</v>
+        <v>136</v>
+      </c>
+      <c r="P23" s="17" t="s">
+        <v>141</v>
       </c>
       <c r="Q23" s="21" t="s">
         <v>115</v>
       </c>
       <c r="R23" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="S23" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="T23" s="21" t="s">
-        <v>17</v>
+      <c r="T23" s="17" t="s">
+        <v>140</v>
       </c>
       <c r="U23" s="21"/>
       <c r="V23" s="21" t="s">
@@ -2193,61 +2279,61 @@
       <c r="X23" s="10"/>
     </row>
     <row r="24" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A24" s="27" t="s">
+      <c r="A24" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="26" t="s">
         <v>33</v>
       </c>
       <c r="C24" s="21"/>
-      <c r="D24" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="E24" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="F24" s="21" t="s">
-        <v>17</v>
+      <c r="D24" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>136</v>
       </c>
       <c r="G24" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="H24" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="I24" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="J24" s="21" t="s">
-        <v>115</v>
+        <v>136</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="I24" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="J24" s="17" t="s">
+        <v>138</v>
       </c>
       <c r="K24" s="21" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="L24" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="M24" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="N24" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="O24" s="21"/>
       <c r="P24" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="Q24" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R24" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="S24" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="T24" s="21" t="s">
-        <v>17</v>
+      <c r="T24" s="17" t="s">
+        <v>140</v>
       </c>
       <c r="U24" s="21"/>
       <c r="V24" s="21"/>
@@ -2255,47 +2341,47 @@
       <c r="X24" s="10"/>
     </row>
     <row r="25" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A25" s="27" t="s">
+      <c r="A25" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="27" t="s">
+      <c r="B25" s="26" t="s">
         <v>34</v>
       </c>
       <c r="C25" s="21"/>
-      <c r="D25" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="E25" s="21" t="s">
-        <v>115</v>
+      <c r="D25" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>133</v>
       </c>
       <c r="F25" s="21"/>
       <c r="G25" s="21"/>
       <c r="H25" s="21"/>
       <c r="I25" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="J25" s="21" t="s">
-        <v>115</v>
+        <v>133</v>
+      </c>
+      <c r="J25" s="17" t="s">
+        <v>138</v>
       </c>
       <c r="K25" s="21" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="L25" s="21"/>
       <c r="M25" s="21"/>
       <c r="N25" s="21"/>
       <c r="O25" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="P25" s="21" t="s">
-        <v>115</v>
+        <v>138</v>
+      </c>
+      <c r="P25" s="17" t="s">
+        <v>141</v>
       </c>
       <c r="Q25" s="21" t="s">
         <v>115</v>
       </c>
       <c r="R25" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="S25" s="28"/>
+        <v>140</v>
+      </c>
+      <c r="S25" s="27"/>
       <c r="T25" s="21"/>
       <c r="U25" s="21"/>
       <c r="V25" s="21" t="s">
@@ -2305,39 +2391,39 @@
       <c r="X25" s="10"/>
     </row>
     <row r="26" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A26" s="27" t="s">
+      <c r="A26" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="27" t="s">
+      <c r="B26" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C26" s="21"/>
-      <c r="D26" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="E26" s="21" t="s">
-        <v>115</v>
+      <c r="D26" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>136</v>
       </c>
       <c r="F26" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G26" s="21"/>
       <c r="H26" s="21"/>
       <c r="I26" s="21"/>
-      <c r="J26" s="21" t="s">
-        <v>115</v>
+      <c r="J26" s="17" t="s">
+        <v>138</v>
       </c>
       <c r="K26" s="21" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="L26" s="21"/>
       <c r="M26" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="N26" s="21"/>
       <c r="O26" s="21"/>
       <c r="P26" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="Q26" s="21" t="s">
         <v>17</v>
@@ -2351,28 +2437,28 @@
       <c r="X26" s="10"/>
     </row>
     <row r="27" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A27" s="27" t="s">
+      <c r="A27" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="27" t="s">
+      <c r="B27" s="26" t="s">
         <v>36</v>
       </c>
       <c r="C27" s="21"/>
-      <c r="D27" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="E27" s="21" t="s">
-        <v>115</v>
+      <c r="D27" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>133</v>
       </c>
       <c r="F27" s="21"/>
       <c r="G27" s="21"/>
       <c r="H27" s="21"/>
       <c r="I27" s="21"/>
-      <c r="J27" s="21" t="s">
-        <v>115</v>
+      <c r="J27" s="17" t="s">
+        <v>138</v>
       </c>
       <c r="K27" s="21" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="L27" s="21"/>
       <c r="M27" s="21"/>
@@ -2391,127 +2477,127 @@
       </c>
     </row>
     <row r="28" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A28" s="27" t="s">
+      <c r="A28" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="27" t="s">
+      <c r="B28" s="26" t="s">
         <v>38</v>
       </c>
       <c r="C28" s="21"/>
-      <c r="D28" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="E28" s="21" t="s">
-        <v>115</v>
+      <c r="D28" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>133</v>
       </c>
       <c r="F28" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G28" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="H28" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="I28" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="J28" s="21" t="s">
-        <v>115</v>
+        <v>136</v>
+      </c>
+      <c r="J28" s="17" t="s">
+        <v>138</v>
       </c>
       <c r="K28" s="21" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="L28" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="M28" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="N28" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
+      </c>
+      <c r="N28" s="17" t="s">
+        <v>136</v>
       </c>
       <c r="O28" s="21"/>
       <c r="P28" s="21" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="Q28" s="21" t="s">
         <v>115</v>
       </c>
       <c r="R28" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="S28" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="T28" s="21" t="s">
-        <v>17</v>
+      <c r="T28" s="17" t="s">
+        <v>140</v>
       </c>
       <c r="U28" s="21"/>
       <c r="V28" s="21"/>
       <c r="W28" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="X28" s="10" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="27" t="s">
+      <c r="B29" s="26" t="s">
         <v>39</v>
       </c>
       <c r="C29" s="21"/>
       <c r="D29" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="F29" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="G29" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="H29" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="I29" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="J29" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="E29" s="21" t="s">
-        <v>138</v>
-      </c>
-      <c r="F29" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="G29" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="H29" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="I29" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="J29" s="21" t="s">
-        <v>115</v>
-      </c>
       <c r="K29" s="21" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="L29" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="M29" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="N29" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
+      </c>
+      <c r="N29" s="17" t="s">
+        <v>136</v>
       </c>
       <c r="O29" s="21"/>
       <c r="P29" s="21" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="Q29" s="21" t="s">
         <v>115</v>
       </c>
       <c r="R29" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="S29" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="T29" s="21" t="s">
-        <v>17</v>
+      <c r="T29" s="17" t="s">
+        <v>140</v>
       </c>
       <c r="U29" s="21"/>
       <c r="V29" s="21"/>
@@ -2519,61 +2605,61 @@
       <c r="X29" s="10"/>
     </row>
     <row r="30" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="27" t="s">
+      <c r="B30" s="26" t="s">
         <v>40</v>
       </c>
       <c r="C30" s="21"/>
-      <c r="D30" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="E30" s="21" t="s">
-        <v>115</v>
+      <c r="D30" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>133</v>
       </c>
       <c r="F30" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G30" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="H30" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="I30" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="J30" s="21" t="s">
-        <v>115</v>
+        <v>136</v>
+      </c>
+      <c r="J30" s="17" t="s">
+        <v>138</v>
       </c>
       <c r="K30" s="21" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="L30" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="M30" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="N30" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
+      </c>
+      <c r="N30" s="17" t="s">
+        <v>136</v>
       </c>
       <c r="O30" s="21"/>
       <c r="P30" s="21" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="Q30" s="21" t="s">
         <v>115</v>
       </c>
       <c r="R30" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="S30" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="T30" s="21" t="s">
-        <v>17</v>
+      <c r="T30" s="17" t="s">
+        <v>140</v>
       </c>
       <c r="U30" s="21"/>
       <c r="V30" s="21"/>
@@ -2581,61 +2667,61 @@
       <c r="X30" s="10"/>
     </row>
     <row r="31" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="27" t="s">
+      <c r="B31" s="26" t="s">
         <v>41</v>
       </c>
       <c r="C31" s="21"/>
       <c r="D31" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="E31" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="F31" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="G31" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="H31" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="I31" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="J31" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="E31" s="21" t="s">
-        <v>138</v>
-      </c>
-      <c r="F31" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="G31" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="H31" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="I31" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="J31" s="21" t="s">
-        <v>115</v>
-      </c>
       <c r="K31" s="21" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="L31" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="M31" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="N31" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
+      </c>
+      <c r="N31" s="17" t="s">
+        <v>136</v>
       </c>
       <c r="O31" s="21"/>
       <c r="P31" s="21" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="Q31" s="21" t="s">
         <v>115</v>
       </c>
       <c r="R31" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="S31" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="T31" s="21" t="s">
-        <v>17</v>
+      <c r="T31" s="17" t="s">
+        <v>140</v>
       </c>
       <c r="U31" s="21"/>
       <c r="V31" s="21"/>
@@ -2643,61 +2729,61 @@
       <c r="X31" s="10"/>
     </row>
     <row r="32" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A32" s="27" t="s">
+      <c r="A32" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="27" t="s">
+      <c r="B32" s="26" t="s">
         <v>42</v>
       </c>
       <c r="C32" s="21"/>
-      <c r="D32" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="E32" s="21" t="s">
-        <v>115</v>
+      <c r="D32" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E32" s="17" t="s">
+        <v>133</v>
       </c>
       <c r="F32" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G32" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="H32" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="I32" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="J32" s="21" t="s">
-        <v>115</v>
+        <v>136</v>
+      </c>
+      <c r="J32" s="17" t="s">
+        <v>138</v>
       </c>
       <c r="K32" s="21" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="L32" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="M32" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="N32" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
+      </c>
+      <c r="N32" s="17" t="s">
+        <v>136</v>
       </c>
       <c r="O32" s="21"/>
       <c r="P32" s="21" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="Q32" s="21" t="s">
         <v>115</v>
       </c>
       <c r="R32" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="S32" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="T32" s="21" t="s">
-        <v>17</v>
+      <c r="T32" s="17" t="s">
+        <v>140</v>
       </c>
       <c r="U32" s="21"/>
       <c r="V32" s="21"/>
@@ -2705,63 +2791,63 @@
       <c r="X32" s="10"/>
     </row>
     <row r="33" spans="1:24" s="13" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A33" s="27" t="s">
+      <c r="A33" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="27" t="s">
-        <v>124</v>
+      <c r="B33" s="26" t="s">
+        <v>122</v>
       </c>
       <c r="C33" s="21"/>
-      <c r="D33" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="E33" s="21" t="s">
-        <v>115</v>
+      <c r="D33" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>133</v>
       </c>
       <c r="F33" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G33" s="21" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="H33" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="I33" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="J33" s="21" t="s">
-        <v>115</v>
+        <v>133</v>
+      </c>
+      <c r="J33" s="17" t="s">
+        <v>138</v>
       </c>
       <c r="K33" s="21" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="L33" s="21" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="M33" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="N33" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="O33" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
+      </c>
+      <c r="N33" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="O33" s="17" t="s">
+        <v>136</v>
       </c>
       <c r="P33" s="21" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="Q33" s="21" t="s">
         <v>115</v>
       </c>
       <c r="R33" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="S33" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="T33" s="21" t="s">
-        <v>17</v>
+      <c r="T33" s="17" t="s">
+        <v>140</v>
       </c>
       <c r="U33" s="21" t="s">
         <v>17</v>
@@ -2772,40 +2858,40 @@
       <c r="W33" s="21"/>
       <c r="X33" s="12"/>
     </row>
-    <row r="34" spans="1:24" s="33" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A34" s="27" t="s">
+    <row r="34" spans="1:24" s="32" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A34" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="27" t="s">
-        <v>135</v>
+      <c r="B34" s="26" t="s">
+        <v>129</v>
       </c>
       <c r="C34" s="21"/>
-      <c r="D34" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="E34" s="21" t="s">
-        <v>115</v>
+      <c r="D34" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>136</v>
       </c>
       <c r="F34" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G34" s="21"/>
       <c r="H34" s="21"/>
       <c r="I34" s="21"/>
       <c r="J34" s="21" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="K34" s="21" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="L34" s="21"/>
       <c r="M34" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="N34" s="21"/>
       <c r="O34" s="21"/>
       <c r="P34" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="Q34" s="21" t="s">
         <v>17</v>
@@ -2816,24 +2902,24 @@
       <c r="U34" s="21"/>
       <c r="V34" s="21"/>
       <c r="W34" s="21"/>
-      <c r="X34" s="32"/>
+      <c r="X34" s="31"/>
     </row>
     <row r="35" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A35" s="27" t="s">
+      <c r="A35" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="26" t="s">
         <v>44</v>
       </c>
       <c r="C35" s="21"/>
       <c r="D35" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="F35" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G35" s="21" t="s">
         <v>19</v>
@@ -2841,19 +2927,19 @@
       <c r="H35" s="21"/>
       <c r="I35" s="21"/>
       <c r="J35" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="K35" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="L35" s="21"/>
       <c r="M35" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="N35" s="21"/>
       <c r="O35" s="21"/>
       <c r="P35" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="Q35" s="21" t="s">
         <v>17</v>
@@ -2861,7 +2947,7 @@
       <c r="R35" s="21"/>
       <c r="S35" s="21"/>
       <c r="T35" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="U35" s="21"/>
       <c r="V35" s="21"/>
@@ -2869,63 +2955,63 @@
       <c r="X35" s="10"/>
     </row>
     <row r="36" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A36" s="27" t="s">
+      <c r="A36" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B36" s="27" t="s">
+      <c r="B36" s="26" t="s">
         <v>45</v>
       </c>
       <c r="C36" s="21"/>
       <c r="D36" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="F36" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G36" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="H36" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="I36" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="J36" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="K36" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="L36" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="M36" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="N36" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="O36" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="P36" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="Q36" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R36" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="S36" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T36" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="U36" s="21"/>
       <c r="V36" s="21" t="s">
@@ -2935,63 +3021,63 @@
       <c r="X36" s="10"/>
     </row>
     <row r="37" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A37" s="27" t="s">
+      <c r="A37" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B37" s="27" t="s">
+      <c r="B37" s="26" t="s">
         <v>46</v>
       </c>
       <c r="C37" s="21"/>
       <c r="D37" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="F37" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G37" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="H37" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="I37" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="J37" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="K37" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="L37" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="M37" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="N37" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="O37" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="P37" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="Q37" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R37" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="S37" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T37" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="U37" s="21"/>
       <c r="V37" s="21" t="s">
@@ -3001,63 +3087,63 @@
       <c r="X37" s="10"/>
     </row>
     <row r="38" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A38" s="27" t="s">
+      <c r="A38" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="27" t="s">
+      <c r="B38" s="26" t="s">
         <v>47</v>
       </c>
       <c r="C38" s="21"/>
       <c r="D38" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="E38" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="F38" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G38" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="H38" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="I38" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="J38" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="K38" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="L38" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="M38" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="N38" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="O38" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="P38" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="Q38" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R38" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="S38" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T38" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="U38" s="21"/>
       <c r="V38" s="21" t="s">
@@ -3067,63 +3153,63 @@
       <c r="X38" s="10"/>
     </row>
     <row r="39" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A39" s="27" t="s">
+      <c r="A39" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="27" t="s">
+      <c r="B39" s="26" t="s">
         <v>48</v>
       </c>
       <c r="C39" s="21"/>
       <c r="D39" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="E39" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="F39" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G39" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="H39" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="I39" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="J39" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="K39" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="L39" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="M39" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="N39" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="O39" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="P39" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="Q39" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R39" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="S39" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T39" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="U39" s="21"/>
       <c r="V39" s="21" t="s">
@@ -3133,63 +3219,63 @@
       <c r="X39" s="10"/>
     </row>
     <row r="40" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A40" s="27" t="s">
+      <c r="A40" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B40" s="27" t="s">
+      <c r="B40" s="26" t="s">
         <v>49</v>
       </c>
       <c r="C40" s="21"/>
       <c r="D40" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="E40" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="F40" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G40" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="H40" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="I40" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="J40" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="K40" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="L40" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="M40" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="N40" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="O40" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="P40" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="Q40" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R40" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="S40" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T40" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="U40" s="21"/>
       <c r="V40" s="21" t="s">
@@ -3199,55 +3285,55 @@
       <c r="X40" s="10"/>
     </row>
     <row r="41" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A41" s="27" t="s">
+      <c r="A41" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B41" s="27" t="s">
+      <c r="B41" s="26" t="s">
         <v>50</v>
       </c>
       <c r="C41" s="21"/>
       <c r="D41" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="E41" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="F41" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G41" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="H41" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="I41" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="J41" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="K41" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="L41" s="21"/>
       <c r="M41" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="N41" s="21"/>
       <c r="O41" s="21"/>
       <c r="P41" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="Q41" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R41" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="S41" s="21"/>
       <c r="T41" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="U41" s="21"/>
       <c r="V41" s="21" t="s">
@@ -3257,63 +3343,63 @@
       <c r="X41" s="10"/>
     </row>
     <row r="42" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A42" s="27" t="s">
+      <c r="A42" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B42" s="27" t="s">
+      <c r="B42" s="26" t="s">
         <v>51</v>
       </c>
       <c r="C42" s="21"/>
       <c r="D42" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="E42" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="F42" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G42" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="H42" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="I42" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="J42" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="K42" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="L42" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="M42" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="N42" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="O42" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="P42" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="Q42" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R42" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="S42" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T42" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="U42" s="21"/>
       <c r="V42" s="21" t="s">
@@ -3323,39 +3409,39 @@
       <c r="X42" s="10"/>
     </row>
     <row r="43" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A43" s="27" t="s">
+      <c r="A43" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B43" s="27" t="s">
+      <c r="B43" s="26" t="s">
         <v>52</v>
       </c>
       <c r="C43" s="21"/>
       <c r="D43" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="E43" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="F43" s="21"/>
       <c r="G43" s="21"/>
       <c r="H43" s="21"/>
       <c r="I43" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="J43" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="K43" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="L43" s="21"/>
       <c r="M43" s="21"/>
       <c r="N43" s="21"/>
       <c r="O43" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="P43" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="Q43" s="21" t="s">
         <v>17</v>
@@ -3363,7 +3449,7 @@
       <c r="R43" s="21"/>
       <c r="S43" s="21"/>
       <c r="T43" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="U43" s="21"/>
       <c r="V43" s="21" t="s">
@@ -3373,21 +3459,21 @@
       <c r="X43" s="10"/>
     </row>
     <row r="44" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A44" s="27" t="s">
+      <c r="A44" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="27" t="s">
+      <c r="B44" s="26" t="s">
         <v>53</v>
       </c>
       <c r="C44" s="21"/>
       <c r="D44" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="E44" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="F44" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G44" s="21"/>
       <c r="H44" s="21" t="s">
@@ -3395,21 +3481,21 @@
       </c>
       <c r="I44" s="21"/>
       <c r="J44" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="K44" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="L44" s="21"/>
       <c r="M44" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="N44" s="21" t="s">
         <v>19</v>
       </c>
       <c r="O44" s="21"/>
       <c r="P44" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="Q44" s="21" t="s">
         <v>17</v>
@@ -3423,39 +3509,39 @@
       <c r="X44" s="10"/>
     </row>
     <row r="45" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A45" s="27" t="s">
+      <c r="A45" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B45" s="27" t="s">
+      <c r="B45" s="26" t="s">
         <v>54</v>
       </c>
       <c r="C45" s="21"/>
       <c r="D45" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="E45" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="F45" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G45" s="21"/>
       <c r="H45" s="21"/>
       <c r="I45" s="21"/>
       <c r="J45" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="K45" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="L45" s="21"/>
       <c r="M45" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="N45" s="21"/>
       <c r="O45" s="21"/>
       <c r="P45" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="Q45" s="21" t="s">
         <v>17</v>
@@ -3463,7 +3549,7 @@
       <c r="R45" s="21"/>
       <c r="S45" s="21"/>
       <c r="T45" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="U45" s="21"/>
       <c r="V45" s="21"/>
@@ -3471,39 +3557,39 @@
       <c r="X45" s="10"/>
     </row>
     <row r="46" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A46" s="27" t="s">
+      <c r="A46" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B46" s="27" t="s">
+      <c r="B46" s="26" t="s">
         <v>55</v>
       </c>
       <c r="C46" s="21"/>
       <c r="D46" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="E46" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="F46" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G46" s="21"/>
       <c r="H46" s="21"/>
       <c r="I46" s="21"/>
       <c r="J46" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="K46" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="L46" s="21"/>
       <c r="M46" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="N46" s="21"/>
       <c r="O46" s="21"/>
       <c r="P46" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="Q46" s="21" t="s">
         <v>17</v>
@@ -3511,7 +3597,7 @@
       <c r="R46" s="21"/>
       <c r="S46" s="21"/>
       <c r="T46" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="U46" s="21"/>
       <c r="V46" s="21"/>
@@ -3519,39 +3605,39 @@
       <c r="X46" s="10"/>
     </row>
     <row r="47" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A47" s="27" t="s">
+      <c r="A47" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B47" s="27" t="s">
+      <c r="B47" s="26" t="s">
         <v>56</v>
       </c>
       <c r="C47" s="21"/>
       <c r="D47" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="E47" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="F47" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G47" s="21"/>
       <c r="H47" s="21"/>
       <c r="I47" s="21"/>
       <c r="J47" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="K47" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="L47" s="21"/>
       <c r="M47" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="N47" s="21"/>
       <c r="O47" s="21"/>
       <c r="P47" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="Q47" s="21" t="s">
         <v>17</v>
@@ -3559,129 +3645,129 @@
       <c r="R47" s="21"/>
       <c r="S47" s="21"/>
       <c r="T47" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="U47" s="21"/>
       <c r="V47" s="21"/>
       <c r="W47" s="21"/>
       <c r="X47" s="10"/>
     </row>
-    <row r="48" spans="1:24" s="30" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A48" s="27" t="s">
+    <row r="48" spans="1:24" s="29" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A48" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B48" s="27" t="s">
-        <v>133</v>
+      <c r="B48" s="26" t="s">
+        <v>127</v>
       </c>
       <c r="C48" s="21"/>
       <c r="D48" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="E48" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="F48" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G48" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="H48" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="I48" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="J48" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="K48" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="L48" s="21"/>
       <c r="M48" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="N48" s="21"/>
       <c r="O48" s="21"/>
       <c r="P48" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="Q48" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R48" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="S48" s="21"/>
       <c r="T48" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="U48" s="21"/>
       <c r="V48" s="21" t="s">
         <v>17</v>
       </c>
       <c r="W48" s="21"/>
-      <c r="X48" s="29"/>
+      <c r="X48" s="28"/>
     </row>
     <row r="49" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A49" s="27" t="s">
+      <c r="A49" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B49" s="27" t="s">
+      <c r="B49" s="26" t="s">
         <v>57</v>
       </c>
       <c r="C49" s="21"/>
       <c r="D49" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="E49" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="F49" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G49" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="H49" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="I49" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="J49" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="K49" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="L49" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="M49" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="N49" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="O49" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="P49" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="Q49" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R49" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="S49" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T49" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="U49" s="21"/>
       <c r="V49" s="21" t="s">
@@ -3690,118 +3776,126 @@
       <c r="W49" s="21"/>
       <c r="X49" s="10"/>
     </row>
-    <row r="50" spans="1:24" s="36" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A50" s="27" t="s">
+    <row r="50" spans="1:24" s="35" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A50" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B50" s="27" t="s">
-        <v>137</v>
+      <c r="B50" s="26" t="s">
+        <v>131</v>
       </c>
       <c r="C50" s="21"/>
       <c r="D50" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="E50" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="F50" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G50" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="H50" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="I50" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="J50" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="K50" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="L50" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="M50" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="N50" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="O50" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="P50" s="21"/>
-      <c r="Q50" s="21"/>
-      <c r="R50" s="21"/>
-      <c r="S50" s="21"/>
+        <v>136</v>
+      </c>
+      <c r="P50" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q50" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="R50" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="S50" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="T50" s="21"/>
       <c r="U50" s="21"/>
       <c r="V50" s="21"/>
       <c r="W50" s="21"/>
-      <c r="X50" s="35"/>
+      <c r="X50" s="34"/>
     </row>
     <row r="51" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A51" s="27" t="s">
+      <c r="A51" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="B51" s="27" t="s">
+      <c r="B51" s="26" t="s">
         <v>59</v>
       </c>
       <c r="C51" s="21"/>
       <c r="D51" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="E51" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="F51" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G51" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="H51" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="I51" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="J51" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="K51" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="L51" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="M51" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="N51" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="O51" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="P51" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="Q51" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R51" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="S51" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T51" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="U51" s="21" t="s">
         <v>17</v>
@@ -3810,68 +3904,68 @@
         <v>17</v>
       </c>
       <c r="W51" s="21"/>
-      <c r="X51" s="37" t="s">
+      <c r="X51" s="36" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="52" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A52" s="27" t="s">
+      <c r="A52" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="B52" s="27" t="s">
+      <c r="B52" s="26" t="s">
         <v>61</v>
       </c>
       <c r="C52" s="21"/>
       <c r="D52" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="E52" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="F52" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G52" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="H52" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="I52" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="J52" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="K52" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="L52" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="M52" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="N52" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="O52" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="P52" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="Q52" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R52" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="S52" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T52" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="U52" s="21" t="s">
         <v>17</v>
@@ -3880,64 +3974,64 @@
         <v>17</v>
       </c>
       <c r="W52" s="21"/>
-      <c r="X52" s="38"/>
+      <c r="X52" s="37"/>
     </row>
     <row r="53" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A53" s="27" t="s">
+      <c r="A53" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="B53" s="27" t="s">
+      <c r="B53" s="26" t="s">
         <v>62</v>
       </c>
       <c r="C53" s="21"/>
       <c r="D53" s="21" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="E53" s="21" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="F53" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="G53" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="H53" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="I53" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="J53" s="21" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="K53" s="21" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="L53" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="M53" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="N53" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="O53" s="21" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="P53" s="21" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="Q53" s="21" t="s">
         <v>115</v>
       </c>
       <c r="R53" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="S53" s="21"/>
       <c r="T53" s="21" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="U53" s="21" t="s">
         <v>115</v>
@@ -3956,25 +4050,21 @@
         <v>64</v>
       </c>
       <c r="C54" s="19"/>
-      <c r="D54" s="19" t="s">
-        <v>115</v>
+      <c r="D54" s="21" t="s">
+        <v>133</v>
       </c>
       <c r="E54" s="19"/>
       <c r="F54" s="19"/>
       <c r="G54" s="19"/>
       <c r="H54" s="19"/>
       <c r="I54" s="19"/>
-      <c r="J54" s="19" t="s">
-        <v>115</v>
-      </c>
+      <c r="J54" s="19"/>
       <c r="K54" s="19"/>
       <c r="L54" s="19"/>
       <c r="M54" s="19"/>
       <c r="N54" s="19"/>
       <c r="O54" s="19"/>
-      <c r="P54" s="19" t="s">
-        <v>115</v>
-      </c>
+      <c r="P54" s="19"/>
       <c r="Q54" s="19"/>
       <c r="R54" s="19"/>
       <c r="S54" s="19"/>
@@ -3994,8 +4084,8 @@
         <v>66</v>
       </c>
       <c r="C55" s="17"/>
-      <c r="D55" s="17" t="s">
-        <v>115</v>
+      <c r="D55" s="21" t="s">
+        <v>133</v>
       </c>
       <c r="E55" s="17"/>
       <c r="F55" s="17" t="s">
@@ -4037,8 +4127,8 @@
         <v>67</v>
       </c>
       <c r="C56" s="17"/>
-      <c r="D56" s="17" t="s">
-        <v>115</v>
+      <c r="D56" s="21" t="s">
+        <v>133</v>
       </c>
       <c r="E56" s="17"/>
       <c r="F56" s="17"/>
@@ -4068,8 +4158,8 @@
         <v>68</v>
       </c>
       <c r="C57" s="17"/>
-      <c r="D57" s="17" t="s">
-        <v>115</v>
+      <c r="D57" s="21" t="s">
+        <v>133</v>
       </c>
       <c r="E57" s="17"/>
       <c r="F57" s="17"/>
@@ -4099,8 +4189,8 @@
         <v>69</v>
       </c>
       <c r="C58" s="17"/>
-      <c r="D58" s="17" t="s">
-        <v>115</v>
+      <c r="D58" s="21" t="s">
+        <v>133</v>
       </c>
       <c r="E58" s="17"/>
       <c r="F58" s="17"/>
@@ -4122,16 +4212,16 @@
       <c r="V58" s="17"/>
       <c r="W58" s="17"/>
     </row>
-    <row r="59" spans="1:24" s="34" customFormat="1" ht="15.75" customHeight="1">
+    <row r="59" spans="1:24" s="33" customFormat="1" ht="15.75" customHeight="1">
       <c r="A59" s="16" t="s">
         <v>63</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C59" s="17"/>
-      <c r="D59" s="17" t="s">
-        <v>115</v>
+      <c r="D59" s="21" t="s">
+        <v>133</v>
       </c>
       <c r="E59" s="17"/>
       <c r="F59" s="17"/>
@@ -4162,7 +4252,7 @@
       </c>
       <c r="C60" s="20"/>
       <c r="D60" s="21" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="E60" s="20"/>
       <c r="F60" s="20"/>
@@ -4186,46 +4276,46 @@
     </row>
     <row r="61" spans="1:24" ht="15.75" customHeight="1">
       <c r="A61" s="16" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C61" s="20"/>
       <c r="D61" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="E61" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="F61" s="31"/>
-      <c r="G61" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="H61" s="31"/>
-      <c r="I61" s="31"/>
-      <c r="J61" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="K61" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="L61" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="M61" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="N61" s="31"/>
-      <c r="O61" s="31"/>
-      <c r="P61" s="31"/>
-      <c r="Q61" s="31"/>
-      <c r="R61" s="31"/>
-      <c r="S61" s="31"/>
-      <c r="T61" s="31"/>
-      <c r="U61" s="31"/>
-      <c r="V61" s="31"/>
-      <c r="W61" s="31"/>
+        <v>137</v>
+      </c>
+      <c r="E61" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="F61" s="30"/>
+      <c r="G61" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="H61" s="30"/>
+      <c r="I61" s="30"/>
+      <c r="J61" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="K61" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="L61" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="M61" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="N61" s="30"/>
+      <c r="O61" s="30"/>
+      <c r="P61" s="30"/>
+      <c r="Q61" s="30"/>
+      <c r="R61" s="30"/>
+      <c r="S61" s="30"/>
+      <c r="T61" s="30"/>
+      <c r="U61" s="30"/>
+      <c r="V61" s="30"/>
+      <c r="W61" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -4251,7 +4341,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -4500,7 +4590,7 @@
     </row>
     <row r="17" spans="1:5" ht="15">
       <c r="A17" s="23" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B17" s="23" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
HAR-2315 Suunniteltua muutoshintaa ei voi poistaa
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28700" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="39460" windowHeight="22360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="143">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -422,9 +422,6 @@
   </si>
   <si>
     <t>R*,W*</t>
-  </si>
-  <si>
-    <t>R*,W*,poista</t>
   </si>
   <si>
     <t>R*,W*,sido</t>
@@ -1097,10 +1094,10 @@
   <dimension ref="A1:X61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="S27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="S44" sqref="S44"/>
+      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1269,7 +1266,7 @@
         <v>90</v>
       </c>
       <c r="S6" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="T6" s="9" t="s">
         <v>91</v>
@@ -1299,49 +1296,49 @@
         <v>133</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J7" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="K7" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="K7" s="17" t="s">
-        <v>139</v>
-      </c>
       <c r="L7" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M7" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N7" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O7" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="P7" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Q7" s="17" t="s">
         <v>115</v>
       </c>
       <c r="R7" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S7" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T7" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U7" s="17" t="s">
         <v>17</v>
@@ -1367,25 +1364,25 @@
         <v>133</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G8" s="21"/>
       <c r="H8" s="21"/>
       <c r="I8" s="21"/>
       <c r="J8" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="K8" s="17" t="s">
         <v>138</v>
-      </c>
-      <c r="K8" s="17" t="s">
-        <v>139</v>
       </c>
       <c r="L8" s="21"/>
       <c r="M8" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N8" s="21"/>
       <c r="O8" s="17"/>
       <c r="P8" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q8" s="21" t="s">
         <v>17</v>
@@ -1393,7 +1390,7 @@
       <c r="R8" s="17"/>
       <c r="S8" s="17"/>
       <c r="T8" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U8" s="17" t="s">
         <v>19</v>
@@ -1421,25 +1418,25 @@
         <v>133</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G9" s="21"/>
       <c r="H9" s="21"/>
       <c r="I9" s="21"/>
       <c r="J9" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="K9" s="17" t="s">
         <v>138</v>
-      </c>
-      <c r="K9" s="17" t="s">
-        <v>139</v>
       </c>
       <c r="L9" s="21"/>
       <c r="M9" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N9" s="21"/>
       <c r="O9" s="17"/>
       <c r="P9" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q9" s="21" t="s">
         <v>17</v>
@@ -1447,7 +1444,7 @@
       <c r="R9" s="17"/>
       <c r="S9" s="17"/>
       <c r="T9" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U9" s="17"/>
       <c r="V9" s="17"/>
@@ -1463,31 +1460,31 @@
       </c>
       <c r="C10" s="17"/>
       <c r="D10" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E10" s="17" t="s">
         <v>133</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G10" s="21"/>
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
       <c r="J10" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="K10" s="17" t="s">
         <v>138</v>
-      </c>
-      <c r="K10" s="17" t="s">
-        <v>139</v>
       </c>
       <c r="L10" s="21"/>
       <c r="M10" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N10" s="21"/>
       <c r="O10" s="17"/>
       <c r="P10" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q10" s="21" t="s">
         <v>17</v>
@@ -1495,7 +1492,7 @@
       <c r="R10" s="17"/>
       <c r="S10" s="17"/>
       <c r="T10" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U10" s="17"/>
       <c r="V10" s="17"/>
@@ -1517,47 +1514,47 @@
         <v>133</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I11" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J11" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="K11" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="K11" s="17" t="s">
-        <v>139</v>
-      </c>
       <c r="L11" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M11" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N11" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O11" s="17"/>
       <c r="P11" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q11" s="17" t="s">
         <v>17</v>
       </c>
       <c r="R11" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S11" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T11" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U11" s="17"/>
       <c r="V11" s="17"/>
@@ -1579,47 +1576,47 @@
         <v>133</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J12" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="K12" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="K12" s="17" t="s">
-        <v>139</v>
-      </c>
       <c r="L12" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M12" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N12" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O12" s="17"/>
       <c r="P12" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q12" s="17" t="s">
         <v>17</v>
       </c>
       <c r="R12" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S12" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T12" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U12" s="17"/>
       <c r="V12" s="17"/>
@@ -1638,30 +1635,30 @@
         <v>133</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G13" s="21"/>
       <c r="H13" s="21"/>
       <c r="I13" s="21"/>
       <c r="J13" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K13" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L13" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M13" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N13" s="21"/>
       <c r="O13" s="17"/>
       <c r="P13" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Q13" s="17" t="s">
         <v>115</v>
@@ -1669,7 +1666,7 @@
       <c r="R13" s="21"/>
       <c r="S13" s="17"/>
       <c r="T13" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U13" s="17"/>
       <c r="V13" s="17"/>
@@ -1688,30 +1685,30 @@
         <v>133</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
       <c r="I14" s="21"/>
       <c r="J14" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K14" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L14" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M14" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N14" s="21"/>
       <c r="O14" s="17"/>
       <c r="P14" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Q14" s="17" t="s">
         <v>115</v>
@@ -1719,7 +1716,7 @@
       <c r="R14" s="21"/>
       <c r="S14" s="17"/>
       <c r="T14" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U14" s="17"/>
       <c r="V14" s="17"/>
@@ -1738,30 +1735,30 @@
         <v>133</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G15" s="21"/>
       <c r="H15" s="21"/>
       <c r="I15" s="21"/>
       <c r="J15" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K15" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L15" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M15" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N15" s="21"/>
       <c r="O15" s="17"/>
       <c r="P15" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Q15" s="17" t="s">
         <v>115</v>
@@ -1769,7 +1766,7 @@
       <c r="R15" s="21"/>
       <c r="S15" s="17"/>
       <c r="T15" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U15" s="17"/>
       <c r="V15" s="17"/>
@@ -1788,50 +1785,50 @@
         <v>133</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J16" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K16" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L16" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M16" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N16" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O16" s="17"/>
       <c r="P16" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Q16" s="17" t="s">
         <v>115</v>
       </c>
       <c r="R16" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S16" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T16" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U16" s="17"/>
       <c r="V16" s="17"/>
@@ -1850,50 +1847,50 @@
         <v>133</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I17" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J17" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K17" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L17" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M17" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N17" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O17" s="17"/>
       <c r="P17" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Q17" s="17" t="s">
         <v>115</v>
       </c>
       <c r="R17" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S17" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T17" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U17" s="17"/>
       <c r="V17" s="17"/>
@@ -1912,30 +1909,30 @@
         <v>133</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G18" s="21"/>
       <c r="H18" s="21"/>
       <c r="I18" s="21"/>
       <c r="J18" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="K18" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="K18" s="17" t="s">
-        <v>139</v>
-      </c>
       <c r="L18" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M18" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N18" s="21"/>
       <c r="O18" s="17"/>
       <c r="P18" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q18" s="17" t="s">
         <v>17</v>
@@ -1943,7 +1940,7 @@
       <c r="R18" s="21"/>
       <c r="S18" s="21"/>
       <c r="T18" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U18" s="17"/>
       <c r="V18" s="17"/>
@@ -1962,50 +1959,50 @@
         <v>133</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I19" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J19" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K19" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L19" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M19" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N19" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O19" s="17"/>
       <c r="P19" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Q19" s="17" t="s">
         <v>115</v>
       </c>
       <c r="R19" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S19" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T19" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U19" s="17"/>
       <c r="V19" s="17"/>
@@ -2027,49 +2024,49 @@
         <v>133</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G20" s="17" t="s">
         <v>133</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J20" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="K20" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="K20" s="17" t="s">
-        <v>139</v>
-      </c>
       <c r="L20" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M20" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N20" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O20" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="P20" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Q20" s="17" t="s">
         <v>115</v>
       </c>
       <c r="R20" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S20" s="21" t="s">
         <v>115</v>
       </c>
       <c r="T20" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U20" s="17"/>
       <c r="V20" s="21" t="s">
@@ -2093,49 +2090,49 @@
         <v>133</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G21" s="17" t="s">
         <v>133</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I21" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J21" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="K21" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="K21" s="17" t="s">
-        <v>139</v>
-      </c>
       <c r="L21" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M21" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N21" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O21" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="P21" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Q21" s="21" t="s">
         <v>115</v>
       </c>
       <c r="R21" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S21" s="21" t="s">
         <v>115</v>
       </c>
       <c r="T21" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U21" s="21" t="s">
         <v>17</v>
@@ -2161,47 +2158,47 @@
         <v>133</v>
       </c>
       <c r="F22" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G22" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H22" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I22" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J22" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K22" s="21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L22" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M22" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N22" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O22" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="P22" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q22" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R22" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S22" s="21"/>
       <c r="T22" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U22" s="21"/>
       <c r="V22" s="21" t="s">
@@ -2227,49 +2224,49 @@
         <v>133</v>
       </c>
       <c r="F23" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G23" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J23" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="K23" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="K23" s="21" t="s">
-        <v>139</v>
-      </c>
       <c r="L23" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M23" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N23" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O23" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="P23" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Q23" s="21" t="s">
         <v>115</v>
       </c>
       <c r="R23" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S23" s="21" t="s">
         <v>115</v>
       </c>
       <c r="T23" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U23" s="21"/>
       <c r="V23" s="21" t="s">
@@ -2293,47 +2290,47 @@
         <v>133</v>
       </c>
       <c r="F24" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G24" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H24" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I24" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J24" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="K24" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="K24" s="21" t="s">
-        <v>139</v>
-      </c>
       <c r="L24" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M24" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N24" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O24" s="21"/>
       <c r="P24" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q24" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R24" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S24" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T24" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U24" s="21"/>
       <c r="V24" s="21"/>
@@ -2361,25 +2358,25 @@
         <v>133</v>
       </c>
       <c r="J25" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="K25" s="21" t="s">
         <v>138</v>
-      </c>
-      <c r="K25" s="21" t="s">
-        <v>139</v>
       </c>
       <c r="L25" s="21"/>
       <c r="M25" s="21"/>
       <c r="N25" s="21"/>
       <c r="O25" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P25" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Q25" s="21" t="s">
         <v>115</v>
       </c>
       <c r="R25" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S25" s="27"/>
       <c r="T25" s="21"/>
@@ -2399,31 +2396,31 @@
       </c>
       <c r="C26" s="21"/>
       <c r="D26" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F26" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G26" s="21"/>
       <c r="H26" s="21"/>
       <c r="I26" s="21"/>
       <c r="J26" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="K26" s="21" t="s">
         <v>138</v>
-      </c>
-      <c r="K26" s="21" t="s">
-        <v>139</v>
       </c>
       <c r="L26" s="21"/>
       <c r="M26" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N26" s="21"/>
       <c r="O26" s="21"/>
       <c r="P26" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q26" s="21" t="s">
         <v>17</v>
@@ -2455,10 +2452,10 @@
       <c r="H27" s="21"/>
       <c r="I27" s="21"/>
       <c r="J27" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="K27" s="21" t="s">
         <v>138</v>
-      </c>
-      <c r="K27" s="21" t="s">
-        <v>139</v>
       </c>
       <c r="L27" s="21"/>
       <c r="M27" s="21"/>
@@ -2491,47 +2488,47 @@
         <v>133</v>
       </c>
       <c r="F28" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G28" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H28" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I28" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J28" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="K28" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="K28" s="21" t="s">
-        <v>139</v>
-      </c>
       <c r="L28" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M28" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N28" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O28" s="21"/>
       <c r="P28" s="21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Q28" s="21" t="s">
         <v>115</v>
       </c>
       <c r="R28" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S28" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T28" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U28" s="21"/>
       <c r="V28" s="21"/>
@@ -2551,53 +2548,53 @@
       </c>
       <c r="C29" s="21"/>
       <c r="D29" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F29" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G29" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H29" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I29" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J29" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="K29" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="K29" s="21" t="s">
-        <v>139</v>
-      </c>
       <c r="L29" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M29" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N29" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O29" s="21"/>
       <c r="P29" s="21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Q29" s="21" t="s">
         <v>115</v>
       </c>
       <c r="R29" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S29" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T29" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U29" s="21"/>
       <c r="V29" s="21"/>
@@ -2619,47 +2616,47 @@
         <v>133</v>
       </c>
       <c r="F30" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G30" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H30" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I30" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J30" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K30" s="21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L30" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M30" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N30" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O30" s="21"/>
       <c r="P30" s="21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Q30" s="21" t="s">
         <v>115</v>
       </c>
       <c r="R30" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S30" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T30" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U30" s="21"/>
       <c r="V30" s="21"/>
@@ -2675,53 +2672,53 @@
       </c>
       <c r="C31" s="21"/>
       <c r="D31" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F31" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G31" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H31" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I31" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J31" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="K31" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="K31" s="21" t="s">
-        <v>139</v>
-      </c>
       <c r="L31" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M31" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N31" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O31" s="21"/>
       <c r="P31" s="21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Q31" s="21" t="s">
         <v>115</v>
       </c>
       <c r="R31" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S31" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T31" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U31" s="21"/>
       <c r="V31" s="21"/>
@@ -2743,47 +2740,47 @@
         <v>133</v>
       </c>
       <c r="F32" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G32" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H32" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I32" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J32" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="K32" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="K32" s="21" t="s">
-        <v>139</v>
-      </c>
       <c r="L32" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M32" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N32" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O32" s="21"/>
       <c r="P32" s="21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Q32" s="21" t="s">
         <v>115</v>
       </c>
       <c r="R32" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S32" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T32" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U32" s="21"/>
       <c r="V32" s="21"/>
@@ -2805,49 +2802,49 @@
         <v>133</v>
       </c>
       <c r="F33" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G33" s="21" t="s">
         <v>133</v>
       </c>
       <c r="H33" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I33" s="21" t="s">
         <v>133</v>
       </c>
       <c r="J33" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K33" s="21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L33" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M33" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N33" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O33" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="P33" s="21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Q33" s="21" t="s">
         <v>115</v>
       </c>
       <c r="R33" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S33" s="21" t="s">
         <v>115</v>
       </c>
       <c r="T33" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U33" s="21" t="s">
         <v>17</v>
@@ -2867,31 +2864,31 @@
       </c>
       <c r="C34" s="21"/>
       <c r="D34" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F34" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G34" s="21"/>
       <c r="H34" s="21"/>
       <c r="I34" s="21"/>
       <c r="J34" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K34" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L34" s="21"/>
       <c r="M34" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N34" s="21"/>
       <c r="O34" s="21"/>
       <c r="P34" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q34" s="21" t="s">
         <v>17</v>
@@ -2913,13 +2910,13 @@
       </c>
       <c r="C35" s="21"/>
       <c r="D35" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F35" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G35" s="21" t="s">
         <v>19</v>
@@ -2927,19 +2924,19 @@
       <c r="H35" s="21"/>
       <c r="I35" s="21"/>
       <c r="J35" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K35" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L35" s="21"/>
       <c r="M35" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N35" s="21"/>
       <c r="O35" s="21"/>
       <c r="P35" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q35" s="21" t="s">
         <v>17</v>
@@ -2947,7 +2944,7 @@
       <c r="R35" s="21"/>
       <c r="S35" s="21"/>
       <c r="T35" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U35" s="21"/>
       <c r="V35" s="21"/>
@@ -2963,55 +2960,55 @@
       </c>
       <c r="C36" s="21"/>
       <c r="D36" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F36" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G36" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H36" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I36" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J36" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K36" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L36" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M36" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N36" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O36" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="P36" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q36" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R36" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S36" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T36" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U36" s="21"/>
       <c r="V36" s="21" t="s">
@@ -3029,55 +3026,55 @@
       </c>
       <c r="C37" s="21"/>
       <c r="D37" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F37" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G37" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H37" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I37" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J37" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K37" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L37" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M37" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N37" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O37" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="P37" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q37" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R37" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S37" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T37" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U37" s="21"/>
       <c r="V37" s="21" t="s">
@@ -3095,55 +3092,55 @@
       </c>
       <c r="C38" s="21"/>
       <c r="D38" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E38" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F38" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G38" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H38" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I38" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J38" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K38" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L38" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M38" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N38" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O38" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="P38" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q38" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R38" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S38" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T38" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U38" s="21"/>
       <c r="V38" s="21" t="s">
@@ -3161,55 +3158,55 @@
       </c>
       <c r="C39" s="21"/>
       <c r="D39" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E39" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F39" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G39" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H39" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I39" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J39" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K39" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L39" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M39" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N39" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O39" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="P39" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q39" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R39" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S39" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T39" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U39" s="21"/>
       <c r="V39" s="21" t="s">
@@ -3227,55 +3224,55 @@
       </c>
       <c r="C40" s="21"/>
       <c r="D40" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E40" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F40" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G40" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H40" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I40" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J40" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K40" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L40" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M40" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N40" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O40" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="P40" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q40" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R40" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S40" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T40" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U40" s="21"/>
       <c r="V40" s="21" t="s">
@@ -3293,47 +3290,47 @@
       </c>
       <c r="C41" s="21"/>
       <c r="D41" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E41" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F41" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G41" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H41" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I41" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J41" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K41" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L41" s="21"/>
       <c r="M41" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N41" s="21"/>
       <c r="O41" s="21"/>
       <c r="P41" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q41" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R41" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S41" s="21"/>
       <c r="T41" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U41" s="21"/>
       <c r="V41" s="21" t="s">
@@ -3351,55 +3348,55 @@
       </c>
       <c r="C42" s="21"/>
       <c r="D42" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E42" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F42" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G42" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H42" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I42" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J42" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K42" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L42" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M42" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N42" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O42" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="P42" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q42" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R42" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S42" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T42" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U42" s="21"/>
       <c r="V42" s="21" t="s">
@@ -3417,31 +3414,31 @@
       </c>
       <c r="C43" s="21"/>
       <c r="D43" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E43" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F43" s="21"/>
       <c r="G43" s="21"/>
       <c r="H43" s="21"/>
       <c r="I43" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J43" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K43" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L43" s="21"/>
       <c r="M43" s="21"/>
       <c r="N43" s="21"/>
       <c r="O43" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="P43" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q43" s="21" t="s">
         <v>17</v>
@@ -3449,7 +3446,7 @@
       <c r="R43" s="21"/>
       <c r="S43" s="21"/>
       <c r="T43" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U43" s="21"/>
       <c r="V43" s="21" t="s">
@@ -3467,13 +3464,13 @@
       </c>
       <c r="C44" s="21"/>
       <c r="D44" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E44" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F44" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G44" s="21"/>
       <c r="H44" s="21" t="s">
@@ -3481,21 +3478,21 @@
       </c>
       <c r="I44" s="21"/>
       <c r="J44" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K44" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L44" s="21"/>
       <c r="M44" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N44" s="21" t="s">
         <v>19</v>
       </c>
       <c r="O44" s="21"/>
       <c r="P44" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q44" s="21" t="s">
         <v>17</v>
@@ -3517,31 +3514,31 @@
       </c>
       <c r="C45" s="21"/>
       <c r="D45" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E45" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F45" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G45" s="21"/>
       <c r="H45" s="21"/>
       <c r="I45" s="21"/>
       <c r="J45" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K45" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L45" s="21"/>
       <c r="M45" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N45" s="21"/>
       <c r="O45" s="21"/>
       <c r="P45" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q45" s="21" t="s">
         <v>17</v>
@@ -3549,7 +3546,7 @@
       <c r="R45" s="21"/>
       <c r="S45" s="21"/>
       <c r="T45" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U45" s="21"/>
       <c r="V45" s="21"/>
@@ -3565,31 +3562,31 @@
       </c>
       <c r="C46" s="21"/>
       <c r="D46" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E46" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F46" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G46" s="21"/>
       <c r="H46" s="21"/>
       <c r="I46" s="21"/>
       <c r="J46" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K46" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L46" s="21"/>
       <c r="M46" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N46" s="21"/>
       <c r="O46" s="21"/>
       <c r="P46" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q46" s="21" t="s">
         <v>17</v>
@@ -3597,7 +3594,7 @@
       <c r="R46" s="21"/>
       <c r="S46" s="21"/>
       <c r="T46" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U46" s="21"/>
       <c r="V46" s="21"/>
@@ -3613,31 +3610,31 @@
       </c>
       <c r="C47" s="21"/>
       <c r="D47" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E47" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F47" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G47" s="21"/>
       <c r="H47" s="21"/>
       <c r="I47" s="21"/>
       <c r="J47" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K47" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L47" s="21"/>
       <c r="M47" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N47" s="21"/>
       <c r="O47" s="21"/>
       <c r="P47" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q47" s="21" t="s">
         <v>17</v>
@@ -3645,7 +3642,7 @@
       <c r="R47" s="21"/>
       <c r="S47" s="21"/>
       <c r="T47" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U47" s="21"/>
       <c r="V47" s="21"/>
@@ -3661,47 +3658,47 @@
       </c>
       <c r="C48" s="21"/>
       <c r="D48" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E48" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F48" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G48" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H48" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I48" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J48" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K48" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L48" s="21"/>
       <c r="M48" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N48" s="21"/>
       <c r="O48" s="21"/>
       <c r="P48" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q48" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R48" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S48" s="21"/>
       <c r="T48" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U48" s="21"/>
       <c r="V48" s="21" t="s">
@@ -3719,55 +3716,55 @@
       </c>
       <c r="C49" s="21"/>
       <c r="D49" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E49" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F49" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G49" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H49" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I49" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J49" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K49" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L49" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M49" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N49" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O49" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="P49" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q49" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R49" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S49" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T49" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U49" s="21"/>
       <c r="V49" s="21" t="s">
@@ -3785,49 +3782,49 @@
       </c>
       <c r="C50" s="21"/>
       <c r="D50" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E50" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F50" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G50" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H50" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I50" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J50" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K50" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L50" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M50" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N50" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O50" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="P50" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q50" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R50" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S50" s="21" t="s">
         <v>17</v>
@@ -3847,55 +3844,55 @@
       </c>
       <c r="C51" s="21"/>
       <c r="D51" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E51" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F51" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G51" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H51" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I51" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J51" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K51" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L51" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M51" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N51" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O51" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="P51" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q51" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R51" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S51" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T51" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U51" s="21" t="s">
         <v>17</v>
@@ -3917,55 +3914,55 @@
       </c>
       <c r="C52" s="21"/>
       <c r="D52" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E52" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F52" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G52" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H52" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I52" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J52" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K52" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L52" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M52" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N52" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O52" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="P52" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q52" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R52" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S52" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T52" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U52" s="21" t="s">
         <v>17</v>
@@ -3991,47 +3988,47 @@
         <v>133</v>
       </c>
       <c r="F53" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G53" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H53" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I53" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J53" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="K53" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="K53" s="21" t="s">
-        <v>139</v>
-      </c>
       <c r="L53" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M53" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N53" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O53" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="P53" s="21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Q53" s="21" t="s">
         <v>115</v>
       </c>
       <c r="R53" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S53" s="21"/>
       <c r="T53" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U53" s="21" t="s">
         <v>115</v>
@@ -4283,28 +4280,28 @@
       </c>
       <c r="C61" s="20"/>
       <c r="D61" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E61" s="30" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F61" s="30"/>
       <c r="G61" s="30" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H61" s="30"/>
       <c r="I61" s="30"/>
       <c r="J61" s="30" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K61" s="30" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L61" s="30" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M61" s="30" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N61" s="30"/>
       <c r="O61" s="30"/>

</xml_diff>

<commit_message>
Rooli-excel: Til.ur.valv. saa kirj. vain omaan urakkaan
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="39460" windowHeight="22360" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25580" windowHeight="27980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="144">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -449,6 +449,9 @@
   </si>
   <si>
     <t>R*,W,päätös</t>
+  </si>
+  <si>
+    <t>R*,W,sido</t>
   </si>
 </sst>
 </file>
@@ -565,8 +568,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="61">
+  <cellStyleXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -696,7 +703,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="61">
+  <cellStyles count="65">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -727,6 +734,8 @@
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -757,6 +766,8 @@
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1093,11 +1104,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="2" ySplit="6" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomRight" activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1293,7 +1304,7 @@
         <v>133</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="F7" s="17" t="s">
         <v>135</v>
@@ -1361,7 +1372,7 @@
         <v>133</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="F8" s="17" t="s">
         <v>135</v>
@@ -1415,7 +1426,7 @@
         <v>133</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="F9" s="17" t="s">
         <v>135</v>
@@ -1463,7 +1474,7 @@
         <v>133</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="F10" s="17" t="s">
         <v>135</v>
@@ -1511,7 +1522,7 @@
         <v>133</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>135</v>
@@ -1573,7 +1584,7 @@
         <v>133</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="F12" s="17" t="s">
         <v>135</v>
@@ -2021,7 +2032,7 @@
         <v>133</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="F20" s="17" t="s">
         <v>135</v>
@@ -2087,7 +2098,7 @@
         <v>133</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="F21" s="17" t="s">
         <v>135</v>
@@ -2155,7 +2166,7 @@
         <v>133</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="F22" s="17" t="s">
         <v>135</v>
@@ -2221,7 +2232,7 @@
         <v>133</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="F23" s="17" t="s">
         <v>135</v>
@@ -2287,7 +2298,7 @@
         <v>133</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="F24" s="17" t="s">
         <v>135</v>
@@ -2349,7 +2360,7 @@
         <v>133</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="F25" s="21"/>
       <c r="G25" s="21"/>
@@ -2445,7 +2456,7 @@
         <v>133</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="F27" s="21"/>
       <c r="G27" s="21"/>
@@ -2485,7 +2496,7 @@
         <v>133</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="F28" s="21" t="s">
         <v>135</v>
@@ -2551,7 +2562,7 @@
         <v>134</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="F29" s="21" t="s">
         <v>135</v>
@@ -2613,7 +2624,7 @@
         <v>133</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="F30" s="21" t="s">
         <v>135</v>
@@ -2675,7 +2686,7 @@
         <v>134</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="F31" s="21" t="s">
         <v>135</v>
@@ -2737,7 +2748,7 @@
         <v>133</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="F32" s="21" t="s">
         <v>135</v>
@@ -2799,7 +2810,7 @@
         <v>133</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="F33" s="21" t="s">
         <v>135</v>
@@ -3984,8 +3995,8 @@
       <c r="D53" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="E53" s="21" t="s">
-        <v>133</v>
+      <c r="E53" s="17" t="s">
+        <v>138</v>
       </c>
       <c r="F53" s="21" t="s">
         <v>135</v>

</xml_diff>

<commit_message>
Korjaa ELY_Peruskayttaja oikeuksien hallinta
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25580" windowHeight="27980" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28760" windowHeight="28260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="143">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -350,9 +350,6 @@
   </si>
   <si>
     <t>ELY_Paakayttaja</t>
-  </si>
-  <si>
-    <t>hallintayksikko</t>
   </si>
   <si>
     <t>Testaus</t>
@@ -568,8 +565,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="65">
+  <cellStyleXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -703,7 +704,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="65">
+  <cellStyles count="69">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -736,6 +737,8 @@
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -768,6 +771,8 @@
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1105,10 +1110,10 @@
   <dimension ref="A1:X61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E61" sqref="E61"/>
+      <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1144,7 +1149,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D1" s="37"/>
       <c r="E1" s="37"/>
@@ -1277,7 +1282,7 @@
         <v>90</v>
       </c>
       <c r="S6" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T6" s="9" t="s">
         <v>91</v>
@@ -1289,7 +1294,7 @@
         <v>82</v>
       </c>
       <c r="W6" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:24" ht="15.75" customHeight="1">
@@ -1301,55 +1306,55 @@
       </c>
       <c r="C7" s="17"/>
       <c r="D7" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J7" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="K7" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="K7" s="17" t="s">
-        <v>138</v>
-      </c>
       <c r="L7" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M7" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N7" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O7" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P7" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q7" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R7" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S7" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T7" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U7" s="17" t="s">
         <v>17</v>
@@ -1369,31 +1374,31 @@
       </c>
       <c r="C8" s="17"/>
       <c r="D8" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G8" s="21"/>
       <c r="H8" s="21"/>
       <c r="I8" s="21"/>
       <c r="J8" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="K8" s="17" t="s">
         <v>137</v>
-      </c>
-      <c r="K8" s="17" t="s">
-        <v>138</v>
       </c>
       <c r="L8" s="21"/>
       <c r="M8" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N8" s="21"/>
       <c r="O8" s="17"/>
       <c r="P8" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q8" s="21" t="s">
         <v>17</v>
@@ -1401,7 +1406,7 @@
       <c r="R8" s="17"/>
       <c r="S8" s="17"/>
       <c r="T8" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U8" s="17" t="s">
         <v>19</v>
@@ -1411,7 +1416,7 @@
       </c>
       <c r="W8" s="17"/>
       <c r="X8" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="15.75" customHeight="1">
@@ -1423,31 +1428,31 @@
       </c>
       <c r="C9" s="17"/>
       <c r="D9" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G9" s="21"/>
       <c r="H9" s="21"/>
       <c r="I9" s="21"/>
       <c r="J9" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="K9" s="17" t="s">
         <v>137</v>
-      </c>
-      <c r="K9" s="17" t="s">
-        <v>138</v>
       </c>
       <c r="L9" s="21"/>
       <c r="M9" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N9" s="21"/>
       <c r="O9" s="17"/>
       <c r="P9" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q9" s="21" t="s">
         <v>17</v>
@@ -1455,7 +1460,7 @@
       <c r="R9" s="17"/>
       <c r="S9" s="17"/>
       <c r="T9" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U9" s="17"/>
       <c r="V9" s="17"/>
@@ -1467,35 +1472,35 @@
         <v>15</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C10" s="17"/>
       <c r="D10" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G10" s="21"/>
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
       <c r="J10" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="K10" s="17" t="s">
         <v>137</v>
-      </c>
-      <c r="K10" s="17" t="s">
-        <v>138</v>
       </c>
       <c r="L10" s="21"/>
       <c r="M10" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N10" s="21"/>
       <c r="O10" s="17"/>
       <c r="P10" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q10" s="21" t="s">
         <v>17</v>
@@ -1503,7 +1508,7 @@
       <c r="R10" s="17"/>
       <c r="S10" s="17"/>
       <c r="T10" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U10" s="17"/>
       <c r="V10" s="17"/>
@@ -1519,53 +1524,53 @@
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I11" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J11" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="K11" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="K11" s="17" t="s">
-        <v>138</v>
-      </c>
       <c r="L11" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M11" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N11" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O11" s="17"/>
       <c r="P11" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q11" s="17" t="s">
         <v>17</v>
       </c>
       <c r="R11" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S11" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T11" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U11" s="17"/>
       <c r="V11" s="17"/>
@@ -1581,53 +1586,53 @@
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J12" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="K12" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="K12" s="17" t="s">
-        <v>138</v>
-      </c>
       <c r="L12" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M12" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N12" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O12" s="17"/>
       <c r="P12" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q12" s="17" t="s">
         <v>17</v>
       </c>
       <c r="R12" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S12" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T12" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U12" s="17"/>
       <c r="V12" s="17"/>
@@ -1643,41 +1648,41 @@
       </c>
       <c r="C13" s="17"/>
       <c r="D13" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G13" s="21"/>
       <c r="H13" s="21"/>
       <c r="I13" s="21"/>
       <c r="J13" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K13" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L13" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M13" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N13" s="21"/>
       <c r="O13" s="17"/>
       <c r="P13" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q13" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R13" s="21"/>
       <c r="S13" s="17"/>
       <c r="T13" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U13" s="17"/>
       <c r="V13" s="17"/>
@@ -1693,41 +1698,41 @@
       </c>
       <c r="C14" s="17"/>
       <c r="D14" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
       <c r="I14" s="21"/>
       <c r="J14" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K14" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L14" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M14" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N14" s="21"/>
       <c r="O14" s="17"/>
       <c r="P14" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q14" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R14" s="21"/>
       <c r="S14" s="17"/>
       <c r="T14" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U14" s="17"/>
       <c r="V14" s="17"/>
@@ -1739,45 +1744,45 @@
         <v>15</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G15" s="21"/>
       <c r="H15" s="21"/>
       <c r="I15" s="21"/>
       <c r="J15" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K15" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L15" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M15" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N15" s="21"/>
       <c r="O15" s="17"/>
       <c r="P15" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q15" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R15" s="21"/>
       <c r="S15" s="17"/>
       <c r="T15" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U15" s="17"/>
       <c r="V15" s="17"/>
@@ -1793,53 +1798,53 @@
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J16" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K16" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L16" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M16" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N16" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O16" s="17"/>
       <c r="P16" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q16" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R16" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S16" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T16" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U16" s="17"/>
       <c r="V16" s="17"/>
@@ -1855,53 +1860,53 @@
       </c>
       <c r="C17" s="17"/>
       <c r="D17" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I17" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J17" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K17" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L17" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M17" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N17" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O17" s="17"/>
       <c r="P17" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q17" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R17" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S17" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T17" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U17" s="17"/>
       <c r="V17" s="17"/>
@@ -1917,33 +1922,33 @@
       </c>
       <c r="C18" s="17"/>
       <c r="D18" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G18" s="21"/>
       <c r="H18" s="21"/>
       <c r="I18" s="21"/>
       <c r="J18" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="K18" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="K18" s="17" t="s">
-        <v>138</v>
-      </c>
       <c r="L18" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M18" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N18" s="21"/>
       <c r="O18" s="17"/>
       <c r="P18" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q18" s="17" t="s">
         <v>17</v>
@@ -1951,7 +1956,7 @@
       <c r="R18" s="21"/>
       <c r="S18" s="21"/>
       <c r="T18" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U18" s="17"/>
       <c r="V18" s="17"/>
@@ -1967,53 +1972,53 @@
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I19" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J19" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K19" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L19" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M19" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N19" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O19" s="17"/>
       <c r="P19" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q19" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R19" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S19" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T19" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U19" s="17"/>
       <c r="V19" s="17"/>
@@ -2029,55 +2034,55 @@
       </c>
       <c r="C20" s="17"/>
       <c r="D20" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J20" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="K20" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="K20" s="17" t="s">
-        <v>138</v>
-      </c>
       <c r="L20" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M20" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N20" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O20" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P20" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q20" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R20" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S20" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="T20" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U20" s="17"/>
       <c r="V20" s="21" t="s">
@@ -2095,55 +2100,55 @@
       </c>
       <c r="C21" s="21"/>
       <c r="D21" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I21" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J21" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="K21" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="K21" s="17" t="s">
-        <v>138</v>
-      </c>
       <c r="L21" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M21" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N21" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O21" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P21" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q21" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R21" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S21" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="T21" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U21" s="21" t="s">
         <v>17</v>
@@ -2163,53 +2168,53 @@
       </c>
       <c r="C22" s="21"/>
       <c r="D22" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F22" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G22" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H22" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I22" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J22" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K22" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L22" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M22" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N22" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O22" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P22" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q22" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R22" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S22" s="21"/>
       <c r="T22" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U22" s="21"/>
       <c r="V22" s="21" t="s">
@@ -2217,7 +2222,7 @@
       </c>
       <c r="W22" s="21"/>
       <c r="X22" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="23" spans="1:24" ht="15.75" customHeight="1">
@@ -2229,55 +2234,55 @@
       </c>
       <c r="C23" s="21"/>
       <c r="D23" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F23" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G23" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J23" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="K23" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="K23" s="21" t="s">
-        <v>138</v>
-      </c>
       <c r="L23" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M23" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N23" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O23" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P23" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q23" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R23" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S23" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="T23" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U23" s="21"/>
       <c r="V23" s="21" t="s">
@@ -2295,53 +2300,53 @@
       </c>
       <c r="C24" s="21"/>
       <c r="D24" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F24" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G24" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H24" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I24" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J24" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="K24" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="K24" s="21" t="s">
-        <v>138</v>
-      </c>
       <c r="L24" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M24" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N24" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O24" s="21"/>
       <c r="P24" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q24" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R24" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S24" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T24" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U24" s="21"/>
       <c r="V24" s="21"/>
@@ -2357,43 +2362,43 @@
       </c>
       <c r="C25" s="21"/>
       <c r="D25" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F25" s="21"/>
       <c r="G25" s="21"/>
       <c r="H25" s="21"/>
       <c r="I25" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J25" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="K25" s="21" t="s">
         <v>137</v>
-      </c>
-      <c r="K25" s="21" t="s">
-        <v>138</v>
       </c>
       <c r="L25" s="21"/>
       <c r="M25" s="21"/>
       <c r="N25" s="21"/>
       <c r="O25" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="P25" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q25" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R25" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S25" s="27"/>
       <c r="T25" s="21"/>
       <c r="U25" s="21"/>
       <c r="V25" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="W25" s="21"/>
       <c r="X25" s="10"/>
@@ -2407,31 +2412,31 @@
       </c>
       <c r="C26" s="21"/>
       <c r="D26" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F26" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G26" s="21"/>
       <c r="H26" s="21"/>
       <c r="I26" s="21"/>
       <c r="J26" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="K26" s="21" t="s">
         <v>137</v>
-      </c>
-      <c r="K26" s="21" t="s">
-        <v>138</v>
       </c>
       <c r="L26" s="21"/>
       <c r="M26" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N26" s="21"/>
       <c r="O26" s="21"/>
       <c r="P26" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q26" s="21" t="s">
         <v>17</v>
@@ -2453,20 +2458,20 @@
       </c>
       <c r="C27" s="21"/>
       <c r="D27" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F27" s="21"/>
       <c r="G27" s="21"/>
       <c r="H27" s="21"/>
       <c r="I27" s="21"/>
       <c r="J27" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="K27" s="21" t="s">
         <v>137</v>
-      </c>
-      <c r="K27" s="21" t="s">
-        <v>138</v>
       </c>
       <c r="L27" s="21"/>
       <c r="M27" s="21"/>
@@ -2493,61 +2498,61 @@
       </c>
       <c r="C28" s="21"/>
       <c r="D28" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F28" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G28" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H28" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I28" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J28" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="K28" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="K28" s="21" t="s">
-        <v>138</v>
-      </c>
       <c r="L28" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M28" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N28" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O28" s="21"/>
       <c r="P28" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q28" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R28" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S28" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T28" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U28" s="21"/>
       <c r="V28" s="21"/>
       <c r="W28" s="21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="X28" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="29" spans="1:24" ht="15.75" customHeight="1">
@@ -2559,53 +2564,53 @@
       </c>
       <c r="C29" s="21"/>
       <c r="D29" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F29" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G29" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H29" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I29" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J29" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="K29" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="K29" s="21" t="s">
-        <v>138</v>
-      </c>
       <c r="L29" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M29" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N29" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O29" s="21"/>
       <c r="P29" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q29" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R29" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S29" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T29" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U29" s="21"/>
       <c r="V29" s="21"/>
@@ -2621,53 +2626,53 @@
       </c>
       <c r="C30" s="21"/>
       <c r="D30" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F30" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G30" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H30" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I30" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J30" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K30" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L30" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M30" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N30" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O30" s="21"/>
       <c r="P30" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q30" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R30" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S30" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T30" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U30" s="21"/>
       <c r="V30" s="21"/>
@@ -2683,53 +2688,53 @@
       </c>
       <c r="C31" s="21"/>
       <c r="D31" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F31" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G31" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H31" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I31" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J31" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="K31" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="K31" s="21" t="s">
-        <v>138</v>
-      </c>
       <c r="L31" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M31" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N31" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O31" s="21"/>
       <c r="P31" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q31" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R31" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S31" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T31" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U31" s="21"/>
       <c r="V31" s="21"/>
@@ -2745,53 +2750,53 @@
       </c>
       <c r="C32" s="21"/>
       <c r="D32" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F32" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G32" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H32" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I32" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J32" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="K32" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="K32" s="21" t="s">
-        <v>138</v>
-      </c>
       <c r="L32" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M32" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N32" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O32" s="21"/>
       <c r="P32" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q32" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R32" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S32" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T32" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U32" s="21"/>
       <c r="V32" s="21"/>
@@ -2803,59 +2808,59 @@
         <v>15</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C33" s="21"/>
       <c r="D33" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F33" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G33" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H33" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I33" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J33" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K33" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L33" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M33" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N33" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O33" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P33" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q33" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R33" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S33" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="T33" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U33" s="21" t="s">
         <v>17</v>
@@ -2871,35 +2876,35 @@
         <v>43</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C34" s="21"/>
       <c r="D34" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F34" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G34" s="21"/>
       <c r="H34" s="21"/>
       <c r="I34" s="21"/>
       <c r="J34" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K34" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L34" s="21"/>
       <c r="M34" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N34" s="21"/>
       <c r="O34" s="21"/>
       <c r="P34" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q34" s="21" t="s">
         <v>17</v>
@@ -2921,13 +2926,13 @@
       </c>
       <c r="C35" s="21"/>
       <c r="D35" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F35" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G35" s="21" t="s">
         <v>19</v>
@@ -2935,19 +2940,19 @@
       <c r="H35" s="21"/>
       <c r="I35" s="21"/>
       <c r="J35" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K35" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L35" s="21"/>
       <c r="M35" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N35" s="21"/>
       <c r="O35" s="21"/>
       <c r="P35" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q35" s="21" t="s">
         <v>17</v>
@@ -2955,7 +2960,7 @@
       <c r="R35" s="21"/>
       <c r="S35" s="21"/>
       <c r="T35" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U35" s="21"/>
       <c r="V35" s="21"/>
@@ -2971,55 +2976,55 @@
       </c>
       <c r="C36" s="21"/>
       <c r="D36" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F36" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G36" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H36" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I36" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J36" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K36" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L36" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M36" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N36" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O36" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P36" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q36" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R36" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S36" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T36" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U36" s="21"/>
       <c r="V36" s="21" t="s">
@@ -3037,55 +3042,55 @@
       </c>
       <c r="C37" s="21"/>
       <c r="D37" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F37" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G37" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H37" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I37" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J37" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K37" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L37" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M37" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N37" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O37" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P37" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q37" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R37" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S37" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T37" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U37" s="21"/>
       <c r="V37" s="21" t="s">
@@ -3103,55 +3108,55 @@
       </c>
       <c r="C38" s="21"/>
       <c r="D38" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E38" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F38" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G38" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H38" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I38" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J38" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K38" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L38" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M38" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N38" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O38" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P38" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q38" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R38" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S38" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T38" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U38" s="21"/>
       <c r="V38" s="21" t="s">
@@ -3169,55 +3174,55 @@
       </c>
       <c r="C39" s="21"/>
       <c r="D39" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E39" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F39" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G39" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H39" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I39" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J39" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K39" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L39" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M39" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N39" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O39" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P39" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q39" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R39" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S39" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T39" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U39" s="21"/>
       <c r="V39" s="21" t="s">
@@ -3235,55 +3240,55 @@
       </c>
       <c r="C40" s="21"/>
       <c r="D40" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E40" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F40" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G40" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H40" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I40" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J40" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K40" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L40" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M40" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N40" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O40" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P40" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q40" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R40" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S40" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T40" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U40" s="21"/>
       <c r="V40" s="21" t="s">
@@ -3301,47 +3306,47 @@
       </c>
       <c r="C41" s="21"/>
       <c r="D41" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E41" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F41" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G41" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H41" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I41" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J41" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K41" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L41" s="21"/>
       <c r="M41" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N41" s="21"/>
       <c r="O41" s="21"/>
       <c r="P41" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q41" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R41" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S41" s="21"/>
       <c r="T41" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U41" s="21"/>
       <c r="V41" s="21" t="s">
@@ -3359,55 +3364,55 @@
       </c>
       <c r="C42" s="21"/>
       <c r="D42" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E42" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F42" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G42" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H42" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I42" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J42" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K42" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L42" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M42" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N42" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O42" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P42" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q42" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R42" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S42" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T42" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U42" s="21"/>
       <c r="V42" s="21" t="s">
@@ -3425,31 +3430,31 @@
       </c>
       <c r="C43" s="21"/>
       <c r="D43" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E43" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F43" s="21"/>
       <c r="G43" s="21"/>
       <c r="H43" s="21"/>
       <c r="I43" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J43" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K43" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L43" s="21"/>
       <c r="M43" s="21"/>
       <c r="N43" s="21"/>
       <c r="O43" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P43" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q43" s="21" t="s">
         <v>17</v>
@@ -3457,7 +3462,7 @@
       <c r="R43" s="21"/>
       <c r="S43" s="21"/>
       <c r="T43" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U43" s="21"/>
       <c r="V43" s="21" t="s">
@@ -3475,13 +3480,13 @@
       </c>
       <c r="C44" s="21"/>
       <c r="D44" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E44" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F44" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G44" s="21"/>
       <c r="H44" s="21" t="s">
@@ -3489,21 +3494,21 @@
       </c>
       <c r="I44" s="21"/>
       <c r="J44" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K44" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L44" s="21"/>
       <c r="M44" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N44" s="21" t="s">
         <v>19</v>
       </c>
       <c r="O44" s="21"/>
       <c r="P44" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q44" s="21" t="s">
         <v>17</v>
@@ -3525,31 +3530,31 @@
       </c>
       <c r="C45" s="21"/>
       <c r="D45" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E45" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F45" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G45" s="21"/>
       <c r="H45" s="21"/>
       <c r="I45" s="21"/>
       <c r="J45" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K45" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L45" s="21"/>
       <c r="M45" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N45" s="21"/>
       <c r="O45" s="21"/>
       <c r="P45" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q45" s="21" t="s">
         <v>17</v>
@@ -3557,7 +3562,7 @@
       <c r="R45" s="21"/>
       <c r="S45" s="21"/>
       <c r="T45" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U45" s="21"/>
       <c r="V45" s="21"/>
@@ -3573,31 +3578,31 @@
       </c>
       <c r="C46" s="21"/>
       <c r="D46" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E46" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F46" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G46" s="21"/>
       <c r="H46" s="21"/>
       <c r="I46" s="21"/>
       <c r="J46" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K46" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L46" s="21"/>
       <c r="M46" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N46" s="21"/>
       <c r="O46" s="21"/>
       <c r="P46" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q46" s="21" t="s">
         <v>17</v>
@@ -3605,7 +3610,7 @@
       <c r="R46" s="21"/>
       <c r="S46" s="21"/>
       <c r="T46" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U46" s="21"/>
       <c r="V46" s="21"/>
@@ -3621,31 +3626,31 @@
       </c>
       <c r="C47" s="21"/>
       <c r="D47" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E47" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F47" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G47" s="21"/>
       <c r="H47" s="21"/>
       <c r="I47" s="21"/>
       <c r="J47" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K47" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L47" s="21"/>
       <c r="M47" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N47" s="21"/>
       <c r="O47" s="21"/>
       <c r="P47" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q47" s="21" t="s">
         <v>17</v>
@@ -3653,7 +3658,7 @@
       <c r="R47" s="21"/>
       <c r="S47" s="21"/>
       <c r="T47" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U47" s="21"/>
       <c r="V47" s="21"/>
@@ -3665,51 +3670,51 @@
         <v>43</v>
       </c>
       <c r="B48" s="26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C48" s="21"/>
       <c r="D48" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E48" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F48" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G48" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H48" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I48" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J48" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K48" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L48" s="21"/>
       <c r="M48" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N48" s="21"/>
       <c r="O48" s="21"/>
       <c r="P48" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q48" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R48" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S48" s="21"/>
       <c r="T48" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U48" s="21"/>
       <c r="V48" s="21" t="s">
@@ -3727,55 +3732,55 @@
       </c>
       <c r="C49" s="21"/>
       <c r="D49" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E49" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F49" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G49" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H49" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I49" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J49" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K49" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L49" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M49" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N49" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O49" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P49" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q49" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R49" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S49" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T49" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U49" s="21"/>
       <c r="V49" s="21" t="s">
@@ -3789,53 +3794,53 @@
         <v>43</v>
       </c>
       <c r="B50" s="26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C50" s="21"/>
       <c r="D50" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E50" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F50" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G50" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H50" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I50" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J50" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K50" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L50" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M50" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N50" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O50" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P50" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q50" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R50" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S50" s="21" t="s">
         <v>17</v>
@@ -3855,55 +3860,55 @@
       </c>
       <c r="C51" s="21"/>
       <c r="D51" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E51" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F51" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G51" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H51" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I51" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J51" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K51" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L51" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M51" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N51" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O51" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P51" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q51" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R51" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S51" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T51" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U51" s="21" t="s">
         <v>17</v>
@@ -3925,55 +3930,55 @@
       </c>
       <c r="C52" s="21"/>
       <c r="D52" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E52" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F52" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G52" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H52" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I52" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J52" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K52" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L52" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M52" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N52" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O52" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P52" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q52" s="21" t="s">
         <v>17</v>
       </c>
       <c r="R52" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S52" s="21" t="s">
         <v>17</v>
       </c>
       <c r="T52" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U52" s="21" t="s">
         <v>17</v>
@@ -3993,56 +3998,56 @@
       </c>
       <c r="C53" s="21"/>
       <c r="D53" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E53" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F53" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G53" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H53" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I53" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J53" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="K53" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="K53" s="21" t="s">
-        <v>138</v>
-      </c>
       <c r="L53" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M53" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N53" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O53" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P53" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q53" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R53" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S53" s="21"/>
       <c r="T53" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U53" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="V53" s="21" t="s">
         <v>17</v>
@@ -4059,7 +4064,7 @@
       </c>
       <c r="C54" s="19"/>
       <c r="D54" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E54" s="19"/>
       <c r="F54" s="19"/>
@@ -4093,7 +4098,7 @@
       </c>
       <c r="C55" s="17"/>
       <c r="D55" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E55" s="17"/>
       <c r="F55" s="17" t="s">
@@ -4136,7 +4141,7 @@
       </c>
       <c r="C56" s="17"/>
       <c r="D56" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E56" s="17"/>
       <c r="F56" s="17"/>
@@ -4167,7 +4172,7 @@
       </c>
       <c r="C57" s="17"/>
       <c r="D57" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E57" s="17"/>
       <c r="F57" s="17"/>
@@ -4198,7 +4203,7 @@
       </c>
       <c r="C58" s="17"/>
       <c r="D58" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E58" s="17"/>
       <c r="F58" s="17"/>
@@ -4225,11 +4230,11 @@
         <v>63</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C59" s="17"/>
       <c r="D59" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E59" s="17"/>
       <c r="F59" s="17"/>
@@ -4253,14 +4258,14 @@
     </row>
     <row r="60" spans="1:24" ht="15.75" customHeight="1">
       <c r="A60" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B60" s="16" t="s">
         <v>111</v>
-      </c>
-      <c r="B60" s="16" t="s">
-        <v>112</v>
       </c>
       <c r="C60" s="20"/>
       <c r="D60" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E60" s="20"/>
       <c r="F60" s="20"/>
@@ -4284,35 +4289,35 @@
     </row>
     <row r="61" spans="1:24" ht="15.75" customHeight="1">
       <c r="A61" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B61" s="16" t="s">
         <v>125</v>
-      </c>
-      <c r="B61" s="16" t="s">
-        <v>126</v>
       </c>
       <c r="C61" s="20"/>
       <c r="D61" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E61" s="30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F61" s="30"/>
       <c r="G61" s="30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H61" s="30"/>
       <c r="I61" s="30"/>
       <c r="J61" s="30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K61" s="30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L61" s="30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M61" s="30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N61" s="30"/>
       <c r="O61" s="30"/>
@@ -4349,7 +4354,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -4374,7 +4379,7 @@
         <v>94</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15">
@@ -4486,9 +4491,7 @@
       <c r="C9" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="24" t="s">
-        <v>110</v>
-      </c>
+      <c r="D9" s="24"/>
       <c r="E9" s="24"/>
     </row>
     <row r="10" spans="1:5" ht="15">
@@ -4501,9 +4504,7 @@
       <c r="C10" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="24" t="s">
-        <v>110</v>
-      </c>
+      <c r="D10" s="24"/>
       <c r="E10" s="24"/>
     </row>
     <row r="11" spans="1:5" ht="15">
@@ -4516,9 +4517,7 @@
       <c r="C11" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="24" t="s">
-        <v>110</v>
-      </c>
+      <c r="D11" s="24"/>
       <c r="E11" s="24"/>
     </row>
     <row r="12" spans="1:5" ht="15">
@@ -4598,7 +4597,7 @@
     </row>
     <row r="17" spans="1:5" ht="15">
       <c r="A17" s="23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B17" s="23" t="s">
         <v>11</v>
@@ -4658,10 +4657,10 @@
     </row>
     <row r="21" spans="1:5" ht="15">
       <c r="A21" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="B21" s="23" t="s">
         <v>118</v>
-      </c>
-      <c r="B21" s="23" t="s">
-        <v>119</v>
       </c>
       <c r="C21" s="23" t="s">
         <v>4</v>
@@ -4670,11 +4669,12 @@
         <v>95</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Korjaa urakoitsijan ur. laadunvast oikeudet
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="14960" tabRatio="500"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="142">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -440,9 +440,6 @@
   </si>
   <si>
     <t>R+,W+</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Urakan laadunvalvoja</t>
   </si>
   <si>
     <t>R*,W,päätös</t>
@@ -1118,10 +1115,10 @@
   <dimension ref="A1:X61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="E38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="O7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="L48" sqref="L48"/>
+      <selection pane="bottomRight" activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1290,7 +1287,7 @@
         <v>90</v>
       </c>
       <c r="S6" s="9" t="s">
-        <v>140</v>
+        <v>92</v>
       </c>
       <c r="T6" s="9" t="s">
         <v>91</v>
@@ -2189,7 +2186,7 @@
         <v>136</v>
       </c>
       <c r="K22" s="21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L22" s="21" t="s">
         <v>134</v>
@@ -2567,7 +2564,7 @@
         <v>133</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F29" s="21" t="s">
         <v>134</v>
@@ -2641,7 +2638,7 @@
         <v>136</v>
       </c>
       <c r="K30" s="21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L30" s="21"/>
       <c r="M30" s="21" t="s">
@@ -2683,7 +2680,7 @@
         <v>133</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F31" s="21" t="s">
         <v>134</v>
@@ -2817,7 +2814,7 @@
         <v>136</v>
       </c>
       <c r="K33" s="21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L33" s="21" t="s">
         <v>136</v>
@@ -4338,7 +4335,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Korjaa Rooli-exceliin tilaajan turv.vastaavan osapuoli
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="14960" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="26580" windowHeight="27760" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -562,8 +562,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="73">
+  <cellStyleXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -705,7 +709,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="73">
+  <cellStyles count="77">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -742,6 +746,8 @@
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -778,6 +784,8 @@
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1114,11 +1122,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="O7" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="S6" sqref="S6"/>
+      <selection pane="bottomRight" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -4334,8 +4342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -4440,7 +4448,7 @@
         <v>81</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D7" s="24" t="s">
         <v>95</v>

</xml_diff>

<commit_message>
Korjaa päätöksen antamisen oikeustarkistus
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26812"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarihan/Desktop/Harja/harja/resources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="26580" windowHeight="27760" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="8780" yWindow="460" windowWidth="26580" windowHeight="27040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -1122,14 +1127,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X61"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="I25" sqref="I25"/>
+      <selection pane="bottomRight" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.5" bestFit="1" customWidth="1"/>
@@ -1156,7 +1161,7 @@
     <col min="24" max="24" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" customHeight="1">
+    <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1176,7 +1181,7 @@
       <c r="M1" s="37"/>
       <c r="N1" s="37"/>
     </row>
-    <row r="2" spans="1:24" ht="15.75" customHeight="1">
+    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="39" t="s">
@@ -1194,7 +1199,7 @@
       <c r="M2" s="37"/>
       <c r="N2" s="37"/>
     </row>
-    <row r="3" spans="1:24" ht="15.75" customHeight="1">
+    <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -1209,10 +1214,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="15.75" customHeight="1">
+    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:24" ht="15.75" customHeight="1">
+    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C5" s="38" t="s">
         <v>6</v>
       </c>
@@ -1241,7 +1246,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="15.75" customHeight="1">
+    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -1310,7 +1315,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="15.75" customHeight="1">
+    <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="16" t="s">
         <v>15</v>
       </c>
@@ -1378,7 +1383,7 @@
       <c r="W7" s="17"/>
       <c r="X7" s="10"/>
     </row>
-    <row r="8" spans="1:24" ht="15.75" customHeight="1">
+    <row r="8" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="16" t="s">
         <v>15</v>
       </c>
@@ -1432,7 +1437,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="15.75" customHeight="1">
+    <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="16" t="s">
         <v>15</v>
       </c>
@@ -1480,7 +1485,7 @@
       <c r="W9" s="17"/>
       <c r="X9" s="10"/>
     </row>
-    <row r="10" spans="1:24" ht="15.75" customHeight="1">
+    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="16" t="s">
         <v>15</v>
       </c>
@@ -1528,7 +1533,7 @@
       <c r="W10" s="17"/>
       <c r="X10" s="10"/>
     </row>
-    <row r="11" spans="1:24" ht="15.75" customHeight="1">
+    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="16" t="s">
         <v>15</v>
       </c>
@@ -1590,7 +1595,7 @@
       <c r="W11" s="17"/>
       <c r="X11" s="10"/>
     </row>
-    <row r="12" spans="1:24" ht="15.75" customHeight="1">
+    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="16" t="s">
         <v>15</v>
       </c>
@@ -1652,7 +1657,7 @@
       <c r="W12" s="17"/>
       <c r="X12" s="10"/>
     </row>
-    <row r="13" spans="1:24" ht="15.75" customHeight="1">
+    <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="16" t="s">
         <v>15</v>
       </c>
@@ -1700,7 +1705,7 @@
       <c r="W13" s="17"/>
       <c r="X13" s="10"/>
     </row>
-    <row r="14" spans="1:24" ht="15.75" customHeight="1">
+    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="16" t="s">
         <v>15</v>
       </c>
@@ -1748,7 +1753,7 @@
       <c r="W14" s="17"/>
       <c r="X14" s="10"/>
     </row>
-    <row r="15" spans="1:24" ht="15.75" customHeight="1">
+    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="16" t="s">
         <v>15</v>
       </c>
@@ -1796,7 +1801,7 @@
       <c r="W15" s="17"/>
       <c r="X15" s="10"/>
     </row>
-    <row r="16" spans="1:24" ht="15.75" customHeight="1">
+    <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="16" t="s">
         <v>15</v>
       </c>
@@ -1858,7 +1863,7 @@
       <c r="W16" s="17"/>
       <c r="X16" s="10"/>
     </row>
-    <row r="17" spans="1:24" ht="15.75" customHeight="1">
+    <row r="17" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="16" t="s">
         <v>15</v>
       </c>
@@ -1920,7 +1925,7 @@
       <c r="W17" s="17"/>
       <c r="X17" s="10"/>
     </row>
-    <row r="18" spans="1:24" ht="15.75" customHeight="1">
+    <row r="18" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="16" t="s">
         <v>15</v>
       </c>
@@ -1968,7 +1973,7 @@
       <c r="W18" s="17"/>
       <c r="X18" s="10"/>
     </row>
-    <row r="19" spans="1:24" ht="15.75" customHeight="1">
+    <row r="19" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="16" t="s">
         <v>15</v>
       </c>
@@ -2030,7 +2035,7 @@
       <c r="W19" s="17"/>
       <c r="X19" s="10"/>
     </row>
-    <row r="20" spans="1:24" ht="15.75" customHeight="1">
+    <row r="20" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="16" t="s">
         <v>15</v>
       </c>
@@ -2096,7 +2101,7 @@
       <c r="W20" s="17"/>
       <c r="X20" s="10"/>
     </row>
-    <row r="21" spans="1:24" ht="15.75" customHeight="1">
+    <row r="21" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="26" t="s">
         <v>15</v>
       </c>
@@ -2164,7 +2169,7 @@
       <c r="W21" s="21"/>
       <c r="X21" s="10"/>
     </row>
-    <row r="22" spans="1:24" ht="15.75" customHeight="1">
+    <row r="22" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="26" t="s">
         <v>15</v>
       </c>
@@ -2230,7 +2235,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="23" spans="1:24" ht="15.75" customHeight="1">
+    <row r="23" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="26" t="s">
         <v>15</v>
       </c>
@@ -2296,7 +2301,7 @@
       <c r="W23" s="21"/>
       <c r="X23" s="10"/>
     </row>
-    <row r="24" spans="1:24" ht="15.75" customHeight="1">
+    <row r="24" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="26" t="s">
         <v>15</v>
       </c>
@@ -2358,7 +2363,7 @@
       <c r="W24" s="21"/>
       <c r="X24" s="10"/>
     </row>
-    <row r="25" spans="1:24" ht="15.75" customHeight="1">
+    <row r="25" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="26" t="s">
         <v>15</v>
       </c>
@@ -2408,7 +2413,7 @@
       <c r="W25" s="21"/>
       <c r="X25" s="10"/>
     </row>
-    <row r="26" spans="1:24" ht="15.75" customHeight="1">
+    <row r="26" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="26" t="s">
         <v>15</v>
       </c>
@@ -2454,7 +2459,7 @@
       <c r="W26" s="21"/>
       <c r="X26" s="10"/>
     </row>
-    <row r="27" spans="1:24" ht="15.75" customHeight="1">
+    <row r="27" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="26" t="s">
         <v>15</v>
       </c>
@@ -2494,7 +2499,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:24" ht="15.75" customHeight="1">
+    <row r="28" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="26" t="s">
         <v>15</v>
       </c>
@@ -2560,7 +2565,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="29" spans="1:24" ht="15.75" customHeight="1">
+    <row r="29" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="26" t="s">
         <v>15</v>
       </c>
@@ -2618,7 +2623,7 @@
       <c r="W29" s="21"/>
       <c r="X29" s="10"/>
     </row>
-    <row r="30" spans="1:24" ht="15.75" customHeight="1">
+    <row r="30" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="26" t="s">
         <v>15</v>
       </c>
@@ -2626,8 +2631,8 @@
         <v>40</v>
       </c>
       <c r="C30" s="21"/>
-      <c r="D30" s="17" t="s">
-        <v>132</v>
+      <c r="D30" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="E30" s="17" t="s">
         <v>137</v>
@@ -2676,7 +2681,7 @@
       <c r="W30" s="21"/>
       <c r="X30" s="10"/>
     </row>
-    <row r="31" spans="1:24" ht="15.75" customHeight="1">
+    <row r="31" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="26" t="s">
         <v>15</v>
       </c>
@@ -2734,7 +2739,7 @@
       <c r="W31" s="21"/>
       <c r="X31" s="10"/>
     </row>
-    <row r="32" spans="1:24" ht="15.75" customHeight="1">
+    <row r="32" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="26" t="s">
         <v>15</v>
       </c>
@@ -2792,7 +2797,7 @@
       <c r="W32" s="21"/>
       <c r="X32" s="10"/>
     </row>
-    <row r="33" spans="1:24" s="13" customFormat="1" ht="15.75" customHeight="1">
+    <row r="33" spans="1:24" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="26" t="s">
         <v>15</v>
       </c>
@@ -2860,7 +2865,7 @@
       <c r="W33" s="21"/>
       <c r="X33" s="12"/>
     </row>
-    <row r="34" spans="1:24" s="32" customFormat="1" ht="15.75" customHeight="1">
+    <row r="34" spans="1:24" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="26" t="s">
         <v>43</v>
       </c>
@@ -2906,7 +2911,7 @@
       <c r="W34" s="21"/>
       <c r="X34" s="31"/>
     </row>
-    <row r="35" spans="1:24" ht="15.75" customHeight="1">
+    <row r="35" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="26" t="s">
         <v>43</v>
       </c>
@@ -2956,7 +2961,7 @@
       <c r="W35" s="21"/>
       <c r="X35" s="10"/>
     </row>
-    <row r="36" spans="1:24" ht="15.75" customHeight="1">
+    <row r="36" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="26" t="s">
         <v>43</v>
       </c>
@@ -3022,7 +3027,7 @@
       <c r="W36" s="21"/>
       <c r="X36" s="10"/>
     </row>
-    <row r="37" spans="1:24" ht="15.75" customHeight="1">
+    <row r="37" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="26" t="s">
         <v>43</v>
       </c>
@@ -3088,7 +3093,7 @@
       <c r="W37" s="21"/>
       <c r="X37" s="10"/>
     </row>
-    <row r="38" spans="1:24" ht="15.75" customHeight="1">
+    <row r="38" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="26" t="s">
         <v>43</v>
       </c>
@@ -3154,7 +3159,7 @@
       <c r="W38" s="21"/>
       <c r="X38" s="10"/>
     </row>
-    <row r="39" spans="1:24" ht="15.75" customHeight="1">
+    <row r="39" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="26" t="s">
         <v>43</v>
       </c>
@@ -3220,7 +3225,7 @@
       <c r="W39" s="21"/>
       <c r="X39" s="10"/>
     </row>
-    <row r="40" spans="1:24" ht="15.75" customHeight="1">
+    <row r="40" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="26" t="s">
         <v>43</v>
       </c>
@@ -3286,7 +3291,7 @@
       <c r="W40" s="21"/>
       <c r="X40" s="10"/>
     </row>
-    <row r="41" spans="1:24" ht="15.75" customHeight="1">
+    <row r="41" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="26" t="s">
         <v>43</v>
       </c>
@@ -3346,7 +3351,7 @@
       <c r="W41" s="21"/>
       <c r="X41" s="10"/>
     </row>
-    <row r="42" spans="1:24" ht="15.75" customHeight="1">
+    <row r="42" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="26" t="s">
         <v>43</v>
       </c>
@@ -3412,7 +3417,7 @@
       <c r="W42" s="21"/>
       <c r="X42" s="10"/>
     </row>
-    <row r="43" spans="1:24" ht="15.75" customHeight="1">
+    <row r="43" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="26" t="s">
         <v>43</v>
       </c>
@@ -3462,7 +3467,7 @@
       <c r="W43" s="21"/>
       <c r="X43" s="10"/>
     </row>
-    <row r="44" spans="1:24" ht="15.75" customHeight="1">
+    <row r="44" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="26" t="s">
         <v>43</v>
       </c>
@@ -3512,7 +3517,7 @@
       <c r="W44" s="21"/>
       <c r="X44" s="10"/>
     </row>
-    <row r="45" spans="1:24" ht="15.75" customHeight="1">
+    <row r="45" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="26" t="s">
         <v>43</v>
       </c>
@@ -3560,7 +3565,7 @@
       <c r="W45" s="21"/>
       <c r="X45" s="10"/>
     </row>
-    <row r="46" spans="1:24" ht="15.75" customHeight="1">
+    <row r="46" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="26" t="s">
         <v>43</v>
       </c>
@@ -3608,7 +3613,7 @@
       <c r="W46" s="21"/>
       <c r="X46" s="10"/>
     </row>
-    <row r="47" spans="1:24" ht="15.75" customHeight="1">
+    <row r="47" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="26" t="s">
         <v>43</v>
       </c>
@@ -3656,7 +3661,7 @@
       <c r="W47" s="21"/>
       <c r="X47" s="10"/>
     </row>
-    <row r="48" spans="1:24" s="29" customFormat="1" ht="15.75" customHeight="1">
+    <row r="48" spans="1:24" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="26" t="s">
         <v>43</v>
       </c>
@@ -3712,7 +3717,7 @@
       <c r="W48" s="21"/>
       <c r="X48" s="28"/>
     </row>
-    <row r="49" spans="1:24" ht="15.75" customHeight="1">
+    <row r="49" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="26" t="s">
         <v>43</v>
       </c>
@@ -3778,7 +3783,7 @@
       <c r="W49" s="21"/>
       <c r="X49" s="10"/>
     </row>
-    <row r="50" spans="1:24" s="35" customFormat="1" ht="15.75" customHeight="1">
+    <row r="50" spans="1:24" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="26" t="s">
         <v>43</v>
       </c>
@@ -3840,7 +3845,7 @@
       <c r="W50" s="21"/>
       <c r="X50" s="34"/>
     </row>
-    <row r="51" spans="1:24" ht="15.75" customHeight="1">
+    <row r="51" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="26" t="s">
         <v>58</v>
       </c>
@@ -3910,7 +3915,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="1:24" ht="15.75" customHeight="1">
+    <row r="52" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="26" t="s">
         <v>58</v>
       </c>
@@ -3978,7 +3983,7 @@
       <c r="W52" s="21"/>
       <c r="X52" s="37"/>
     </row>
-    <row r="53" spans="1:24" ht="15.75" customHeight="1">
+    <row r="53" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="26" t="s">
         <v>62</v>
       </c>
@@ -4044,7 +4049,7 @@
       <c r="W53" s="21"/>
       <c r="X53" s="10"/>
     </row>
-    <row r="54" spans="1:24" s="15" customFormat="1" ht="15.75" customHeight="1">
+    <row r="54" spans="1:24" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="18" t="s">
         <v>63</v>
       </c>
@@ -4078,7 +4083,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="55" spans="1:24" ht="15.75" customHeight="1">
+    <row r="55" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="16" t="s">
         <v>63</v>
       </c>
@@ -4121,7 +4126,7 @@
       <c r="V55" s="17"/>
       <c r="W55" s="17"/>
     </row>
-    <row r="56" spans="1:24" ht="15.75" customHeight="1">
+    <row r="56" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="16" t="s">
         <v>63</v>
       </c>
@@ -4152,7 +4157,7 @@
       <c r="V56" s="17"/>
       <c r="W56" s="17"/>
     </row>
-    <row r="57" spans="1:24" ht="15.75" customHeight="1">
+    <row r="57" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="16" t="s">
         <v>63</v>
       </c>
@@ -4183,7 +4188,7 @@
       <c r="V57" s="17"/>
       <c r="W57" s="17"/>
     </row>
-    <row r="58" spans="1:24" ht="15.75" customHeight="1">
+    <row r="58" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="16" t="s">
         <v>63</v>
       </c>
@@ -4214,7 +4219,7 @@
       <c r="V58" s="17"/>
       <c r="W58" s="17"/>
     </row>
-    <row r="59" spans="1:24" s="33" customFormat="1" ht="15.75" customHeight="1">
+    <row r="59" spans="1:24" s="33" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="16" t="s">
         <v>63</v>
       </c>
@@ -4245,7 +4250,7 @@
       <c r="V59" s="17"/>
       <c r="W59" s="17"/>
     </row>
-    <row r="60" spans="1:24" ht="15.75" customHeight="1">
+    <row r="60" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="16" t="s">
         <v>110</v>
       </c>
@@ -4276,7 +4281,7 @@
       <c r="V60" s="20"/>
       <c r="W60" s="20"/>
     </row>
-    <row r="61" spans="1:24" ht="15.75" customHeight="1">
+    <row r="61" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="16" t="s">
         <v>124</v>
       </c>
@@ -4330,11 +4335,6 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4342,11 +4342,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="29.6640625" customWidth="1"/>
     <col min="2" max="2" width="28.1640625" customWidth="1"/>
@@ -4354,7 +4354,7 @@
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
         <v>70</v>
       </c>
@@ -4371,7 +4371,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15">
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
         <v>73</v>
       </c>
@@ -4384,7 +4384,7 @@
       <c r="D2" s="24"/>
       <c r="E2" s="24"/>
     </row>
-    <row r="3" spans="1:5" ht="15">
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
         <v>75</v>
       </c>
@@ -4397,7 +4397,7 @@
       <c r="D3" s="24"/>
       <c r="E3" s="24"/>
     </row>
-    <row r="4" spans="1:5" ht="15">
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
         <v>77</v>
       </c>
@@ -4410,7 +4410,7 @@
       <c r="D4" s="24"/>
       <c r="E4" s="24"/>
     </row>
-    <row r="5" spans="1:5" ht="15">
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
         <v>97</v>
       </c>
@@ -4425,7 +4425,7 @@
       </c>
       <c r="E5" s="24"/>
     </row>
-    <row r="6" spans="1:5" ht="15">
+    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
         <v>98</v>
       </c>
@@ -4440,7 +4440,7 @@
       </c>
       <c r="E6" s="24"/>
     </row>
-    <row r="7" spans="1:5" ht="15">
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
         <v>99</v>
       </c>
@@ -4455,7 +4455,7 @@
       </c>
       <c r="E7" s="24"/>
     </row>
-    <row r="8" spans="1:5" ht="15">
+    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
         <v>100</v>
       </c>
@@ -4470,7 +4470,7 @@
       </c>
       <c r="E8" s="24"/>
     </row>
-    <row r="9" spans="1:5" ht="15">
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
         <v>109</v>
       </c>
@@ -4483,7 +4483,7 @@
       <c r="D9" s="24"/>
       <c r="E9" s="24"/>
     </row>
-    <row r="10" spans="1:5" ht="15">
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
         <v>108</v>
       </c>
@@ -4496,7 +4496,7 @@
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
     </row>
-    <row r="11" spans="1:5" ht="15">
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
         <v>107</v>
       </c>
@@ -4509,7 +4509,7 @@
       <c r="D11" s="24"/>
       <c r="E11" s="24"/>
     </row>
-    <row r="12" spans="1:5" ht="15">
+    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
         <v>101</v>
       </c>
@@ -4524,7 +4524,7 @@
       </c>
       <c r="E12" s="24"/>
     </row>
-    <row r="13" spans="1:5" ht="15">
+    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
         <v>106</v>
       </c>
@@ -4539,7 +4539,7 @@
       </c>
       <c r="E13" s="24"/>
     </row>
-    <row r="14" spans="1:5" ht="15">
+    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
         <v>102</v>
       </c>
@@ -4554,7 +4554,7 @@
       </c>
       <c r="E14" s="24"/>
     </row>
-    <row r="15" spans="1:5" ht="15">
+    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
         <v>103</v>
       </c>
@@ -4569,7 +4569,7 @@
       </c>
       <c r="E15" s="24"/>
     </row>
-    <row r="16" spans="1:5" ht="15">
+    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
         <v>104</v>
       </c>
@@ -4584,7 +4584,7 @@
       </c>
       <c r="E16" s="24"/>
     </row>
-    <row r="17" spans="1:5" ht="15">
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
         <v>127</v>
       </c>
@@ -4599,7 +4599,7 @@
       </c>
       <c r="E17" s="24"/>
     </row>
-    <row r="18" spans="1:5" ht="15">
+    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
         <v>12</v>
       </c>
@@ -4614,7 +4614,7 @@
       </c>
       <c r="E18" s="24"/>
     </row>
-    <row r="19" spans="1:5" ht="15">
+    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
         <v>13</v>
       </c>
@@ -4629,7 +4629,7 @@
       </c>
       <c r="E19" s="24"/>
     </row>
-    <row r="20" spans="1:5" ht="15">
+    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
         <v>105</v>
       </c>
@@ -4644,7 +4644,7 @@
       </c>
       <c r="E20" s="24"/>
     </row>
-    <row r="21" spans="1:5" ht="15">
+    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
         <v>117</v>
       </c>
@@ -4664,10 +4664,5 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Anna JVH:lle oikeus käsitellä päällystys-/paikkauslomake
</commit_message>
<xml_diff>
--- a/resources/roolit.xlsx
+++ b/resources/roolit.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26812"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarihan/Desktop/Harja/harja/resources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="26580" windowHeight="27760" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="8780" yWindow="460" windowWidth="26580" windowHeight="27040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Oikeudet" sheetId="1" r:id="rId1"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="143">
   <si>
     <t xml:space="preserve">Rooleissa: </t>
   </si>
@@ -446,6 +451,9 @@
   </si>
   <si>
     <t>R*,W,sido</t>
+  </si>
+  <si>
+    <t>R*,W*,päätös</t>
   </si>
 </sst>
 </file>
@@ -1122,19 +1130,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X61"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="I25" sqref="I25"/>
+      <selection pane="bottomRight" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" customWidth="1"/>
+    <col min="4" max="4" width="12.5" customWidth="1"/>
     <col min="5" max="5" width="11.5" customWidth="1"/>
     <col min="6" max="6" width="10.1640625" customWidth="1"/>
     <col min="7" max="7" width="9.83203125" customWidth="1"/>
@@ -1156,7 +1164,7 @@
     <col min="24" max="24" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" customHeight="1">
+    <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1176,7 +1184,7 @@
       <c r="M1" s="37"/>
       <c r="N1" s="37"/>
     </row>
-    <row r="2" spans="1:24" ht="15.75" customHeight="1">
+    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="39" t="s">
@@ -1194,7 +1202,7 @@
       <c r="M2" s="37"/>
       <c r="N2" s="37"/>
     </row>
-    <row r="3" spans="1:24" ht="15.75" customHeight="1">
+    <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -1209,10 +1217,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="15.75" customHeight="1">
+    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:24" ht="15.75" customHeight="1">
+    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C5" s="38" t="s">
         <v>6</v>
       </c>
@@ -1241,7 +1249,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="15.75" customHeight="1">
+    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -1310,7 +1318,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="15.75" customHeight="1">
+    <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="16" t="s">
         <v>15</v>
       </c>
@@ -1378,7 +1386,7 @@
       <c r="W7" s="17"/>
       <c r="X7" s="10"/>
     </row>
-    <row r="8" spans="1:24" ht="15.75" customHeight="1">
+    <row r="8" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="16" t="s">
         <v>15</v>
       </c>
@@ -1432,7 +1440,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="15.75" customHeight="1">
+    <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="16" t="s">
         <v>15</v>
       </c>
@@ -1480,7 +1488,7 @@
       <c r="W9" s="17"/>
       <c r="X9" s="10"/>
     </row>
-    <row r="10" spans="1:24" ht="15.75" customHeight="1">
+    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="16" t="s">
         <v>15</v>
       </c>
@@ -1528,7 +1536,7 @@
       <c r="W10" s="17"/>
       <c r="X10" s="10"/>
     </row>
-    <row r="11" spans="1:24" ht="15.75" customHeight="1">
+    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="16" t="s">
         <v>15</v>
       </c>
@@ -1590,7 +1598,7 @@
       <c r="W11" s="17"/>
       <c r="X11" s="10"/>
     </row>
-    <row r="12" spans="1:24" ht="15.75" customHeight="1">
+    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="16" t="s">
         <v>15</v>
       </c>
@@ -1652,7 +1660,7 @@
       <c r="W12" s="17"/>
       <c r="X12" s="10"/>
     </row>
-    <row r="13" spans="1:24" ht="15.75" customHeight="1">
+    <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="16" t="s">
         <v>15</v>
       </c>
@@ -1700,7 +1708,7 @@
       <c r="W13" s="17"/>
       <c r="X13" s="10"/>
     </row>
-    <row r="14" spans="1:24" ht="15.75" customHeight="1">
+    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="16" t="s">
         <v>15</v>
       </c>
@@ -1748,7 +1756,7 @@
       <c r="W14" s="17"/>
       <c r="X14" s="10"/>
     </row>
-    <row r="15" spans="1:24" ht="15.75" customHeight="1">
+    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="16" t="s">
         <v>15</v>
       </c>
@@ -1796,7 +1804,7 @@
       <c r="W15" s="17"/>
       <c r="X15" s="10"/>
     </row>
-    <row r="16" spans="1:24" ht="15.75" customHeight="1">
+    <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="16" t="s">
         <v>15</v>
       </c>
@@ -1858,7 +1866,7 @@
       <c r="W16" s="17"/>
       <c r="X16" s="10"/>
     </row>
-    <row r="17" spans="1:24" ht="15.75" customHeight="1">
+    <row r="17" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="16" t="s">
         <v>15</v>
       </c>
@@ -1920,7 +1928,7 @@
       <c r="W17" s="17"/>
       <c r="X17" s="10"/>
     </row>
-    <row r="18" spans="1:24" ht="15.75" customHeight="1">
+    <row r="18" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="16" t="s">
         <v>15</v>
       </c>
@@ -1968,7 +1976,7 @@
       <c r="W18" s="17"/>
       <c r="X18" s="10"/>
     </row>
-    <row r="19" spans="1:24" ht="15.75" customHeight="1">
+    <row r="19" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="16" t="s">
         <v>15</v>
       </c>
@@ -2030,7 +2038,7 @@
       <c r="W19" s="17"/>
       <c r="X19" s="10"/>
     </row>
-    <row r="20" spans="1:24" ht="15.75" customHeight="1">
+    <row r="20" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="16" t="s">
         <v>15</v>
       </c>
@@ -2096,7 +2104,7 @@
       <c r="W20" s="17"/>
       <c r="X20" s="10"/>
     </row>
-    <row r="21" spans="1:24" ht="15.75" customHeight="1">
+    <row r="21" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="26" t="s">
         <v>15</v>
       </c>
@@ -2164,7 +2172,7 @@
       <c r="W21" s="21"/>
       <c r="X21" s="10"/>
     </row>
-    <row r="22" spans="1:24" ht="15.75" customHeight="1">
+    <row r="22" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="26" t="s">
         <v>15</v>
       </c>
@@ -2230,7 +2238,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="23" spans="1:24" ht="15.75" customHeight="1">
+    <row r="23" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="26" t="s">
         <v>15</v>
       </c>
@@ -2296,7 +2304,7 @@
       <c r="W23" s="21"/>
       <c r="X23" s="10"/>
     </row>
-    <row r="24" spans="1:24" ht="15.75" customHeight="1">
+    <row r="24" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="26" t="s">
         <v>15</v>
       </c>
@@ -2358,7 +2366,7 @@
       <c r="W24" s="21"/>
       <c r="X24" s="10"/>
     </row>
-    <row r="25" spans="1:24" ht="15.75" customHeight="1">
+    <row r="25" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="26" t="s">
         <v>15</v>
       </c>
@@ -2408,7 +2416,7 @@
       <c r="W25" s="21"/>
       <c r="X25" s="10"/>
     </row>
-    <row r="26" spans="1:24" ht="15.75" customHeight="1">
+    <row r="26" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="26" t="s">
         <v>15</v>
       </c>
@@ -2454,7 +2462,7 @@
       <c r="W26" s="21"/>
       <c r="X26" s="10"/>
     </row>
-    <row r="27" spans="1:24" ht="15.75" customHeight="1">
+    <row r="27" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="26" t="s">
         <v>15</v>
       </c>
@@ -2494,7 +2502,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:24" ht="15.75" customHeight="1">
+    <row r="28" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="26" t="s">
         <v>15</v>
       </c>
@@ -2560,7 +2568,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="29" spans="1:24" ht="15.75" customHeight="1">
+    <row r="29" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="26" t="s">
         <v>15</v>
       </c>
@@ -2618,7 +2626,7 @@
       <c r="W29" s="21"/>
       <c r="X29" s="10"/>
     </row>
-    <row r="30" spans="1:24" ht="15.75" customHeight="1">
+    <row r="30" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="26" t="s">
         <v>15</v>
       </c>
@@ -2627,7 +2635,7 @@
       </c>
       <c r="C30" s="21"/>
       <c r="D30" s="17" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="E30" s="17" t="s">
         <v>137</v>
@@ -2676,7 +2684,7 @@
       <c r="W30" s="21"/>
       <c r="X30" s="10"/>
     </row>
-    <row r="31" spans="1:24" ht="15.75" customHeight="1">
+    <row r="31" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="26" t="s">
         <v>15</v>
       </c>
@@ -2734,7 +2742,7 @@
       <c r="W31" s="21"/>
       <c r="X31" s="10"/>
     </row>
-    <row r="32" spans="1:24" ht="15.75" customHeight="1">
+    <row r="32" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="26" t="s">
         <v>15</v>
       </c>
@@ -2743,7 +2751,7 @@
       </c>
       <c r="C32" s="21"/>
       <c r="D32" s="17" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="E32" s="17" t="s">
         <v>137</v>
@@ -2792,7 +2800,7 @@
       <c r="W32" s="21"/>
       <c r="X32" s="10"/>
     </row>
-    <row r="33" spans="1:24" s="13" customFormat="1" ht="15.75" customHeight="1">
+    <row r="33" spans="1:24" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="26" t="s">
         <v>15</v>
       </c>
@@ -2860,7 +2868,7 @@
       <c r="W33" s="21"/>
       <c r="X33" s="12"/>
     </row>
-    <row r="34" spans="1:24" s="32" customFormat="1" ht="15.75" customHeight="1">
+    <row r="34" spans="1:24" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="26" t="s">
         <v>43</v>
       </c>
@@ -2906,7 +2914,7 @@
       <c r="W34" s="21"/>
       <c r="X34" s="31"/>
     </row>
-    <row r="35" spans="1:24" ht="15.75" customHeight="1">
+    <row r="35" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="26" t="s">
         <v>43</v>
       </c>
@@ -2956,7 +2964,7 @@
       <c r="W35" s="21"/>
       <c r="X35" s="10"/>
     </row>
-    <row r="36" spans="1:24" ht="15.75" customHeight="1">
+    <row r="36" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="26" t="s">
         <v>43</v>
       </c>
@@ -3022,7 +3030,7 @@
       <c r="W36" s="21"/>
       <c r="X36" s="10"/>
     </row>
-    <row r="37" spans="1:24" ht="15.75" customHeight="1">
+    <row r="37" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="26" t="s">
         <v>43</v>
       </c>
@@ -3088,7 +3096,7 @@
       <c r="W37" s="21"/>
       <c r="X37" s="10"/>
     </row>
-    <row r="38" spans="1:24" ht="15.75" customHeight="1">
+    <row r="38" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="26" t="s">
         <v>43</v>
       </c>
@@ -3154,7 +3162,7 @@
       <c r="W38" s="21"/>
       <c r="X38" s="10"/>
     </row>
-    <row r="39" spans="1:24" ht="15.75" customHeight="1">
+    <row r="39" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="26" t="s">
         <v>43</v>
       </c>
@@ -3220,7 +3228,7 @@
       <c r="W39" s="21"/>
       <c r="X39" s="10"/>
     </row>
-    <row r="40" spans="1:24" ht="15.75" customHeight="1">
+    <row r="40" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="26" t="s">
         <v>43</v>
       </c>
@@ -3286,7 +3294,7 @@
       <c r="W40" s="21"/>
       <c r="X40" s="10"/>
     </row>
-    <row r="41" spans="1:24" ht="15.75" customHeight="1">
+    <row r="41" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="26" t="s">
         <v>43</v>
       </c>
@@ -3346,7 +3354,7 @@
       <c r="W41" s="21"/>
       <c r="X41" s="10"/>
     </row>
-    <row r="42" spans="1:24" ht="15.75" customHeight="1">
+    <row r="42" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="26" t="s">
         <v>43</v>
       </c>
@@ -3412,7 +3420,7 @@
       <c r="W42" s="21"/>
       <c r="X42" s="10"/>
     </row>
-    <row r="43" spans="1:24" ht="15.75" customHeight="1">
+    <row r="43" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="26" t="s">
         <v>43</v>
       </c>
@@ -3462,7 +3470,7 @@
       <c r="W43" s="21"/>
       <c r="X43" s="10"/>
     </row>
-    <row r="44" spans="1:24" ht="15.75" customHeight="1">
+    <row r="44" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="26" t="s">
         <v>43</v>
       </c>
@@ -3512,7 +3520,7 @@
       <c r="W44" s="21"/>
       <c r="X44" s="10"/>
     </row>
-    <row r="45" spans="1:24" ht="15.75" customHeight="1">
+    <row r="45" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="26" t="s">
         <v>43</v>
       </c>
@@ -3560,7 +3568,7 @@
       <c r="W45" s="21"/>
       <c r="X45" s="10"/>
     </row>
-    <row r="46" spans="1:24" ht="15.75" customHeight="1">
+    <row r="46" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="26" t="s">
         <v>43</v>
       </c>
@@ -3608,7 +3616,7 @@
       <c r="W46" s="21"/>
       <c r="X46" s="10"/>
     </row>
-    <row r="47" spans="1:24" ht="15.75" customHeight="1">
+    <row r="47" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="26" t="s">
         <v>43</v>
       </c>
@@ -3656,7 +3664,7 @@
       <c r="W47" s="21"/>
       <c r="X47" s="10"/>
     </row>
-    <row r="48" spans="1:24" s="29" customFormat="1" ht="15.75" customHeight="1">
+    <row r="48" spans="1:24" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="26" t="s">
         <v>43</v>
       </c>
@@ -3712,7 +3720,7 @@
       <c r="W48" s="21"/>
       <c r="X48" s="28"/>
     </row>
-    <row r="49" spans="1:24" ht="15.75" customHeight="1">
+    <row r="49" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="26" t="s">
         <v>43</v>
       </c>
@@ -3778,7 +3786,7 @@
       <c r="W49" s="21"/>
       <c r="X49" s="10"/>
     </row>
-    <row r="50" spans="1:24" s="35" customFormat="1" ht="15.75" customHeight="1">
+    <row r="50" spans="1:24" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="26" t="s">
         <v>43</v>
       </c>
@@ -3840,7 +3848,7 @@
       <c r="W50" s="21"/>
       <c r="X50" s="34"/>
     </row>
-    <row r="51" spans="1:24" ht="15.75" customHeight="1">
+    <row r="51" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="26" t="s">
         <v>58</v>
       </c>
@@ -3910,7 +3918,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="1:24" ht="15.75" customHeight="1">
+    <row r="52" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="26" t="s">
         <v>58</v>
       </c>
@@ -3978,7 +3986,7 @@
       <c r="W52" s="21"/>
       <c r="X52" s="37"/>
     </row>
-    <row r="53" spans="1:24" ht="15.75" customHeight="1">
+    <row r="53" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="26" t="s">
         <v>62</v>
       </c>
@@ -4044,7 +4052,7 @@
       <c r="W53" s="21"/>
       <c r="X53" s="10"/>
     </row>
-    <row r="54" spans="1:24" s="15" customFormat="1" ht="15.75" customHeight="1">
+    <row r="54" spans="1:24" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="18" t="s">
         <v>63</v>
       </c>
@@ -4078,7 +4086,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="55" spans="1:24" ht="15.75" customHeight="1">
+    <row r="55" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="16" t="s">
         <v>63</v>
       </c>
@@ -4121,7 +4129,7 @@
       <c r="V55" s="17"/>
       <c r="W55" s="17"/>
     </row>
-    <row r="56" spans="1:24" ht="15.75" customHeight="1">
+    <row r="56" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="16" t="s">
         <v>63</v>
       </c>
@@ -4152,7 +4160,7 @@
       <c r="V56" s="17"/>
       <c r="W56" s="17"/>
     </row>
-    <row r="57" spans="1:24" ht="15.75" customHeight="1">
+    <row r="57" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="16" t="s">
         <v>63</v>
       </c>
@@ -4183,7 +4191,7 @@
       <c r="V57" s="17"/>
       <c r="W57" s="17"/>
     </row>
-    <row r="58" spans="1:24" ht="15.75" customHeight="1">
+    <row r="58" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="16" t="s">
         <v>63</v>
       </c>
@@ -4214,7 +4222,7 @@
       <c r="V58" s="17"/>
       <c r="W58" s="17"/>
     </row>
-    <row r="59" spans="1:24" s="33" customFormat="1" ht="15.75" customHeight="1">
+    <row r="59" spans="1:24" s="33" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="16" t="s">
         <v>63</v>
       </c>
@@ -4245,7 +4253,7 @@
       <c r="V59" s="17"/>
       <c r="W59" s="17"/>
     </row>
-    <row r="60" spans="1:24" ht="15.75" customHeight="1">
+    <row r="60" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="16" t="s">
         <v>110</v>
       </c>
@@ -4276,7 +4284,7 @@
       <c r="V60" s="20"/>
       <c r="W60" s="20"/>
     </row>
-    <row r="61" spans="1:24" ht="15.75" customHeight="1">
+    <row r="61" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="16" t="s">
         <v>124</v>
       </c>
@@ -4330,11 +4338,6 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4342,11 +4345,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="29.6640625" customWidth="1"/>
     <col min="2" max="2" width="28.1640625" customWidth="1"/>
@@ -4354,7 +4357,7 @@
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
         <v>70</v>
       </c>
@@ -4371,7 +4374,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15">
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
         <v>73</v>
       </c>
@@ -4384,7 +4387,7 @@
       <c r="D2" s="24"/>
       <c r="E2" s="24"/>
     </row>
-    <row r="3" spans="1:5" ht="15">
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
         <v>75</v>
       </c>
@@ -4397,7 +4400,7 @@
       <c r="D3" s="24"/>
       <c r="E3" s="24"/>
     </row>
-    <row r="4" spans="1:5" ht="15">
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
         <v>77</v>
       </c>
@@ -4410,7 +4413,7 @@
       <c r="D4" s="24"/>
       <c r="E4" s="24"/>
     </row>
-    <row r="5" spans="1:5" ht="15">
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
         <v>97</v>
       </c>
@@ -4425,7 +4428,7 @@
       </c>
       <c r="E5" s="24"/>
     </row>
-    <row r="6" spans="1:5" ht="15">
+    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
         <v>98</v>
       </c>
@@ -4440,7 +4443,7 @@
       </c>
       <c r="E6" s="24"/>
     </row>
-    <row r="7" spans="1:5" ht="15">
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
         <v>99</v>
       </c>
@@ -4455,7 +4458,7 @@
       </c>
       <c r="E7" s="24"/>
     </row>
-    <row r="8" spans="1:5" ht="15">
+    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
         <v>100</v>
       </c>
@@ -4470,7 +4473,7 @@
       </c>
       <c r="E8" s="24"/>
     </row>
-    <row r="9" spans="1:5" ht="15">
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
         <v>109</v>
       </c>
@@ -4483,7 +4486,7 @@
       <c r="D9" s="24"/>
       <c r="E9" s="24"/>
     </row>
-    <row r="10" spans="1:5" ht="15">
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
         <v>108</v>
       </c>
@@ -4496,7 +4499,7 @@
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
     </row>
-    <row r="11" spans="1:5" ht="15">
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
         <v>107</v>
       </c>
@@ -4509,7 +4512,7 @@
       <c r="D11" s="24"/>
       <c r="E11" s="24"/>
     </row>
-    <row r="12" spans="1:5" ht="15">
+    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
         <v>101</v>
       </c>
@@ -4524,7 +4527,7 @@
       </c>
       <c r="E12" s="24"/>
     </row>
-    <row r="13" spans="1:5" ht="15">
+    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
         <v>106</v>
       </c>
@@ -4539,7 +4542,7 @@
       </c>
       <c r="E13" s="24"/>
     </row>
-    <row r="14" spans="1:5" ht="15">
+    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
         <v>102</v>
       </c>
@@ -4554,7 +4557,7 @@
       </c>
       <c r="E14" s="24"/>
     </row>
-    <row r="15" spans="1:5" ht="15">
+    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
         <v>103</v>
       </c>
@@ -4569,7 +4572,7 @@
       </c>
       <c r="E15" s="24"/>
     </row>
-    <row r="16" spans="1:5" ht="15">
+    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
         <v>104</v>
       </c>
@@ -4584,7 +4587,7 @@
       </c>
       <c r="E16" s="24"/>
     </row>
-    <row r="17" spans="1:5" ht="15">
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
         <v>127</v>
       </c>
@@ -4599,7 +4602,7 @@
       </c>
       <c r="E17" s="24"/>
     </row>
-    <row r="18" spans="1:5" ht="15">
+    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
         <v>12</v>
       </c>
@@ -4614,7 +4617,7 @@
       </c>
       <c r="E18" s="24"/>
     </row>
-    <row r="19" spans="1:5" ht="15">
+    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
         <v>13</v>
       </c>
@@ -4629,7 +4632,7 @@
       </c>
       <c r="E19" s="24"/>
     </row>
-    <row r="20" spans="1:5" ht="15">
+    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
         <v>105</v>
       </c>
@@ -4644,7 +4647,7 @@
       </c>
       <c r="E20" s="24"/>
     </row>
-    <row r="21" spans="1:5" ht="15">
+    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
         <v>117</v>
       </c>
@@ -4664,10 +4667,5 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>